<commit_message>
-Check layout modified based on the user request. -BIR 2307 new format added esignature. -Liqudation reversed entry cannot access bug fixed.
</commit_message>
<xml_diff>
--- a/ExpenseProcessingSystem/ExpenseProcessingSystem/wwwroot/ExcelTemplates/_BIR2307_New.xlsx
+++ b/ExpenseProcessingSystem/ExpenseProcessingSystem/wwwroot/ExcelTemplates/_BIR2307_New.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Mizuho EPS\eps_source\ExpenseProcessingSystem\ExpenseProcessingSystem\wwwroot\ExcelTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA529D8B-5880-4F74-8E39-1DE5CAEF484E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F79945F7-3CCD-49D9-A1E6-64626C4950AC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="-1590" windowWidth="24240" windowHeight="13140" tabRatio="876" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -708,7 +708,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="160">
+  <cellXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -864,6 +864,231 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="2" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="2" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="2" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="2" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -924,248 +1149,17 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="2" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="2" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="2" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="2" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="2" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="2" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="2" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4886,136 +4880,136 @@
   <sheetData>
     <row r="1" spans="1:40" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="138" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63"/>
-      <c r="L2" s="63"/>
-      <c r="M2" s="63"/>
-      <c r="N2" s="63"/>
-      <c r="O2" s="63"/>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63"/>
-      <c r="R2" s="63"/>
-      <c r="S2" s="63"/>
-      <c r="T2" s="63"/>
-      <c r="U2" s="63"/>
-      <c r="V2" s="63"/>
-      <c r="W2" s="63"/>
-      <c r="X2" s="63"/>
-      <c r="Y2" s="63"/>
-      <c r="Z2" s="63"/>
-      <c r="AA2" s="63"/>
-      <c r="AB2" s="63"/>
-      <c r="AC2" s="63"/>
-      <c r="AD2" s="63"/>
-      <c r="AE2" s="63"/>
-      <c r="AF2" s="63"/>
-      <c r="AG2" s="63"/>
-      <c r="AH2" s="63"/>
-      <c r="AI2" s="63"/>
-      <c r="AJ2" s="63"/>
-      <c r="AK2" s="63"/>
-      <c r="AL2" s="63"/>
-      <c r="AM2" s="63"/>
-      <c r="AN2" s="63"/>
+      <c r="B2" s="138"/>
+      <c r="C2" s="138"/>
+      <c r="D2" s="138"/>
+      <c r="E2" s="138"/>
+      <c r="F2" s="138"/>
+      <c r="G2" s="138"/>
+      <c r="H2" s="138"/>
+      <c r="I2" s="138"/>
+      <c r="J2" s="138"/>
+      <c r="K2" s="138"/>
+      <c r="L2" s="138"/>
+      <c r="M2" s="138"/>
+      <c r="N2" s="138"/>
+      <c r="O2" s="138"/>
+      <c r="P2" s="138"/>
+      <c r="Q2" s="138"/>
+      <c r="R2" s="138"/>
+      <c r="S2" s="138"/>
+      <c r="T2" s="138"/>
+      <c r="U2" s="138"/>
+      <c r="V2" s="138"/>
+      <c r="W2" s="138"/>
+      <c r="X2" s="138"/>
+      <c r="Y2" s="138"/>
+      <c r="Z2" s="138"/>
+      <c r="AA2" s="138"/>
+      <c r="AB2" s="138"/>
+      <c r="AC2" s="138"/>
+      <c r="AD2" s="138"/>
+      <c r="AE2" s="138"/>
+      <c r="AF2" s="138"/>
+      <c r="AG2" s="138"/>
+      <c r="AH2" s="138"/>
+      <c r="AI2" s="138"/>
+      <c r="AJ2" s="138"/>
+      <c r="AK2" s="138"/>
+      <c r="AL2" s="138"/>
+      <c r="AM2" s="138"/>
+      <c r="AN2" s="138"/>
     </row>
     <row r="3" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="138" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="63"/>
-      <c r="K3" s="63"/>
-      <c r="L3" s="63"/>
-      <c r="M3" s="63"/>
-      <c r="N3" s="63"/>
-      <c r="O3" s="63"/>
-      <c r="P3" s="63"/>
-      <c r="Q3" s="63"/>
-      <c r="R3" s="63"/>
-      <c r="S3" s="63"/>
-      <c r="T3" s="63"/>
-      <c r="U3" s="63"/>
-      <c r="V3" s="63"/>
-      <c r="W3" s="63"/>
-      <c r="X3" s="63"/>
-      <c r="Y3" s="63"/>
-      <c r="Z3" s="63"/>
-      <c r="AA3" s="63"/>
-      <c r="AB3" s="63"/>
-      <c r="AC3" s="63"/>
-      <c r="AD3" s="63"/>
-      <c r="AE3" s="63"/>
-      <c r="AF3" s="63"/>
-      <c r="AG3" s="63"/>
-      <c r="AH3" s="63"/>
-      <c r="AI3" s="63"/>
-      <c r="AJ3" s="63"/>
-      <c r="AK3" s="63"/>
-      <c r="AL3" s="63"/>
-      <c r="AM3" s="63"/>
-      <c r="AN3" s="63"/>
+      <c r="B3" s="138"/>
+      <c r="C3" s="138"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="138"/>
+      <c r="F3" s="138"/>
+      <c r="G3" s="138"/>
+      <c r="H3" s="138"/>
+      <c r="I3" s="138"/>
+      <c r="J3" s="138"/>
+      <c r="K3" s="138"/>
+      <c r="L3" s="138"/>
+      <c r="M3" s="138"/>
+      <c r="N3" s="138"/>
+      <c r="O3" s="138"/>
+      <c r="P3" s="138"/>
+      <c r="Q3" s="138"/>
+      <c r="R3" s="138"/>
+      <c r="S3" s="138"/>
+      <c r="T3" s="138"/>
+      <c r="U3" s="138"/>
+      <c r="V3" s="138"/>
+      <c r="W3" s="138"/>
+      <c r="X3" s="138"/>
+      <c r="Y3" s="138"/>
+      <c r="Z3" s="138"/>
+      <c r="AA3" s="138"/>
+      <c r="AB3" s="138"/>
+      <c r="AC3" s="138"/>
+      <c r="AD3" s="138"/>
+      <c r="AE3" s="138"/>
+      <c r="AF3" s="138"/>
+      <c r="AG3" s="138"/>
+      <c r="AH3" s="138"/>
+      <c r="AI3" s="138"/>
+      <c r="AJ3" s="138"/>
+      <c r="AK3" s="138"/>
+      <c r="AL3" s="138"/>
+      <c r="AM3" s="138"/>
+      <c r="AN3" s="138"/>
     </row>
     <row r="4" spans="1:40" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="64" t="s">
+      <c r="A4" s="139" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="64"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="64"/>
-      <c r="G4" s="64"/>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
-      <c r="J4" s="64"/>
-      <c r="K4" s="64"/>
-      <c r="L4" s="64"/>
-      <c r="M4" s="64"/>
-      <c r="N4" s="64"/>
-      <c r="O4" s="64"/>
-      <c r="P4" s="64"/>
-      <c r="Q4" s="64"/>
-      <c r="R4" s="64"/>
-      <c r="S4" s="64"/>
-      <c r="T4" s="64"/>
-      <c r="U4" s="64"/>
-      <c r="V4" s="64"/>
-      <c r="W4" s="64"/>
-      <c r="X4" s="64"/>
-      <c r="Y4" s="64"/>
-      <c r="Z4" s="64"/>
-      <c r="AA4" s="64"/>
-      <c r="AB4" s="64"/>
-      <c r="AC4" s="64"/>
-      <c r="AD4" s="64"/>
-      <c r="AE4" s="64"/>
-      <c r="AF4" s="64"/>
-      <c r="AG4" s="64"/>
-      <c r="AH4" s="64"/>
-      <c r="AI4" s="64"/>
-      <c r="AJ4" s="64"/>
-      <c r="AK4" s="64"/>
-      <c r="AL4" s="64"/>
-      <c r="AM4" s="64"/>
-      <c r="AN4" s="64"/>
+      <c r="B4" s="139"/>
+      <c r="C4" s="139"/>
+      <c r="D4" s="139"/>
+      <c r="E4" s="139"/>
+      <c r="F4" s="139"/>
+      <c r="G4" s="139"/>
+      <c r="H4" s="139"/>
+      <c r="I4" s="139"/>
+      <c r="J4" s="139"/>
+      <c r="K4" s="139"/>
+      <c r="L4" s="139"/>
+      <c r="M4" s="139"/>
+      <c r="N4" s="139"/>
+      <c r="O4" s="139"/>
+      <c r="P4" s="139"/>
+      <c r="Q4" s="139"/>
+      <c r="R4" s="139"/>
+      <c r="S4" s="139"/>
+      <c r="T4" s="139"/>
+      <c r="U4" s="139"/>
+      <c r="V4" s="139"/>
+      <c r="W4" s="139"/>
+      <c r="X4" s="139"/>
+      <c r="Y4" s="139"/>
+      <c r="Z4" s="139"/>
+      <c r="AA4" s="139"/>
+      <c r="AB4" s="139"/>
+      <c r="AC4" s="139"/>
+      <c r="AD4" s="139"/>
+      <c r="AE4" s="139"/>
+      <c r="AF4" s="139"/>
+      <c r="AG4" s="139"/>
+      <c r="AH4" s="139"/>
+      <c r="AI4" s="139"/>
+      <c r="AJ4" s="139"/>
+      <c r="AK4" s="139"/>
+      <c r="AL4" s="139"/>
+      <c r="AM4" s="139"/>
+      <c r="AN4" s="139"/>
     </row>
     <row r="5" spans="1:40" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
@@ -5029,25 +5023,25 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-      <c r="L5" s="65" t="s">
+      <c r="L5" s="140" t="s">
         <v>7</v>
       </c>
-      <c r="M5" s="65"/>
-      <c r="N5" s="65"/>
-      <c r="O5" s="65"/>
-      <c r="P5" s="65"/>
-      <c r="Q5" s="65"/>
-      <c r="R5" s="65"/>
-      <c r="S5" s="65"/>
-      <c r="T5" s="65"/>
-      <c r="U5" s="65"/>
-      <c r="V5" s="65"/>
-      <c r="W5" s="65"/>
-      <c r="X5" s="65"/>
-      <c r="Y5" s="65"/>
-      <c r="Z5" s="65"/>
-      <c r="AA5" s="65"/>
-      <c r="AB5" s="65"/>
+      <c r="M5" s="140"/>
+      <c r="N5" s="140"/>
+      <c r="O5" s="140"/>
+      <c r="P5" s="140"/>
+      <c r="Q5" s="140"/>
+      <c r="R5" s="140"/>
+      <c r="S5" s="140"/>
+      <c r="T5" s="140"/>
+      <c r="U5" s="140"/>
+      <c r="V5" s="140"/>
+      <c r="W5" s="140"/>
+      <c r="X5" s="140"/>
+      <c r="Y5" s="140"/>
+      <c r="Z5" s="140"/>
+      <c r="AA5" s="140"/>
+      <c r="AB5" s="140"/>
       <c r="AC5" s="1"/>
       <c r="AD5" s="7"/>
       <c r="AE5" s="1"/>
@@ -5073,23 +5067,23 @@
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
-      <c r="L6" s="66"/>
-      <c r="M6" s="66"/>
-      <c r="N6" s="66"/>
-      <c r="O6" s="66"/>
-      <c r="P6" s="66"/>
-      <c r="Q6" s="66"/>
-      <c r="R6" s="66"/>
-      <c r="S6" s="66"/>
-      <c r="T6" s="66"/>
-      <c r="U6" s="66"/>
-      <c r="V6" s="66"/>
-      <c r="W6" s="66"/>
-      <c r="X6" s="66"/>
-      <c r="Y6" s="66"/>
-      <c r="Z6" s="66"/>
-      <c r="AA6" s="66"/>
-      <c r="AB6" s="66"/>
+      <c r="L6" s="141"/>
+      <c r="M6" s="141"/>
+      <c r="N6" s="141"/>
+      <c r="O6" s="141"/>
+      <c r="P6" s="141"/>
+      <c r="Q6" s="141"/>
+      <c r="R6" s="141"/>
+      <c r="S6" s="141"/>
+      <c r="T6" s="141"/>
+      <c r="U6" s="141"/>
+      <c r="V6" s="141"/>
+      <c r="W6" s="141"/>
+      <c r="X6" s="141"/>
+      <c r="Y6" s="141"/>
+      <c r="Z6" s="141"/>
+      <c r="AA6" s="141"/>
+      <c r="AB6" s="141"/>
       <c r="AC6" s="4"/>
       <c r="AD6" s="8"/>
       <c r="AE6" s="4"/>
@@ -5115,23 +5109,23 @@
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
-      <c r="L7" s="66"/>
-      <c r="M7" s="66"/>
-      <c r="N7" s="66"/>
-      <c r="O7" s="66"/>
-      <c r="P7" s="66"/>
-      <c r="Q7" s="66"/>
-      <c r="R7" s="66"/>
-      <c r="S7" s="66"/>
-      <c r="T7" s="66"/>
-      <c r="U7" s="66"/>
-      <c r="V7" s="66"/>
-      <c r="W7" s="66"/>
-      <c r="X7" s="66"/>
-      <c r="Y7" s="66"/>
-      <c r="Z7" s="66"/>
-      <c r="AA7" s="66"/>
-      <c r="AB7" s="66"/>
+      <c r="L7" s="141"/>
+      <c r="M7" s="141"/>
+      <c r="N7" s="141"/>
+      <c r="O7" s="141"/>
+      <c r="P7" s="141"/>
+      <c r="Q7" s="141"/>
+      <c r="R7" s="141"/>
+      <c r="S7" s="141"/>
+      <c r="T7" s="141"/>
+      <c r="U7" s="141"/>
+      <c r="V7" s="141"/>
+      <c r="W7" s="141"/>
+      <c r="X7" s="141"/>
+      <c r="Y7" s="141"/>
+      <c r="Z7" s="141"/>
+      <c r="AA7" s="141"/>
+      <c r="AB7" s="141"/>
       <c r="AC7" s="4"/>
       <c r="AD7" s="8"/>
       <c r="AE7" s="4"/>
@@ -5157,23 +5151,23 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
-      <c r="L8" s="66"/>
-      <c r="M8" s="66"/>
-      <c r="N8" s="66"/>
-      <c r="O8" s="66"/>
-      <c r="P8" s="66"/>
-      <c r="Q8" s="66"/>
-      <c r="R8" s="66"/>
-      <c r="S8" s="66"/>
-      <c r="T8" s="66"/>
-      <c r="U8" s="66"/>
-      <c r="V8" s="66"/>
-      <c r="W8" s="66"/>
-      <c r="X8" s="66"/>
-      <c r="Y8" s="66"/>
-      <c r="Z8" s="66"/>
-      <c r="AA8" s="66"/>
-      <c r="AB8" s="66"/>
+      <c r="L8" s="141"/>
+      <c r="M8" s="141"/>
+      <c r="N8" s="141"/>
+      <c r="O8" s="141"/>
+      <c r="P8" s="141"/>
+      <c r="Q8" s="141"/>
+      <c r="R8" s="141"/>
+      <c r="S8" s="141"/>
+      <c r="T8" s="141"/>
+      <c r="U8" s="141"/>
+      <c r="V8" s="141"/>
+      <c r="W8" s="141"/>
+      <c r="X8" s="141"/>
+      <c r="Y8" s="141"/>
+      <c r="Z8" s="141"/>
+      <c r="AA8" s="141"/>
+      <c r="AB8" s="141"/>
       <c r="AC8" s="4"/>
       <c r="AD8" s="8"/>
       <c r="AE8" s="4"/>
@@ -5199,23 +5193,23 @@
       <c r="I9" s="13"/>
       <c r="J9" s="13"/>
       <c r="K9" s="13"/>
-      <c r="L9" s="67"/>
-      <c r="M9" s="67"/>
-      <c r="N9" s="67"/>
-      <c r="O9" s="67"/>
-      <c r="P9" s="67"/>
-      <c r="Q9" s="67"/>
-      <c r="R9" s="67"/>
-      <c r="S9" s="67"/>
-      <c r="T9" s="67"/>
-      <c r="U9" s="67"/>
-      <c r="V9" s="67"/>
-      <c r="W9" s="67"/>
-      <c r="X9" s="67"/>
-      <c r="Y9" s="67"/>
-      <c r="Z9" s="67"/>
-      <c r="AA9" s="67"/>
-      <c r="AB9" s="67"/>
+      <c r="L9" s="142"/>
+      <c r="M9" s="142"/>
+      <c r="N9" s="142"/>
+      <c r="O9" s="142"/>
+      <c r="P9" s="142"/>
+      <c r="Q9" s="142"/>
+      <c r="R9" s="142"/>
+      <c r="S9" s="142"/>
+      <c r="T9" s="142"/>
+      <c r="U9" s="142"/>
+      <c r="V9" s="142"/>
+      <c r="W9" s="142"/>
+      <c r="X9" s="142"/>
+      <c r="Y9" s="142"/>
+      <c r="Z9" s="142"/>
+      <c r="AA9" s="142"/>
+      <c r="AB9" s="142"/>
       <c r="AC9" s="32"/>
       <c r="AD9" s="19"/>
       <c r="AE9" s="42"/>
@@ -5274,21 +5268,21 @@
       <c r="AN10" s="21"/>
     </row>
     <row r="11" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A11" s="59">
+      <c r="A11" s="134">
         <v>1</v>
       </c>
-      <c r="B11" s="69" t="s">
+      <c r="B11" s="144" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
+      <c r="C11" s="144"/>
+      <c r="D11" s="144"/>
+      <c r="E11" s="144"/>
       <c r="F11" s="33"/>
       <c r="G11" s="33"/>
-      <c r="H11" s="71" t="s">
+      <c r="H11" s="146" t="s">
         <v>37</v>
       </c>
-      <c r="I11" s="71"/>
+      <c r="I11" s="146"/>
       <c r="J11" s="33"/>
       <c r="K11" s="33"/>
       <c r="L11" s="33"/>
@@ -5297,20 +5291,20 @@
       <c r="O11" s="33"/>
       <c r="P11" s="33"/>
       <c r="Q11" s="33"/>
-      <c r="R11" s="73" t="s">
+      <c r="R11" s="148" t="s">
         <v>8</v>
       </c>
-      <c r="S11" s="73"/>
-      <c r="T11" s="73"/>
-      <c r="U11" s="73"/>
+      <c r="S11" s="148"/>
+      <c r="T11" s="148"/>
+      <c r="U11" s="148"/>
       <c r="V11" s="33"/>
       <c r="W11" s="33"/>
       <c r="X11" s="33"/>
-      <c r="Y11" s="69" t="s">
+      <c r="Y11" s="144" t="s">
         <v>9</v>
       </c>
-      <c r="Z11" s="69"/>
-      <c r="AA11" s="69"/>
+      <c r="Z11" s="144"/>
+      <c r="AA11" s="144"/>
       <c r="AB11" s="33"/>
       <c r="AC11" s="33"/>
       <c r="AD11" s="33"/>
@@ -5318,25 +5312,25 @@
       <c r="AF11" s="33"/>
       <c r="AG11" s="33"/>
       <c r="AH11" s="33"/>
-      <c r="AI11" s="75" t="s">
+      <c r="AI11" s="150" t="s">
         <v>8</v>
       </c>
-      <c r="AJ11" s="75"/>
-      <c r="AK11" s="75"/>
-      <c r="AL11" s="75"/>
-      <c r="AM11" s="75"/>
-      <c r="AN11" s="76"/>
+      <c r="AJ11" s="150"/>
+      <c r="AK11" s="150"/>
+      <c r="AL11" s="150"/>
+      <c r="AM11" s="150"/>
+      <c r="AN11" s="151"/>
     </row>
     <row r="12" spans="1:40" s="55" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="68"/>
-      <c r="B12" s="70"/>
-      <c r="C12" s="70"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="70"/>
+      <c r="A12" s="143"/>
+      <c r="B12" s="145"/>
+      <c r="C12" s="145"/>
+      <c r="D12" s="145"/>
+      <c r="E12" s="145"/>
       <c r="F12" s="54"/>
       <c r="G12" s="54"/>
-      <c r="H12" s="72"/>
-      <c r="I12" s="72"/>
+      <c r="H12" s="147"/>
+      <c r="I12" s="147"/>
       <c r="J12" s="54"/>
       <c r="K12" s="54"/>
       <c r="L12" s="54"/>
@@ -5345,16 +5339,16 @@
       <c r="O12" s="54"/>
       <c r="P12" s="54"/>
       <c r="Q12" s="54"/>
-      <c r="R12" s="74"/>
-      <c r="S12" s="74"/>
-      <c r="T12" s="74"/>
-      <c r="U12" s="74"/>
+      <c r="R12" s="149"/>
+      <c r="S12" s="149"/>
+      <c r="T12" s="149"/>
+      <c r="U12" s="149"/>
       <c r="V12" s="54"/>
       <c r="W12" s="54"/>
       <c r="X12" s="54"/>
-      <c r="Y12" s="70"/>
-      <c r="Z12" s="70"/>
-      <c r="AA12" s="70"/>
+      <c r="Y12" s="145"/>
+      <c r="Z12" s="145"/>
+      <c r="AA12" s="145"/>
       <c r="AB12" s="54"/>
       <c r="AC12" s="54"/>
       <c r="AD12" s="54"/>
@@ -5362,12 +5356,12 @@
       <c r="AF12" s="54"/>
       <c r="AG12" s="54"/>
       <c r="AH12" s="54"/>
-      <c r="AI12" s="77"/>
-      <c r="AJ12" s="77"/>
-      <c r="AK12" s="77"/>
-      <c r="AL12" s="77"/>
-      <c r="AM12" s="77"/>
-      <c r="AN12" s="78"/>
+      <c r="AI12" s="152"/>
+      <c r="AJ12" s="152"/>
+      <c r="AK12" s="152"/>
+      <c r="AL12" s="152"/>
+      <c r="AM12" s="152"/>
+      <c r="AN12" s="153"/>
     </row>
     <row r="13" spans="1:40" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="56" t="s">
@@ -5414,23 +5408,23 @@
       <c r="AN13" s="58"/>
     </row>
     <row r="14" spans="1:40" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="59">
+      <c r="A14" s="134">
         <v>2</v>
       </c>
-      <c r="B14" s="61" t="s">
+      <c r="B14" s="136" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="61"/>
-      <c r="D14" s="61"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="61"/>
-      <c r="G14" s="61"/>
-      <c r="H14" s="61"/>
-      <c r="I14" s="61"/>
-      <c r="J14" s="61"/>
-      <c r="K14" s="61"/>
-      <c r="L14" s="61"/>
-      <c r="M14" s="61"/>
+      <c r="C14" s="136"/>
+      <c r="D14" s="136"/>
+      <c r="E14" s="136"/>
+      <c r="F14" s="136"/>
+      <c r="G14" s="136"/>
+      <c r="H14" s="136"/>
+      <c r="I14" s="136"/>
+      <c r="J14" s="136"/>
+      <c r="K14" s="136"/>
+      <c r="L14" s="136"/>
+      <c r="M14" s="136"/>
       <c r="N14" s="33"/>
       <c r="O14" s="33"/>
       <c r="P14" s="33"/>
@@ -5460,19 +5454,19 @@
       <c r="AN14" s="34"/>
     </row>
     <row r="15" spans="1:40" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="60"/>
-      <c r="B15" s="62"/>
-      <c r="C15" s="62"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="62"/>
-      <c r="G15" s="62"/>
-      <c r="H15" s="62"/>
-      <c r="I15" s="62"/>
-      <c r="J15" s="62"/>
-      <c r="K15" s="62"/>
-      <c r="L15" s="62"/>
-      <c r="M15" s="62"/>
+      <c r="A15" s="135"/>
+      <c r="B15" s="137"/>
+      <c r="C15" s="137"/>
+      <c r="D15" s="137"/>
+      <c r="E15" s="137"/>
+      <c r="F15" s="137"/>
+      <c r="G15" s="137"/>
+      <c r="H15" s="137"/>
+      <c r="I15" s="137"/>
+      <c r="J15" s="137"/>
+      <c r="K15" s="137"/>
+      <c r="L15" s="137"/>
+      <c r="M15" s="137"/>
       <c r="N15" s="16"/>
       <c r="O15" s="16"/>
       <c r="P15" s="16"/>
@@ -5940,23 +5934,23 @@
       <c r="AN25" s="58"/>
     </row>
     <row r="26" spans="1:40" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="59">
+      <c r="A26" s="134">
         <v>6</v>
       </c>
-      <c r="B26" s="61" t="s">
+      <c r="B26" s="136" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="61"/>
-      <c r="D26" s="61"/>
-      <c r="E26" s="61"/>
-      <c r="F26" s="61"/>
-      <c r="G26" s="61"/>
-      <c r="H26" s="61"/>
-      <c r="I26" s="61"/>
-      <c r="J26" s="61"/>
-      <c r="K26" s="61"/>
-      <c r="L26" s="61"/>
-      <c r="M26" s="61"/>
+      <c r="C26" s="136"/>
+      <c r="D26" s="136"/>
+      <c r="E26" s="136"/>
+      <c r="F26" s="136"/>
+      <c r="G26" s="136"/>
+      <c r="H26" s="136"/>
+      <c r="I26" s="136"/>
+      <c r="J26" s="136"/>
+      <c r="K26" s="136"/>
+      <c r="L26" s="136"/>
+      <c r="M26" s="136"/>
       <c r="N26" s="33"/>
       <c r="O26" s="33"/>
       <c r="P26" s="33"/>
@@ -5986,19 +5980,19 @@
       <c r="AN26" s="34"/>
     </row>
     <row r="27" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="60"/>
-      <c r="B27" s="62"/>
-      <c r="C27" s="62"/>
-      <c r="D27" s="62"/>
-      <c r="E27" s="62"/>
-      <c r="F27" s="62"/>
-      <c r="G27" s="62"/>
-      <c r="H27" s="62"/>
-      <c r="I27" s="62"/>
-      <c r="J27" s="62"/>
-      <c r="K27" s="62"/>
-      <c r="L27" s="62"/>
-      <c r="M27" s="62"/>
+      <c r="A27" s="135"/>
+      <c r="B27" s="137"/>
+      <c r="C27" s="137"/>
+      <c r="D27" s="137"/>
+      <c r="E27" s="137"/>
+      <c r="F27" s="137"/>
+      <c r="G27" s="137"/>
+      <c r="H27" s="137"/>
+      <c r="I27" s="137"/>
+      <c r="J27" s="137"/>
+      <c r="K27" s="137"/>
+      <c r="L27" s="137"/>
+      <c r="M27" s="137"/>
       <c r="N27" s="16"/>
       <c r="O27" s="16"/>
       <c r="P27" s="16"/>
@@ -6292,190 +6286,190 @@
       <c r="AN33" s="29"/>
     </row>
     <row r="34" spans="1:40" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="79" t="s">
+      <c r="A34" s="115" t="s">
         <v>20</v>
       </c>
-      <c r="B34" s="80"/>
-      <c r="C34" s="80"/>
-      <c r="D34" s="80"/>
-      <c r="E34" s="80"/>
-      <c r="F34" s="80"/>
-      <c r="G34" s="80"/>
-      <c r="H34" s="80"/>
-      <c r="I34" s="80"/>
-      <c r="J34" s="80"/>
-      <c r="K34" s="80"/>
-      <c r="L34" s="80"/>
-      <c r="M34" s="80"/>
-      <c r="N34" s="80"/>
-      <c r="O34" s="80"/>
-      <c r="P34" s="80"/>
-      <c r="Q34" s="80"/>
-      <c r="R34" s="80"/>
-      <c r="S34" s="80"/>
-      <c r="T34" s="80"/>
-      <c r="U34" s="80"/>
-      <c r="V34" s="80"/>
-      <c r="W34" s="80"/>
-      <c r="X34" s="80"/>
-      <c r="Y34" s="80"/>
-      <c r="Z34" s="80"/>
-      <c r="AA34" s="80"/>
-      <c r="AB34" s="80"/>
-      <c r="AC34" s="80"/>
-      <c r="AD34" s="80"/>
-      <c r="AE34" s="80"/>
-      <c r="AF34" s="80"/>
-      <c r="AG34" s="80"/>
-      <c r="AH34" s="80"/>
-      <c r="AI34" s="80"/>
-      <c r="AJ34" s="80"/>
-      <c r="AK34" s="80"/>
-      <c r="AL34" s="80"/>
-      <c r="AM34" s="80"/>
-      <c r="AN34" s="81"/>
+      <c r="B34" s="116"/>
+      <c r="C34" s="116"/>
+      <c r="D34" s="116"/>
+      <c r="E34" s="116"/>
+      <c r="F34" s="116"/>
+      <c r="G34" s="116"/>
+      <c r="H34" s="116"/>
+      <c r="I34" s="116"/>
+      <c r="J34" s="116"/>
+      <c r="K34" s="116"/>
+      <c r="L34" s="116"/>
+      <c r="M34" s="116"/>
+      <c r="N34" s="116"/>
+      <c r="O34" s="116"/>
+      <c r="P34" s="116"/>
+      <c r="Q34" s="116"/>
+      <c r="R34" s="116"/>
+      <c r="S34" s="116"/>
+      <c r="T34" s="116"/>
+      <c r="U34" s="116"/>
+      <c r="V34" s="116"/>
+      <c r="W34" s="116"/>
+      <c r="X34" s="116"/>
+      <c r="Y34" s="116"/>
+      <c r="Z34" s="116"/>
+      <c r="AA34" s="116"/>
+      <c r="AB34" s="116"/>
+      <c r="AC34" s="116"/>
+      <c r="AD34" s="116"/>
+      <c r="AE34" s="116"/>
+      <c r="AF34" s="116"/>
+      <c r="AG34" s="116"/>
+      <c r="AH34" s="116"/>
+      <c r="AI34" s="116"/>
+      <c r="AJ34" s="116"/>
+      <c r="AK34" s="116"/>
+      <c r="AL34" s="116"/>
+      <c r="AM34" s="116"/>
+      <c r="AN34" s="117"/>
     </row>
     <row r="35" spans="1:40" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="82" t="s">
+      <c r="A35" s="118" t="s">
         <v>22</v>
       </c>
-      <c r="B35" s="83"/>
-      <c r="C35" s="83"/>
-      <c r="D35" s="83"/>
-      <c r="E35" s="83"/>
-      <c r="F35" s="83"/>
-      <c r="G35" s="83"/>
-      <c r="H35" s="83"/>
-      <c r="I35" s="83"/>
-      <c r="J35" s="83"/>
-      <c r="K35" s="84"/>
-      <c r="L35" s="91" t="s">
+      <c r="B35" s="119"/>
+      <c r="C35" s="119"/>
+      <c r="D35" s="119"/>
+      <c r="E35" s="119"/>
+      <c r="F35" s="119"/>
+      <c r="G35" s="119"/>
+      <c r="H35" s="119"/>
+      <c r="I35" s="119"/>
+      <c r="J35" s="119"/>
+      <c r="K35" s="120"/>
+      <c r="L35" s="124" t="s">
         <v>23</v>
       </c>
-      <c r="M35" s="83"/>
-      <c r="N35" s="84"/>
-      <c r="O35" s="94" t="s">
+      <c r="M35" s="119"/>
+      <c r="N35" s="120"/>
+      <c r="O35" s="127" t="s">
         <v>24</v>
       </c>
-      <c r="P35" s="95"/>
-      <c r="Q35" s="95"/>
-      <c r="R35" s="95"/>
-      <c r="S35" s="95"/>
-      <c r="T35" s="95"/>
-      <c r="U35" s="95"/>
-      <c r="V35" s="95"/>
-      <c r="W35" s="95"/>
-      <c r="X35" s="95"/>
-      <c r="Y35" s="95"/>
-      <c r="Z35" s="95"/>
-      <c r="AA35" s="95"/>
-      <c r="AB35" s="95"/>
-      <c r="AC35" s="95"/>
-      <c r="AD35" s="95"/>
-      <c r="AE35" s="95"/>
-      <c r="AF35" s="95"/>
-      <c r="AG35" s="95"/>
-      <c r="AH35" s="96"/>
-      <c r="AI35" s="91" t="s">
+      <c r="P35" s="128"/>
+      <c r="Q35" s="128"/>
+      <c r="R35" s="128"/>
+      <c r="S35" s="128"/>
+      <c r="T35" s="128"/>
+      <c r="U35" s="128"/>
+      <c r="V35" s="128"/>
+      <c r="W35" s="128"/>
+      <c r="X35" s="128"/>
+      <c r="Y35" s="128"/>
+      <c r="Z35" s="128"/>
+      <c r="AA35" s="128"/>
+      <c r="AB35" s="128"/>
+      <c r="AC35" s="128"/>
+      <c r="AD35" s="128"/>
+      <c r="AE35" s="128"/>
+      <c r="AF35" s="128"/>
+      <c r="AG35" s="128"/>
+      <c r="AH35" s="129"/>
+      <c r="AI35" s="124" t="s">
         <v>21</v>
       </c>
-      <c r="AJ35" s="83"/>
-      <c r="AK35" s="83"/>
-      <c r="AL35" s="83"/>
-      <c r="AM35" s="83"/>
-      <c r="AN35" s="97"/>
+      <c r="AJ35" s="119"/>
+      <c r="AK35" s="119"/>
+      <c r="AL35" s="119"/>
+      <c r="AM35" s="119"/>
+      <c r="AN35" s="130"/>
     </row>
     <row r="36" spans="1:40" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="85"/>
-      <c r="B36" s="86"/>
-      <c r="C36" s="86"/>
-      <c r="D36" s="86"/>
-      <c r="E36" s="86"/>
-      <c r="F36" s="86"/>
-      <c r="G36" s="86"/>
-      <c r="H36" s="86"/>
-      <c r="I36" s="86"/>
-      <c r="J36" s="86"/>
-      <c r="K36" s="87"/>
-      <c r="L36" s="92"/>
-      <c r="M36" s="86"/>
-      <c r="N36" s="87"/>
-      <c r="O36" s="100" t="s">
+      <c r="A36" s="121"/>
+      <c r="B36" s="122"/>
+      <c r="C36" s="122"/>
+      <c r="D36" s="122"/>
+      <c r="E36" s="122"/>
+      <c r="F36" s="122"/>
+      <c r="G36" s="122"/>
+      <c r="H36" s="122"/>
+      <c r="I36" s="122"/>
+      <c r="J36" s="122"/>
+      <c r="K36" s="123"/>
+      <c r="L36" s="125"/>
+      <c r="M36" s="122"/>
+      <c r="N36" s="123"/>
+      <c r="O36" s="133" t="s">
         <v>28</v>
       </c>
-      <c r="P36" s="101"/>
-      <c r="Q36" s="101"/>
-      <c r="R36" s="101"/>
-      <c r="S36" s="102"/>
-      <c r="T36" s="100" t="s">
+      <c r="P36" s="108"/>
+      <c r="Q36" s="108"/>
+      <c r="R36" s="108"/>
+      <c r="S36" s="109"/>
+      <c r="T36" s="133" t="s">
         <v>27</v>
       </c>
-      <c r="U36" s="101"/>
-      <c r="V36" s="101"/>
-      <c r="W36" s="101"/>
-      <c r="X36" s="102"/>
-      <c r="Y36" s="100" t="s">
+      <c r="U36" s="108"/>
+      <c r="V36" s="108"/>
+      <c r="W36" s="108"/>
+      <c r="X36" s="109"/>
+      <c r="Y36" s="133" t="s">
         <v>26</v>
       </c>
-      <c r="Z36" s="101"/>
-      <c r="AA36" s="101"/>
-      <c r="AB36" s="101"/>
-      <c r="AC36" s="102"/>
-      <c r="AD36" s="100" t="s">
+      <c r="Z36" s="108"/>
+      <c r="AA36" s="108"/>
+      <c r="AB36" s="108"/>
+      <c r="AC36" s="109"/>
+      <c r="AD36" s="133" t="s">
         <v>25</v>
       </c>
-      <c r="AE36" s="101"/>
-      <c r="AF36" s="101"/>
-      <c r="AG36" s="101"/>
-      <c r="AH36" s="102"/>
-      <c r="AI36" s="92"/>
-      <c r="AJ36" s="86"/>
-      <c r="AK36" s="86"/>
-      <c r="AL36" s="86"/>
-      <c r="AM36" s="86"/>
-      <c r="AN36" s="98"/>
+      <c r="AE36" s="108"/>
+      <c r="AF36" s="108"/>
+      <c r="AG36" s="108"/>
+      <c r="AH36" s="109"/>
+      <c r="AI36" s="125"/>
+      <c r="AJ36" s="122"/>
+      <c r="AK36" s="122"/>
+      <c r="AL36" s="122"/>
+      <c r="AM36" s="122"/>
+      <c r="AN36" s="131"/>
     </row>
     <row r="37" spans="1:40" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="88"/>
-      <c r="B37" s="89"/>
-      <c r="C37" s="89"/>
-      <c r="D37" s="89"/>
-      <c r="E37" s="89"/>
-      <c r="F37" s="89"/>
-      <c r="G37" s="89"/>
-      <c r="H37" s="89"/>
-      <c r="I37" s="89"/>
-      <c r="J37" s="89"/>
-      <c r="K37" s="90"/>
-      <c r="L37" s="93"/>
-      <c r="M37" s="89"/>
-      <c r="N37" s="90"/>
-      <c r="O37" s="93"/>
-      <c r="P37" s="89"/>
-      <c r="Q37" s="89"/>
-      <c r="R37" s="89"/>
-      <c r="S37" s="90"/>
-      <c r="T37" s="93"/>
-      <c r="U37" s="89"/>
-      <c r="V37" s="89"/>
-      <c r="W37" s="89"/>
-      <c r="X37" s="90"/>
-      <c r="Y37" s="93"/>
-      <c r="Z37" s="89"/>
-      <c r="AA37" s="89"/>
-      <c r="AB37" s="89"/>
-      <c r="AC37" s="90"/>
-      <c r="AD37" s="93"/>
-      <c r="AE37" s="89"/>
-      <c r="AF37" s="89"/>
-      <c r="AG37" s="89"/>
-      <c r="AH37" s="90"/>
-      <c r="AI37" s="93"/>
-      <c r="AJ37" s="89"/>
-      <c r="AK37" s="89"/>
-      <c r="AL37" s="89"/>
-      <c r="AM37" s="89"/>
-      <c r="AN37" s="99"/>
+      <c r="A37" s="110"/>
+      <c r="B37" s="111"/>
+      <c r="C37" s="111"/>
+      <c r="D37" s="111"/>
+      <c r="E37" s="111"/>
+      <c r="F37" s="111"/>
+      <c r="G37" s="111"/>
+      <c r="H37" s="111"/>
+      <c r="I37" s="111"/>
+      <c r="J37" s="111"/>
+      <c r="K37" s="112"/>
+      <c r="L37" s="126"/>
+      <c r="M37" s="111"/>
+      <c r="N37" s="112"/>
+      <c r="O37" s="126"/>
+      <c r="P37" s="111"/>
+      <c r="Q37" s="111"/>
+      <c r="R37" s="111"/>
+      <c r="S37" s="112"/>
+      <c r="T37" s="126"/>
+      <c r="U37" s="111"/>
+      <c r="V37" s="111"/>
+      <c r="W37" s="111"/>
+      <c r="X37" s="112"/>
+      <c r="Y37" s="126"/>
+      <c r="Z37" s="111"/>
+      <c r="AA37" s="111"/>
+      <c r="AB37" s="111"/>
+      <c r="AC37" s="112"/>
+      <c r="AD37" s="126"/>
+      <c r="AE37" s="111"/>
+      <c r="AF37" s="111"/>
+      <c r="AG37" s="111"/>
+      <c r="AH37" s="112"/>
+      <c r="AI37" s="126"/>
+      <c r="AJ37" s="111"/>
+      <c r="AK37" s="111"/>
+      <c r="AL37" s="111"/>
+      <c r="AM37" s="111"/>
+      <c r="AN37" s="132"/>
     </row>
     <row r="38" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="154"/>
@@ -6489,38 +6483,38 @@
       <c r="I38" s="155"/>
       <c r="J38" s="155"/>
       <c r="K38" s="156"/>
-      <c r="L38" s="106"/>
-      <c r="M38" s="107"/>
-      <c r="N38" s="108"/>
-      <c r="O38" s="109"/>
-      <c r="P38" s="110"/>
-      <c r="Q38" s="110"/>
-      <c r="R38" s="110"/>
-      <c r="S38" s="111"/>
-      <c r="T38" s="109"/>
-      <c r="U38" s="110"/>
-      <c r="V38" s="110"/>
-      <c r="W38" s="110"/>
-      <c r="X38" s="111"/>
-      <c r="Y38" s="109"/>
-      <c r="Z38" s="110"/>
-      <c r="AA38" s="110"/>
-      <c r="AB38" s="110"/>
-      <c r="AC38" s="111"/>
-      <c r="AD38" s="103">
+      <c r="L38" s="95"/>
+      <c r="M38" s="96"/>
+      <c r="N38" s="97"/>
+      <c r="O38" s="98"/>
+      <c r="P38" s="99"/>
+      <c r="Q38" s="99"/>
+      <c r="R38" s="99"/>
+      <c r="S38" s="100"/>
+      <c r="T38" s="98"/>
+      <c r="U38" s="99"/>
+      <c r="V38" s="99"/>
+      <c r="W38" s="99"/>
+      <c r="X38" s="100"/>
+      <c r="Y38" s="98"/>
+      <c r="Z38" s="99"/>
+      <c r="AA38" s="99"/>
+      <c r="AB38" s="99"/>
+      <c r="AC38" s="100"/>
+      <c r="AD38" s="82">
         <f>SUM(O38:AC38)</f>
         <v>0</v>
       </c>
-      <c r="AE38" s="104"/>
-      <c r="AF38" s="104"/>
-      <c r="AG38" s="104"/>
-      <c r="AH38" s="112"/>
-      <c r="AI38" s="103"/>
-      <c r="AJ38" s="104"/>
-      <c r="AK38" s="104"/>
-      <c r="AL38" s="104"/>
-      <c r="AM38" s="104"/>
-      <c r="AN38" s="105"/>
+      <c r="AE38" s="83"/>
+      <c r="AF38" s="83"/>
+      <c r="AG38" s="83"/>
+      <c r="AH38" s="103"/>
+      <c r="AI38" s="82"/>
+      <c r="AJ38" s="83"/>
+      <c r="AK38" s="83"/>
+      <c r="AL38" s="83"/>
+      <c r="AM38" s="83"/>
+      <c r="AN38" s="84"/>
     </row>
     <row r="39" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="154"/>
@@ -6534,38 +6528,38 @@
       <c r="I39" s="155"/>
       <c r="J39" s="155"/>
       <c r="K39" s="156"/>
-      <c r="L39" s="106"/>
-      <c r="M39" s="107"/>
-      <c r="N39" s="108"/>
-      <c r="O39" s="109"/>
-      <c r="P39" s="110"/>
-      <c r="Q39" s="110"/>
-      <c r="R39" s="110"/>
-      <c r="S39" s="111"/>
-      <c r="T39" s="109"/>
-      <c r="U39" s="110"/>
-      <c r="V39" s="110"/>
-      <c r="W39" s="110"/>
-      <c r="X39" s="111"/>
-      <c r="Y39" s="109"/>
-      <c r="Z39" s="110"/>
-      <c r="AA39" s="110"/>
-      <c r="AB39" s="110"/>
-      <c r="AC39" s="111"/>
-      <c r="AD39" s="103">
+      <c r="L39" s="95"/>
+      <c r="M39" s="96"/>
+      <c r="N39" s="97"/>
+      <c r="O39" s="98"/>
+      <c r="P39" s="99"/>
+      <c r="Q39" s="99"/>
+      <c r="R39" s="99"/>
+      <c r="S39" s="100"/>
+      <c r="T39" s="98"/>
+      <c r="U39" s="99"/>
+      <c r="V39" s="99"/>
+      <c r="W39" s="99"/>
+      <c r="X39" s="100"/>
+      <c r="Y39" s="98"/>
+      <c r="Z39" s="99"/>
+      <c r="AA39" s="99"/>
+      <c r="AB39" s="99"/>
+      <c r="AC39" s="100"/>
+      <c r="AD39" s="82">
         <f t="shared" ref="AD39:AD47" si="0">SUM(O39:AC39)</f>
         <v>0</v>
       </c>
-      <c r="AE39" s="104"/>
-      <c r="AF39" s="104"/>
-      <c r="AG39" s="104"/>
-      <c r="AH39" s="112"/>
-      <c r="AI39" s="106"/>
-      <c r="AJ39" s="107"/>
-      <c r="AK39" s="107"/>
-      <c r="AL39" s="107"/>
-      <c r="AM39" s="107"/>
-      <c r="AN39" s="113"/>
+      <c r="AE39" s="83"/>
+      <c r="AF39" s="83"/>
+      <c r="AG39" s="83"/>
+      <c r="AH39" s="103"/>
+      <c r="AI39" s="95"/>
+      <c r="AJ39" s="96"/>
+      <c r="AK39" s="96"/>
+      <c r="AL39" s="96"/>
+      <c r="AM39" s="96"/>
+      <c r="AN39" s="114"/>
     </row>
     <row r="40" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="154"/>
@@ -6579,38 +6573,38 @@
       <c r="I40" s="155"/>
       <c r="J40" s="155"/>
       <c r="K40" s="156"/>
-      <c r="L40" s="106"/>
-      <c r="M40" s="107"/>
-      <c r="N40" s="108"/>
-      <c r="O40" s="109"/>
-      <c r="P40" s="110"/>
-      <c r="Q40" s="110"/>
-      <c r="R40" s="110"/>
-      <c r="S40" s="111"/>
-      <c r="T40" s="109"/>
-      <c r="U40" s="110"/>
-      <c r="V40" s="110"/>
-      <c r="W40" s="110"/>
-      <c r="X40" s="111"/>
-      <c r="Y40" s="109"/>
-      <c r="Z40" s="110"/>
-      <c r="AA40" s="110"/>
-      <c r="AB40" s="110"/>
-      <c r="AC40" s="111"/>
-      <c r="AD40" s="103">
+      <c r="L40" s="95"/>
+      <c r="M40" s="96"/>
+      <c r="N40" s="97"/>
+      <c r="O40" s="98"/>
+      <c r="P40" s="99"/>
+      <c r="Q40" s="99"/>
+      <c r="R40" s="99"/>
+      <c r="S40" s="100"/>
+      <c r="T40" s="98"/>
+      <c r="U40" s="99"/>
+      <c r="V40" s="99"/>
+      <c r="W40" s="99"/>
+      <c r="X40" s="100"/>
+      <c r="Y40" s="98"/>
+      <c r="Z40" s="99"/>
+      <c r="AA40" s="99"/>
+      <c r="AB40" s="99"/>
+      <c r="AC40" s="100"/>
+      <c r="AD40" s="82">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AE40" s="104"/>
-      <c r="AF40" s="104"/>
-      <c r="AG40" s="104"/>
-      <c r="AH40" s="112"/>
-      <c r="AI40" s="106"/>
-      <c r="AJ40" s="107"/>
-      <c r="AK40" s="107"/>
-      <c r="AL40" s="107"/>
-      <c r="AM40" s="107"/>
-      <c r="AN40" s="113"/>
+      <c r="AE40" s="83"/>
+      <c r="AF40" s="83"/>
+      <c r="AG40" s="83"/>
+      <c r="AH40" s="103"/>
+      <c r="AI40" s="95"/>
+      <c r="AJ40" s="96"/>
+      <c r="AK40" s="96"/>
+      <c r="AL40" s="96"/>
+      <c r="AM40" s="96"/>
+      <c r="AN40" s="114"/>
     </row>
     <row r="41" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="154"/>
@@ -6624,38 +6618,38 @@
       <c r="I41" s="155"/>
       <c r="J41" s="155"/>
       <c r="K41" s="156"/>
-      <c r="L41" s="106"/>
-      <c r="M41" s="107"/>
-      <c r="N41" s="108"/>
-      <c r="O41" s="109"/>
-      <c r="P41" s="110"/>
-      <c r="Q41" s="110"/>
-      <c r="R41" s="110"/>
-      <c r="S41" s="111"/>
-      <c r="T41" s="109"/>
-      <c r="U41" s="110"/>
-      <c r="V41" s="110"/>
-      <c r="W41" s="110"/>
-      <c r="X41" s="111"/>
-      <c r="Y41" s="109"/>
-      <c r="Z41" s="110"/>
-      <c r="AA41" s="110"/>
-      <c r="AB41" s="110"/>
-      <c r="AC41" s="111"/>
-      <c r="AD41" s="103">
+      <c r="L41" s="95"/>
+      <c r="M41" s="96"/>
+      <c r="N41" s="97"/>
+      <c r="O41" s="98"/>
+      <c r="P41" s="99"/>
+      <c r="Q41" s="99"/>
+      <c r="R41" s="99"/>
+      <c r="S41" s="100"/>
+      <c r="T41" s="98"/>
+      <c r="U41" s="99"/>
+      <c r="V41" s="99"/>
+      <c r="W41" s="99"/>
+      <c r="X41" s="100"/>
+      <c r="Y41" s="98"/>
+      <c r="Z41" s="99"/>
+      <c r="AA41" s="99"/>
+      <c r="AB41" s="99"/>
+      <c r="AC41" s="100"/>
+      <c r="AD41" s="82">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AE41" s="104"/>
-      <c r="AF41" s="104"/>
-      <c r="AG41" s="104"/>
-      <c r="AH41" s="112"/>
-      <c r="AI41" s="106"/>
-      <c r="AJ41" s="107"/>
-      <c r="AK41" s="107"/>
-      <c r="AL41" s="107"/>
-      <c r="AM41" s="107"/>
-      <c r="AN41" s="113"/>
+      <c r="AE41" s="83"/>
+      <c r="AF41" s="83"/>
+      <c r="AG41" s="83"/>
+      <c r="AH41" s="103"/>
+      <c r="AI41" s="95"/>
+      <c r="AJ41" s="96"/>
+      <c r="AK41" s="96"/>
+      <c r="AL41" s="96"/>
+      <c r="AM41" s="96"/>
+      <c r="AN41" s="114"/>
     </row>
     <row r="42" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="154"/>
@@ -6669,38 +6663,38 @@
       <c r="I42" s="155"/>
       <c r="J42" s="155"/>
       <c r="K42" s="156"/>
-      <c r="L42" s="106"/>
-      <c r="M42" s="107"/>
-      <c r="N42" s="108"/>
-      <c r="O42" s="109"/>
-      <c r="P42" s="110"/>
-      <c r="Q42" s="110"/>
-      <c r="R42" s="110"/>
-      <c r="S42" s="111"/>
-      <c r="T42" s="109"/>
-      <c r="U42" s="110"/>
-      <c r="V42" s="110"/>
-      <c r="W42" s="110"/>
-      <c r="X42" s="111"/>
-      <c r="Y42" s="109"/>
-      <c r="Z42" s="110"/>
-      <c r="AA42" s="110"/>
-      <c r="AB42" s="110"/>
-      <c r="AC42" s="111"/>
-      <c r="AD42" s="103">
+      <c r="L42" s="95"/>
+      <c r="M42" s="96"/>
+      <c r="N42" s="97"/>
+      <c r="O42" s="98"/>
+      <c r="P42" s="99"/>
+      <c r="Q42" s="99"/>
+      <c r="R42" s="99"/>
+      <c r="S42" s="100"/>
+      <c r="T42" s="98"/>
+      <c r="U42" s="99"/>
+      <c r="V42" s="99"/>
+      <c r="W42" s="99"/>
+      <c r="X42" s="100"/>
+      <c r="Y42" s="98"/>
+      <c r="Z42" s="99"/>
+      <c r="AA42" s="99"/>
+      <c r="AB42" s="99"/>
+      <c r="AC42" s="100"/>
+      <c r="AD42" s="82">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AE42" s="104"/>
-      <c r="AF42" s="104"/>
-      <c r="AG42" s="104"/>
-      <c r="AH42" s="112"/>
-      <c r="AI42" s="106"/>
-      <c r="AJ42" s="107"/>
-      <c r="AK42" s="107"/>
-      <c r="AL42" s="107"/>
-      <c r="AM42" s="107"/>
-      <c r="AN42" s="113"/>
+      <c r="AE42" s="83"/>
+      <c r="AF42" s="83"/>
+      <c r="AG42" s="83"/>
+      <c r="AH42" s="103"/>
+      <c r="AI42" s="95"/>
+      <c r="AJ42" s="96"/>
+      <c r="AK42" s="96"/>
+      <c r="AL42" s="96"/>
+      <c r="AM42" s="96"/>
+      <c r="AN42" s="114"/>
     </row>
     <row r="43" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="154"/>
@@ -6714,38 +6708,38 @@
       <c r="I43" s="155"/>
       <c r="J43" s="155"/>
       <c r="K43" s="156"/>
-      <c r="L43" s="106"/>
-      <c r="M43" s="107"/>
-      <c r="N43" s="108"/>
-      <c r="O43" s="109"/>
-      <c r="P43" s="110"/>
-      <c r="Q43" s="110"/>
-      <c r="R43" s="110"/>
-      <c r="S43" s="111"/>
-      <c r="T43" s="109"/>
-      <c r="U43" s="110"/>
-      <c r="V43" s="110"/>
-      <c r="W43" s="110"/>
-      <c r="X43" s="111"/>
-      <c r="Y43" s="109"/>
-      <c r="Z43" s="110"/>
-      <c r="AA43" s="110"/>
-      <c r="AB43" s="110"/>
-      <c r="AC43" s="111"/>
-      <c r="AD43" s="103">
+      <c r="L43" s="95"/>
+      <c r="M43" s="96"/>
+      <c r="N43" s="97"/>
+      <c r="O43" s="98"/>
+      <c r="P43" s="99"/>
+      <c r="Q43" s="99"/>
+      <c r="R43" s="99"/>
+      <c r="S43" s="100"/>
+      <c r="T43" s="98"/>
+      <c r="U43" s="99"/>
+      <c r="V43" s="99"/>
+      <c r="W43" s="99"/>
+      <c r="X43" s="100"/>
+      <c r="Y43" s="98"/>
+      <c r="Z43" s="99"/>
+      <c r="AA43" s="99"/>
+      <c r="AB43" s="99"/>
+      <c r="AC43" s="100"/>
+      <c r="AD43" s="82">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AE43" s="104"/>
-      <c r="AF43" s="104"/>
-      <c r="AG43" s="104"/>
-      <c r="AH43" s="112"/>
-      <c r="AI43" s="106"/>
-      <c r="AJ43" s="107"/>
-      <c r="AK43" s="107"/>
-      <c r="AL43" s="107"/>
-      <c r="AM43" s="107"/>
-      <c r="AN43" s="113"/>
+      <c r="AE43" s="83"/>
+      <c r="AF43" s="83"/>
+      <c r="AG43" s="83"/>
+      <c r="AH43" s="103"/>
+      <c r="AI43" s="95"/>
+      <c r="AJ43" s="96"/>
+      <c r="AK43" s="96"/>
+      <c r="AL43" s="96"/>
+      <c r="AM43" s="96"/>
+      <c r="AN43" s="114"/>
     </row>
     <row r="44" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="154"/>
@@ -6759,38 +6753,38 @@
       <c r="I44" s="155"/>
       <c r="J44" s="155"/>
       <c r="K44" s="156"/>
-      <c r="L44" s="106"/>
-      <c r="M44" s="107"/>
-      <c r="N44" s="108"/>
-      <c r="O44" s="109"/>
-      <c r="P44" s="110"/>
-      <c r="Q44" s="110"/>
-      <c r="R44" s="110"/>
-      <c r="S44" s="111"/>
-      <c r="T44" s="109"/>
-      <c r="U44" s="110"/>
-      <c r="V44" s="110"/>
-      <c r="W44" s="110"/>
-      <c r="X44" s="111"/>
-      <c r="Y44" s="109"/>
-      <c r="Z44" s="110"/>
-      <c r="AA44" s="110"/>
-      <c r="AB44" s="110"/>
-      <c r="AC44" s="111"/>
-      <c r="AD44" s="103">
+      <c r="L44" s="95"/>
+      <c r="M44" s="96"/>
+      <c r="N44" s="97"/>
+      <c r="O44" s="98"/>
+      <c r="P44" s="99"/>
+      <c r="Q44" s="99"/>
+      <c r="R44" s="99"/>
+      <c r="S44" s="100"/>
+      <c r="T44" s="98"/>
+      <c r="U44" s="99"/>
+      <c r="V44" s="99"/>
+      <c r="W44" s="99"/>
+      <c r="X44" s="100"/>
+      <c r="Y44" s="98"/>
+      <c r="Z44" s="99"/>
+      <c r="AA44" s="99"/>
+      <c r="AB44" s="99"/>
+      <c r="AC44" s="100"/>
+      <c r="AD44" s="82">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AE44" s="104"/>
-      <c r="AF44" s="104"/>
-      <c r="AG44" s="104"/>
-      <c r="AH44" s="112"/>
-      <c r="AI44" s="106"/>
-      <c r="AJ44" s="107"/>
-      <c r="AK44" s="107"/>
-      <c r="AL44" s="107"/>
-      <c r="AM44" s="107"/>
-      <c r="AN44" s="113"/>
+      <c r="AE44" s="83"/>
+      <c r="AF44" s="83"/>
+      <c r="AG44" s="83"/>
+      <c r="AH44" s="103"/>
+      <c r="AI44" s="95"/>
+      <c r="AJ44" s="96"/>
+      <c r="AK44" s="96"/>
+      <c r="AL44" s="96"/>
+      <c r="AM44" s="96"/>
+      <c r="AN44" s="114"/>
     </row>
     <row r="45" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="154"/>
@@ -6804,38 +6798,38 @@
       <c r="I45" s="155"/>
       <c r="J45" s="155"/>
       <c r="K45" s="156"/>
-      <c r="L45" s="106"/>
-      <c r="M45" s="107"/>
-      <c r="N45" s="108"/>
-      <c r="O45" s="109"/>
-      <c r="P45" s="110"/>
-      <c r="Q45" s="110"/>
-      <c r="R45" s="110"/>
-      <c r="S45" s="111"/>
-      <c r="T45" s="109"/>
-      <c r="U45" s="110"/>
-      <c r="V45" s="110"/>
-      <c r="W45" s="110"/>
-      <c r="X45" s="111"/>
-      <c r="Y45" s="109"/>
-      <c r="Z45" s="110"/>
-      <c r="AA45" s="110"/>
-      <c r="AB45" s="110"/>
-      <c r="AC45" s="111"/>
-      <c r="AD45" s="103">
+      <c r="L45" s="95"/>
+      <c r="M45" s="96"/>
+      <c r="N45" s="97"/>
+      <c r="O45" s="98"/>
+      <c r="P45" s="99"/>
+      <c r="Q45" s="99"/>
+      <c r="R45" s="99"/>
+      <c r="S45" s="100"/>
+      <c r="T45" s="98"/>
+      <c r="U45" s="99"/>
+      <c r="V45" s="99"/>
+      <c r="W45" s="99"/>
+      <c r="X45" s="100"/>
+      <c r="Y45" s="98"/>
+      <c r="Z45" s="99"/>
+      <c r="AA45" s="99"/>
+      <c r="AB45" s="99"/>
+      <c r="AC45" s="100"/>
+      <c r="AD45" s="82">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AE45" s="104"/>
-      <c r="AF45" s="104"/>
-      <c r="AG45" s="104"/>
-      <c r="AH45" s="112"/>
-      <c r="AI45" s="106"/>
-      <c r="AJ45" s="107"/>
-      <c r="AK45" s="107"/>
-      <c r="AL45" s="107"/>
-      <c r="AM45" s="107"/>
-      <c r="AN45" s="113"/>
+      <c r="AE45" s="83"/>
+      <c r="AF45" s="83"/>
+      <c r="AG45" s="83"/>
+      <c r="AH45" s="103"/>
+      <c r="AI45" s="95"/>
+      <c r="AJ45" s="96"/>
+      <c r="AK45" s="96"/>
+      <c r="AL45" s="96"/>
+      <c r="AM45" s="96"/>
+      <c r="AN45" s="114"/>
     </row>
     <row r="46" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="154"/>
@@ -6849,38 +6843,38 @@
       <c r="I46" s="155"/>
       <c r="J46" s="155"/>
       <c r="K46" s="156"/>
-      <c r="L46" s="106"/>
-      <c r="M46" s="107"/>
-      <c r="N46" s="108"/>
-      <c r="O46" s="109"/>
-      <c r="P46" s="110"/>
-      <c r="Q46" s="110"/>
-      <c r="R46" s="110"/>
-      <c r="S46" s="111"/>
-      <c r="T46" s="109"/>
-      <c r="U46" s="110"/>
-      <c r="V46" s="110"/>
-      <c r="W46" s="110"/>
-      <c r="X46" s="111"/>
-      <c r="Y46" s="109"/>
-      <c r="Z46" s="110"/>
-      <c r="AA46" s="110"/>
-      <c r="AB46" s="110"/>
-      <c r="AC46" s="111"/>
-      <c r="AD46" s="103">
+      <c r="L46" s="95"/>
+      <c r="M46" s="96"/>
+      <c r="N46" s="97"/>
+      <c r="O46" s="98"/>
+      <c r="P46" s="99"/>
+      <c r="Q46" s="99"/>
+      <c r="R46" s="99"/>
+      <c r="S46" s="100"/>
+      <c r="T46" s="98"/>
+      <c r="U46" s="99"/>
+      <c r="V46" s="99"/>
+      <c r="W46" s="99"/>
+      <c r="X46" s="100"/>
+      <c r="Y46" s="98"/>
+      <c r="Z46" s="99"/>
+      <c r="AA46" s="99"/>
+      <c r="AB46" s="99"/>
+      <c r="AC46" s="100"/>
+      <c r="AD46" s="82">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AE46" s="104"/>
-      <c r="AF46" s="104"/>
-      <c r="AG46" s="104"/>
-      <c r="AH46" s="112"/>
-      <c r="AI46" s="106"/>
-      <c r="AJ46" s="107"/>
-      <c r="AK46" s="107"/>
-      <c r="AL46" s="107"/>
-      <c r="AM46" s="107"/>
-      <c r="AN46" s="113"/>
+      <c r="AE46" s="83"/>
+      <c r="AF46" s="83"/>
+      <c r="AG46" s="83"/>
+      <c r="AH46" s="103"/>
+      <c r="AI46" s="95"/>
+      <c r="AJ46" s="96"/>
+      <c r="AK46" s="96"/>
+      <c r="AL46" s="96"/>
+      <c r="AM46" s="96"/>
+      <c r="AN46" s="114"/>
     </row>
     <row r="47" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="154"/>
@@ -6894,103 +6888,103 @@
       <c r="I47" s="155"/>
       <c r="J47" s="155"/>
       <c r="K47" s="156"/>
-      <c r="L47" s="106"/>
-      <c r="M47" s="107"/>
-      <c r="N47" s="108"/>
-      <c r="O47" s="109"/>
-      <c r="P47" s="110"/>
-      <c r="Q47" s="110"/>
-      <c r="R47" s="110"/>
-      <c r="S47" s="111"/>
-      <c r="T47" s="109"/>
-      <c r="U47" s="110"/>
-      <c r="V47" s="110"/>
-      <c r="W47" s="110"/>
-      <c r="X47" s="111"/>
-      <c r="Y47" s="109"/>
-      <c r="Z47" s="110"/>
-      <c r="AA47" s="110"/>
-      <c r="AB47" s="110"/>
-      <c r="AC47" s="111"/>
-      <c r="AD47" s="103">
+      <c r="L47" s="95"/>
+      <c r="M47" s="96"/>
+      <c r="N47" s="97"/>
+      <c r="O47" s="98"/>
+      <c r="P47" s="99"/>
+      <c r="Q47" s="99"/>
+      <c r="R47" s="99"/>
+      <c r="S47" s="100"/>
+      <c r="T47" s="98"/>
+      <c r="U47" s="99"/>
+      <c r="V47" s="99"/>
+      <c r="W47" s="99"/>
+      <c r="X47" s="100"/>
+      <c r="Y47" s="98"/>
+      <c r="Z47" s="99"/>
+      <c r="AA47" s="99"/>
+      <c r="AB47" s="99"/>
+      <c r="AC47" s="100"/>
+      <c r="AD47" s="82">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AE47" s="104"/>
-      <c r="AF47" s="104"/>
-      <c r="AG47" s="104"/>
-      <c r="AH47" s="112"/>
-      <c r="AI47" s="106"/>
-      <c r="AJ47" s="107"/>
-      <c r="AK47" s="107"/>
-      <c r="AL47" s="107"/>
-      <c r="AM47" s="107"/>
-      <c r="AN47" s="113"/>
+      <c r="AE47" s="83"/>
+      <c r="AF47" s="83"/>
+      <c r="AG47" s="83"/>
+      <c r="AH47" s="103"/>
+      <c r="AI47" s="95"/>
+      <c r="AJ47" s="96"/>
+      <c r="AK47" s="96"/>
+      <c r="AL47" s="96"/>
+      <c r="AM47" s="96"/>
+      <c r="AN47" s="114"/>
     </row>
     <row r="48" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="119" t="s">
+      <c r="A48" s="92" t="s">
         <v>25</v>
       </c>
-      <c r="B48" s="120"/>
-      <c r="C48" s="120"/>
-      <c r="D48" s="120"/>
-      <c r="E48" s="120"/>
-      <c r="F48" s="120"/>
-      <c r="G48" s="120"/>
-      <c r="H48" s="120"/>
-      <c r="I48" s="120"/>
-      <c r="J48" s="120"/>
-      <c r="K48" s="121"/>
-      <c r="L48" s="106"/>
-      <c r="M48" s="107"/>
-      <c r="N48" s="108"/>
-      <c r="O48" s="109"/>
-      <c r="P48" s="110"/>
-      <c r="Q48" s="110"/>
-      <c r="R48" s="110"/>
-      <c r="S48" s="111"/>
-      <c r="T48" s="109"/>
-      <c r="U48" s="110"/>
-      <c r="V48" s="110"/>
-      <c r="W48" s="110"/>
-      <c r="X48" s="111"/>
-      <c r="Y48" s="109"/>
-      <c r="Z48" s="110"/>
-      <c r="AA48" s="110"/>
-      <c r="AB48" s="110"/>
-      <c r="AC48" s="111"/>
-      <c r="AD48" s="116">
+      <c r="B48" s="93"/>
+      <c r="C48" s="93"/>
+      <c r="D48" s="93"/>
+      <c r="E48" s="93"/>
+      <c r="F48" s="93"/>
+      <c r="G48" s="93"/>
+      <c r="H48" s="93"/>
+      <c r="I48" s="93"/>
+      <c r="J48" s="93"/>
+      <c r="K48" s="94"/>
+      <c r="L48" s="95"/>
+      <c r="M48" s="96"/>
+      <c r="N48" s="97"/>
+      <c r="O48" s="98"/>
+      <c r="P48" s="99"/>
+      <c r="Q48" s="99"/>
+      <c r="R48" s="99"/>
+      <c r="S48" s="100"/>
+      <c r="T48" s="98"/>
+      <c r="U48" s="99"/>
+      <c r="V48" s="99"/>
+      <c r="W48" s="99"/>
+      <c r="X48" s="100"/>
+      <c r="Y48" s="98"/>
+      <c r="Z48" s="99"/>
+      <c r="AA48" s="99"/>
+      <c r="AB48" s="99"/>
+      <c r="AC48" s="100"/>
+      <c r="AD48" s="104">
         <f>SUM(AD38:AH47)</f>
         <v>0</v>
       </c>
-      <c r="AE48" s="114"/>
-      <c r="AF48" s="114"/>
-      <c r="AG48" s="114"/>
-      <c r="AH48" s="115"/>
-      <c r="AI48" s="116">
+      <c r="AE48" s="105"/>
+      <c r="AF48" s="105"/>
+      <c r="AG48" s="105"/>
+      <c r="AH48" s="113"/>
+      <c r="AI48" s="104">
         <f>SUM(AI38:AN47)</f>
         <v>0</v>
       </c>
-      <c r="AJ48" s="114"/>
-      <c r="AK48" s="114"/>
-      <c r="AL48" s="114"/>
-      <c r="AM48" s="114"/>
-      <c r="AN48" s="117"/>
+      <c r="AJ48" s="105"/>
+      <c r="AK48" s="105"/>
+      <c r="AL48" s="105"/>
+      <c r="AM48" s="105"/>
+      <c r="AN48" s="106"/>
     </row>
     <row r="49" spans="1:40" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="118" t="s">
+      <c r="A49" s="107" t="s">
         <v>29</v>
       </c>
-      <c r="B49" s="101"/>
-      <c r="C49" s="101"/>
-      <c r="D49" s="101"/>
-      <c r="E49" s="101"/>
-      <c r="F49" s="101"/>
-      <c r="G49" s="101"/>
-      <c r="H49" s="101"/>
-      <c r="I49" s="101"/>
-      <c r="J49" s="101"/>
-      <c r="K49" s="102"/>
+      <c r="B49" s="108"/>
+      <c r="C49" s="108"/>
+      <c r="D49" s="108"/>
+      <c r="E49" s="108"/>
+      <c r="F49" s="108"/>
+      <c r="G49" s="108"/>
+      <c r="H49" s="108"/>
+      <c r="I49" s="108"/>
+      <c r="J49" s="108"/>
+      <c r="K49" s="109"/>
       <c r="L49" s="23"/>
       <c r="M49" s="25"/>
       <c r="N49" s="38"/>
@@ -7022,17 +7016,17 @@
       <c r="AN49" s="26"/>
     </row>
     <row r="50" spans="1:40" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="88"/>
-      <c r="B50" s="89"/>
-      <c r="C50" s="89"/>
-      <c r="D50" s="89"/>
-      <c r="E50" s="89"/>
-      <c r="F50" s="89"/>
-      <c r="G50" s="89"/>
-      <c r="H50" s="89"/>
-      <c r="I50" s="89"/>
-      <c r="J50" s="89"/>
-      <c r="K50" s="90"/>
+      <c r="A50" s="110"/>
+      <c r="B50" s="111"/>
+      <c r="C50" s="111"/>
+      <c r="D50" s="111"/>
+      <c r="E50" s="111"/>
+      <c r="F50" s="111"/>
+      <c r="G50" s="111"/>
+      <c r="H50" s="111"/>
+      <c r="I50" s="111"/>
+      <c r="J50" s="111"/>
+      <c r="K50" s="112"/>
       <c r="L50" s="24"/>
       <c r="M50" s="16"/>
       <c r="N50" s="37"/>
@@ -7063,501 +7057,501 @@
       <c r="AM50" s="16"/>
       <c r="AN50" s="17"/>
     </row>
-    <row r="51" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="157"/>
-      <c r="B51" s="158"/>
-      <c r="C51" s="158"/>
-      <c r="D51" s="158"/>
-      <c r="E51" s="158"/>
-      <c r="F51" s="158"/>
-      <c r="G51" s="158"/>
-      <c r="H51" s="158"/>
-      <c r="I51" s="158"/>
-      <c r="J51" s="158"/>
-      <c r="K51" s="159"/>
-      <c r="L51" s="106"/>
-      <c r="M51" s="107"/>
-      <c r="N51" s="108"/>
-      <c r="O51" s="109"/>
-      <c r="P51" s="110"/>
-      <c r="Q51" s="110"/>
-      <c r="R51" s="110"/>
-      <c r="S51" s="111"/>
-      <c r="T51" s="109"/>
-      <c r="U51" s="110"/>
-      <c r="V51" s="110"/>
-      <c r="W51" s="110"/>
-      <c r="X51" s="111"/>
-      <c r="Y51" s="109"/>
-      <c r="Z51" s="110"/>
-      <c r="AA51" s="110"/>
-      <c r="AB51" s="110"/>
-      <c r="AC51" s="111"/>
-      <c r="AD51" s="103">
+    <row r="51" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="154"/>
+      <c r="B51" s="155"/>
+      <c r="C51" s="155"/>
+      <c r="D51" s="155"/>
+      <c r="E51" s="155"/>
+      <c r="F51" s="155"/>
+      <c r="G51" s="155"/>
+      <c r="H51" s="155"/>
+      <c r="I51" s="155"/>
+      <c r="J51" s="155"/>
+      <c r="K51" s="156"/>
+      <c r="L51" s="95"/>
+      <c r="M51" s="96"/>
+      <c r="N51" s="97"/>
+      <c r="O51" s="98"/>
+      <c r="P51" s="99"/>
+      <c r="Q51" s="99"/>
+      <c r="R51" s="99"/>
+      <c r="S51" s="100"/>
+      <c r="T51" s="98"/>
+      <c r="U51" s="99"/>
+      <c r="V51" s="99"/>
+      <c r="W51" s="99"/>
+      <c r="X51" s="100"/>
+      <c r="Y51" s="98"/>
+      <c r="Z51" s="99"/>
+      <c r="AA51" s="99"/>
+      <c r="AB51" s="99"/>
+      <c r="AC51" s="100"/>
+      <c r="AD51" s="82">
         <f>SUM(O51:AC51)</f>
         <v>0</v>
       </c>
-      <c r="AE51" s="104"/>
-      <c r="AF51" s="104"/>
-      <c r="AG51" s="104"/>
-      <c r="AH51" s="112"/>
-      <c r="AI51" s="103"/>
-      <c r="AJ51" s="104"/>
-      <c r="AK51" s="104"/>
-      <c r="AL51" s="104"/>
-      <c r="AM51" s="104"/>
-      <c r="AN51" s="105"/>
+      <c r="AE51" s="83"/>
+      <c r="AF51" s="83"/>
+      <c r="AG51" s="83"/>
+      <c r="AH51" s="103"/>
+      <c r="AI51" s="82"/>
+      <c r="AJ51" s="83"/>
+      <c r="AK51" s="83"/>
+      <c r="AL51" s="83"/>
+      <c r="AM51" s="83"/>
+      <c r="AN51" s="84"/>
     </row>
-    <row r="52" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="157"/>
-      <c r="B52" s="158"/>
-      <c r="C52" s="158"/>
-      <c r="D52" s="158"/>
-      <c r="E52" s="158"/>
-      <c r="F52" s="158"/>
-      <c r="G52" s="158"/>
-      <c r="H52" s="158"/>
-      <c r="I52" s="158"/>
-      <c r="J52" s="158"/>
-      <c r="K52" s="159"/>
-      <c r="L52" s="106"/>
-      <c r="M52" s="107"/>
-      <c r="N52" s="108"/>
-      <c r="O52" s="109"/>
-      <c r="P52" s="110"/>
-      <c r="Q52" s="110"/>
-      <c r="R52" s="110"/>
-      <c r="S52" s="111"/>
-      <c r="T52" s="109"/>
-      <c r="U52" s="110"/>
-      <c r="V52" s="110"/>
-      <c r="W52" s="110"/>
-      <c r="X52" s="111"/>
-      <c r="Y52" s="109"/>
-      <c r="Z52" s="110"/>
-      <c r="AA52" s="110"/>
-      <c r="AB52" s="110"/>
-      <c r="AC52" s="111"/>
-      <c r="AD52" s="103">
+    <row r="52" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="154"/>
+      <c r="B52" s="155"/>
+      <c r="C52" s="155"/>
+      <c r="D52" s="155"/>
+      <c r="E52" s="155"/>
+      <c r="F52" s="155"/>
+      <c r="G52" s="155"/>
+      <c r="H52" s="155"/>
+      <c r="I52" s="155"/>
+      <c r="J52" s="155"/>
+      <c r="K52" s="156"/>
+      <c r="L52" s="95"/>
+      <c r="M52" s="96"/>
+      <c r="N52" s="97"/>
+      <c r="O52" s="98"/>
+      <c r="P52" s="99"/>
+      <c r="Q52" s="99"/>
+      <c r="R52" s="99"/>
+      <c r="S52" s="100"/>
+      <c r="T52" s="98"/>
+      <c r="U52" s="99"/>
+      <c r="V52" s="99"/>
+      <c r="W52" s="99"/>
+      <c r="X52" s="100"/>
+      <c r="Y52" s="98"/>
+      <c r="Z52" s="99"/>
+      <c r="AA52" s="99"/>
+      <c r="AB52" s="99"/>
+      <c r="AC52" s="100"/>
+      <c r="AD52" s="82">
         <f t="shared" ref="AD52:AD59" si="1">SUM(O52:AC52)</f>
         <v>0</v>
       </c>
-      <c r="AE52" s="104"/>
-      <c r="AF52" s="104"/>
-      <c r="AG52" s="104"/>
-      <c r="AH52" s="112"/>
-      <c r="AI52" s="103"/>
-      <c r="AJ52" s="104"/>
-      <c r="AK52" s="104"/>
-      <c r="AL52" s="104"/>
-      <c r="AM52" s="104"/>
-      <c r="AN52" s="105"/>
+      <c r="AE52" s="83"/>
+      <c r="AF52" s="83"/>
+      <c r="AG52" s="83"/>
+      <c r="AH52" s="103"/>
+      <c r="AI52" s="82"/>
+      <c r="AJ52" s="83"/>
+      <c r="AK52" s="83"/>
+      <c r="AL52" s="83"/>
+      <c r="AM52" s="83"/>
+      <c r="AN52" s="84"/>
     </row>
-    <row r="53" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="157"/>
-      <c r="B53" s="158"/>
-      <c r="C53" s="158"/>
-      <c r="D53" s="158"/>
-      <c r="E53" s="158"/>
-      <c r="F53" s="158"/>
-      <c r="G53" s="158"/>
-      <c r="H53" s="158"/>
-      <c r="I53" s="158"/>
-      <c r="J53" s="158"/>
-      <c r="K53" s="159"/>
-      <c r="L53" s="106"/>
-      <c r="M53" s="107"/>
-      <c r="N53" s="108"/>
-      <c r="O53" s="109"/>
-      <c r="P53" s="110"/>
-      <c r="Q53" s="110"/>
-      <c r="R53" s="110"/>
-      <c r="S53" s="111"/>
-      <c r="T53" s="109"/>
-      <c r="U53" s="110"/>
-      <c r="V53" s="110"/>
-      <c r="W53" s="110"/>
-      <c r="X53" s="111"/>
-      <c r="Y53" s="109"/>
-      <c r="Z53" s="110"/>
-      <c r="AA53" s="110"/>
-      <c r="AB53" s="110"/>
-      <c r="AC53" s="111"/>
-      <c r="AD53" s="103">
+    <row r="53" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="154"/>
+      <c r="B53" s="155"/>
+      <c r="C53" s="155"/>
+      <c r="D53" s="155"/>
+      <c r="E53" s="155"/>
+      <c r="F53" s="155"/>
+      <c r="G53" s="155"/>
+      <c r="H53" s="155"/>
+      <c r="I53" s="155"/>
+      <c r="J53" s="155"/>
+      <c r="K53" s="156"/>
+      <c r="L53" s="95"/>
+      <c r="M53" s="96"/>
+      <c r="N53" s="97"/>
+      <c r="O53" s="98"/>
+      <c r="P53" s="99"/>
+      <c r="Q53" s="99"/>
+      <c r="R53" s="99"/>
+      <c r="S53" s="100"/>
+      <c r="T53" s="98"/>
+      <c r="U53" s="99"/>
+      <c r="V53" s="99"/>
+      <c r="W53" s="99"/>
+      <c r="X53" s="100"/>
+      <c r="Y53" s="98"/>
+      <c r="Z53" s="99"/>
+      <c r="AA53" s="99"/>
+      <c r="AB53" s="99"/>
+      <c r="AC53" s="100"/>
+      <c r="AD53" s="82">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AE53" s="104"/>
-      <c r="AF53" s="104"/>
-      <c r="AG53" s="104"/>
-      <c r="AH53" s="112"/>
-      <c r="AI53" s="103"/>
-      <c r="AJ53" s="104"/>
-      <c r="AK53" s="104"/>
-      <c r="AL53" s="104"/>
-      <c r="AM53" s="104"/>
-      <c r="AN53" s="105"/>
+      <c r="AE53" s="83"/>
+      <c r="AF53" s="83"/>
+      <c r="AG53" s="83"/>
+      <c r="AH53" s="103"/>
+      <c r="AI53" s="82"/>
+      <c r="AJ53" s="83"/>
+      <c r="AK53" s="83"/>
+      <c r="AL53" s="83"/>
+      <c r="AM53" s="83"/>
+      <c r="AN53" s="84"/>
     </row>
-    <row r="54" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="157"/>
-      <c r="B54" s="158"/>
-      <c r="C54" s="158"/>
-      <c r="D54" s="158"/>
-      <c r="E54" s="158"/>
-      <c r="F54" s="158"/>
-      <c r="G54" s="158"/>
-      <c r="H54" s="158"/>
-      <c r="I54" s="158"/>
-      <c r="J54" s="158"/>
-      <c r="K54" s="159"/>
-      <c r="L54" s="106"/>
-      <c r="M54" s="107"/>
-      <c r="N54" s="108"/>
-      <c r="O54" s="109"/>
-      <c r="P54" s="110"/>
-      <c r="Q54" s="110"/>
-      <c r="R54" s="110"/>
-      <c r="S54" s="111"/>
-      <c r="T54" s="109"/>
-      <c r="U54" s="110"/>
-      <c r="V54" s="110"/>
-      <c r="W54" s="110"/>
-      <c r="X54" s="111"/>
-      <c r="Y54" s="109"/>
-      <c r="Z54" s="110"/>
-      <c r="AA54" s="110"/>
-      <c r="AB54" s="110"/>
-      <c r="AC54" s="111"/>
-      <c r="AD54" s="103">
+    <row r="54" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="154"/>
+      <c r="B54" s="155"/>
+      <c r="C54" s="155"/>
+      <c r="D54" s="155"/>
+      <c r="E54" s="155"/>
+      <c r="F54" s="155"/>
+      <c r="G54" s="155"/>
+      <c r="H54" s="155"/>
+      <c r="I54" s="155"/>
+      <c r="J54" s="155"/>
+      <c r="K54" s="156"/>
+      <c r="L54" s="95"/>
+      <c r="M54" s="96"/>
+      <c r="N54" s="97"/>
+      <c r="O54" s="98"/>
+      <c r="P54" s="99"/>
+      <c r="Q54" s="99"/>
+      <c r="R54" s="99"/>
+      <c r="S54" s="100"/>
+      <c r="T54" s="98"/>
+      <c r="U54" s="99"/>
+      <c r="V54" s="99"/>
+      <c r="W54" s="99"/>
+      <c r="X54" s="100"/>
+      <c r="Y54" s="98"/>
+      <c r="Z54" s="99"/>
+      <c r="AA54" s="99"/>
+      <c r="AB54" s="99"/>
+      <c r="AC54" s="100"/>
+      <c r="AD54" s="82">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AE54" s="104"/>
-      <c r="AF54" s="104"/>
-      <c r="AG54" s="104"/>
-      <c r="AH54" s="112"/>
-      <c r="AI54" s="103"/>
-      <c r="AJ54" s="104"/>
-      <c r="AK54" s="104"/>
-      <c r="AL54" s="104"/>
-      <c r="AM54" s="104"/>
-      <c r="AN54" s="105"/>
+      <c r="AE54" s="83"/>
+      <c r="AF54" s="83"/>
+      <c r="AG54" s="83"/>
+      <c r="AH54" s="103"/>
+      <c r="AI54" s="82"/>
+      <c r="AJ54" s="83"/>
+      <c r="AK54" s="83"/>
+      <c r="AL54" s="83"/>
+      <c r="AM54" s="83"/>
+      <c r="AN54" s="84"/>
     </row>
-    <row r="55" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="157"/>
-      <c r="B55" s="158"/>
-      <c r="C55" s="158"/>
-      <c r="D55" s="158"/>
-      <c r="E55" s="158"/>
-      <c r="F55" s="158"/>
-      <c r="G55" s="158"/>
-      <c r="H55" s="158"/>
-      <c r="I55" s="158"/>
-      <c r="J55" s="158"/>
-      <c r="K55" s="159"/>
-      <c r="L55" s="106"/>
-      <c r="M55" s="107"/>
-      <c r="N55" s="108"/>
-      <c r="O55" s="109"/>
-      <c r="P55" s="110"/>
-      <c r="Q55" s="110"/>
-      <c r="R55" s="110"/>
-      <c r="S55" s="111"/>
-      <c r="T55" s="109"/>
-      <c r="U55" s="110"/>
-      <c r="V55" s="110"/>
-      <c r="W55" s="110"/>
-      <c r="X55" s="111"/>
-      <c r="Y55" s="109"/>
-      <c r="Z55" s="110"/>
-      <c r="AA55" s="110"/>
-      <c r="AB55" s="110"/>
-      <c r="AC55" s="111"/>
-      <c r="AD55" s="103">
+    <row r="55" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="154"/>
+      <c r="B55" s="155"/>
+      <c r="C55" s="155"/>
+      <c r="D55" s="155"/>
+      <c r="E55" s="155"/>
+      <c r="F55" s="155"/>
+      <c r="G55" s="155"/>
+      <c r="H55" s="155"/>
+      <c r="I55" s="155"/>
+      <c r="J55" s="155"/>
+      <c r="K55" s="156"/>
+      <c r="L55" s="95"/>
+      <c r="M55" s="96"/>
+      <c r="N55" s="97"/>
+      <c r="O55" s="98"/>
+      <c r="P55" s="99"/>
+      <c r="Q55" s="99"/>
+      <c r="R55" s="99"/>
+      <c r="S55" s="100"/>
+      <c r="T55" s="98"/>
+      <c r="U55" s="99"/>
+      <c r="V55" s="99"/>
+      <c r="W55" s="99"/>
+      <c r="X55" s="100"/>
+      <c r="Y55" s="98"/>
+      <c r="Z55" s="99"/>
+      <c r="AA55" s="99"/>
+      <c r="AB55" s="99"/>
+      <c r="AC55" s="100"/>
+      <c r="AD55" s="82">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AE55" s="104"/>
-      <c r="AF55" s="104"/>
-      <c r="AG55" s="104"/>
-      <c r="AH55" s="112"/>
-      <c r="AI55" s="103"/>
-      <c r="AJ55" s="104"/>
-      <c r="AK55" s="104"/>
-      <c r="AL55" s="104"/>
-      <c r="AM55" s="104"/>
-      <c r="AN55" s="105"/>
+      <c r="AE55" s="83"/>
+      <c r="AF55" s="83"/>
+      <c r="AG55" s="83"/>
+      <c r="AH55" s="103"/>
+      <c r="AI55" s="82"/>
+      <c r="AJ55" s="83"/>
+      <c r="AK55" s="83"/>
+      <c r="AL55" s="83"/>
+      <c r="AM55" s="83"/>
+      <c r="AN55" s="84"/>
     </row>
-    <row r="56" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="157"/>
-      <c r="B56" s="158"/>
-      <c r="C56" s="158"/>
-      <c r="D56" s="158"/>
-      <c r="E56" s="158"/>
-      <c r="F56" s="158"/>
-      <c r="G56" s="158"/>
-      <c r="H56" s="158"/>
-      <c r="I56" s="158"/>
-      <c r="J56" s="158"/>
-      <c r="K56" s="159"/>
-      <c r="L56" s="106"/>
-      <c r="M56" s="107"/>
-      <c r="N56" s="108"/>
-      <c r="O56" s="109"/>
-      <c r="P56" s="110"/>
-      <c r="Q56" s="110"/>
-      <c r="R56" s="110"/>
-      <c r="S56" s="111"/>
-      <c r="T56" s="109"/>
-      <c r="U56" s="110"/>
-      <c r="V56" s="110"/>
-      <c r="W56" s="110"/>
-      <c r="X56" s="111"/>
-      <c r="Y56" s="109"/>
-      <c r="Z56" s="110"/>
-      <c r="AA56" s="110"/>
-      <c r="AB56" s="110"/>
-      <c r="AC56" s="111"/>
-      <c r="AD56" s="103">
+    <row r="56" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="154"/>
+      <c r="B56" s="155"/>
+      <c r="C56" s="155"/>
+      <c r="D56" s="155"/>
+      <c r="E56" s="155"/>
+      <c r="F56" s="155"/>
+      <c r="G56" s="155"/>
+      <c r="H56" s="155"/>
+      <c r="I56" s="155"/>
+      <c r="J56" s="155"/>
+      <c r="K56" s="156"/>
+      <c r="L56" s="95"/>
+      <c r="M56" s="96"/>
+      <c r="N56" s="97"/>
+      <c r="O56" s="98"/>
+      <c r="P56" s="99"/>
+      <c r="Q56" s="99"/>
+      <c r="R56" s="99"/>
+      <c r="S56" s="100"/>
+      <c r="T56" s="98"/>
+      <c r="U56" s="99"/>
+      <c r="V56" s="99"/>
+      <c r="W56" s="99"/>
+      <c r="X56" s="100"/>
+      <c r="Y56" s="98"/>
+      <c r="Z56" s="99"/>
+      <c r="AA56" s="99"/>
+      <c r="AB56" s="99"/>
+      <c r="AC56" s="100"/>
+      <c r="AD56" s="82">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AE56" s="104"/>
-      <c r="AF56" s="104"/>
-      <c r="AG56" s="104"/>
-      <c r="AH56" s="112"/>
-      <c r="AI56" s="103"/>
-      <c r="AJ56" s="104"/>
-      <c r="AK56" s="104"/>
-      <c r="AL56" s="104"/>
-      <c r="AM56" s="104"/>
-      <c r="AN56" s="105"/>
+      <c r="AE56" s="83"/>
+      <c r="AF56" s="83"/>
+      <c r="AG56" s="83"/>
+      <c r="AH56" s="103"/>
+      <c r="AI56" s="82"/>
+      <c r="AJ56" s="83"/>
+      <c r="AK56" s="83"/>
+      <c r="AL56" s="83"/>
+      <c r="AM56" s="83"/>
+      <c r="AN56" s="84"/>
     </row>
-    <row r="57" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="157"/>
-      <c r="B57" s="158"/>
-      <c r="C57" s="158"/>
-      <c r="D57" s="158"/>
-      <c r="E57" s="158"/>
-      <c r="F57" s="158"/>
-      <c r="G57" s="158"/>
-      <c r="H57" s="158"/>
-      <c r="I57" s="158"/>
-      <c r="J57" s="158"/>
-      <c r="K57" s="159"/>
-      <c r="L57" s="106"/>
-      <c r="M57" s="107"/>
-      <c r="N57" s="108"/>
-      <c r="O57" s="109"/>
-      <c r="P57" s="110"/>
-      <c r="Q57" s="110"/>
-      <c r="R57" s="110"/>
-      <c r="S57" s="111"/>
-      <c r="T57" s="109"/>
-      <c r="U57" s="110"/>
-      <c r="V57" s="110"/>
-      <c r="W57" s="110"/>
-      <c r="X57" s="111"/>
-      <c r="Y57" s="109"/>
-      <c r="Z57" s="110"/>
-      <c r="AA57" s="110"/>
-      <c r="AB57" s="110"/>
-      <c r="AC57" s="111"/>
-      <c r="AD57" s="103">
+    <row r="57" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="154"/>
+      <c r="B57" s="155"/>
+      <c r="C57" s="155"/>
+      <c r="D57" s="155"/>
+      <c r="E57" s="155"/>
+      <c r="F57" s="155"/>
+      <c r="G57" s="155"/>
+      <c r="H57" s="155"/>
+      <c r="I57" s="155"/>
+      <c r="J57" s="155"/>
+      <c r="K57" s="156"/>
+      <c r="L57" s="95"/>
+      <c r="M57" s="96"/>
+      <c r="N57" s="97"/>
+      <c r="O57" s="98"/>
+      <c r="P57" s="99"/>
+      <c r="Q57" s="99"/>
+      <c r="R57" s="99"/>
+      <c r="S57" s="100"/>
+      <c r="T57" s="98"/>
+      <c r="U57" s="99"/>
+      <c r="V57" s="99"/>
+      <c r="W57" s="99"/>
+      <c r="X57" s="100"/>
+      <c r="Y57" s="98"/>
+      <c r="Z57" s="99"/>
+      <c r="AA57" s="99"/>
+      <c r="AB57" s="99"/>
+      <c r="AC57" s="100"/>
+      <c r="AD57" s="82">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AE57" s="104"/>
-      <c r="AF57" s="104"/>
-      <c r="AG57" s="104"/>
-      <c r="AH57" s="112"/>
-      <c r="AI57" s="103"/>
-      <c r="AJ57" s="104"/>
-      <c r="AK57" s="104"/>
-      <c r="AL57" s="104"/>
-      <c r="AM57" s="104"/>
-      <c r="AN57" s="105"/>
+      <c r="AE57" s="83"/>
+      <c r="AF57" s="83"/>
+      <c r="AG57" s="83"/>
+      <c r="AH57" s="103"/>
+      <c r="AI57" s="82"/>
+      <c r="AJ57" s="83"/>
+      <c r="AK57" s="83"/>
+      <c r="AL57" s="83"/>
+      <c r="AM57" s="83"/>
+      <c r="AN57" s="84"/>
     </row>
-    <row r="58" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="157"/>
-      <c r="B58" s="158"/>
-      <c r="C58" s="158"/>
-      <c r="D58" s="158"/>
-      <c r="E58" s="158"/>
-      <c r="F58" s="158"/>
-      <c r="G58" s="158"/>
-      <c r="H58" s="158"/>
-      <c r="I58" s="158"/>
-      <c r="J58" s="158"/>
-      <c r="K58" s="159"/>
-      <c r="L58" s="106"/>
-      <c r="M58" s="107"/>
-      <c r="N58" s="108"/>
-      <c r="O58" s="109"/>
-      <c r="P58" s="110"/>
-      <c r="Q58" s="110"/>
-      <c r="R58" s="110"/>
-      <c r="S58" s="111"/>
-      <c r="T58" s="109"/>
-      <c r="U58" s="110"/>
-      <c r="V58" s="110"/>
-      <c r="W58" s="110"/>
-      <c r="X58" s="111"/>
-      <c r="Y58" s="109"/>
-      <c r="Z58" s="110"/>
-      <c r="AA58" s="110"/>
-      <c r="AB58" s="110"/>
-      <c r="AC58" s="111"/>
-      <c r="AD58" s="103">
+    <row r="58" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="154"/>
+      <c r="B58" s="155"/>
+      <c r="C58" s="155"/>
+      <c r="D58" s="155"/>
+      <c r="E58" s="155"/>
+      <c r="F58" s="155"/>
+      <c r="G58" s="155"/>
+      <c r="H58" s="155"/>
+      <c r="I58" s="155"/>
+      <c r="J58" s="155"/>
+      <c r="K58" s="156"/>
+      <c r="L58" s="95"/>
+      <c r="M58" s="96"/>
+      <c r="N58" s="97"/>
+      <c r="O58" s="98"/>
+      <c r="P58" s="99"/>
+      <c r="Q58" s="99"/>
+      <c r="R58" s="99"/>
+      <c r="S58" s="100"/>
+      <c r="T58" s="98"/>
+      <c r="U58" s="99"/>
+      <c r="V58" s="99"/>
+      <c r="W58" s="99"/>
+      <c r="X58" s="100"/>
+      <c r="Y58" s="98"/>
+      <c r="Z58" s="99"/>
+      <c r="AA58" s="99"/>
+      <c r="AB58" s="99"/>
+      <c r="AC58" s="100"/>
+      <c r="AD58" s="82">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AE58" s="104"/>
-      <c r="AF58" s="104"/>
-      <c r="AG58" s="104"/>
-      <c r="AH58" s="112"/>
-      <c r="AI58" s="103"/>
-      <c r="AJ58" s="104"/>
-      <c r="AK58" s="104"/>
-      <c r="AL58" s="104"/>
-      <c r="AM58" s="104"/>
-      <c r="AN58" s="105"/>
+      <c r="AE58" s="83"/>
+      <c r="AF58" s="83"/>
+      <c r="AG58" s="83"/>
+      <c r="AH58" s="103"/>
+      <c r="AI58" s="82"/>
+      <c r="AJ58" s="83"/>
+      <c r="AK58" s="83"/>
+      <c r="AL58" s="83"/>
+      <c r="AM58" s="83"/>
+      <c r="AN58" s="84"/>
     </row>
-    <row r="59" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="157"/>
-      <c r="B59" s="158"/>
-      <c r="C59" s="158"/>
-      <c r="D59" s="158"/>
-      <c r="E59" s="158"/>
-      <c r="F59" s="158"/>
-      <c r="G59" s="158"/>
-      <c r="H59" s="158"/>
-      <c r="I59" s="158"/>
-      <c r="J59" s="158"/>
-      <c r="K59" s="159"/>
-      <c r="L59" s="106"/>
-      <c r="M59" s="107"/>
-      <c r="N59" s="108"/>
-      <c r="O59" s="109"/>
-      <c r="P59" s="110"/>
-      <c r="Q59" s="110"/>
-      <c r="R59" s="110"/>
-      <c r="S59" s="111"/>
-      <c r="T59" s="109"/>
-      <c r="U59" s="110"/>
-      <c r="V59" s="110"/>
-      <c r="W59" s="110"/>
-      <c r="X59" s="111"/>
-      <c r="Y59" s="109"/>
-      <c r="Z59" s="110"/>
-      <c r="AA59" s="110"/>
-      <c r="AB59" s="110"/>
-      <c r="AC59" s="111"/>
-      <c r="AD59" s="103">
+    <row r="59" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="154"/>
+      <c r="B59" s="155"/>
+      <c r="C59" s="155"/>
+      <c r="D59" s="155"/>
+      <c r="E59" s="155"/>
+      <c r="F59" s="155"/>
+      <c r="G59" s="155"/>
+      <c r="H59" s="155"/>
+      <c r="I59" s="155"/>
+      <c r="J59" s="155"/>
+      <c r="K59" s="156"/>
+      <c r="L59" s="95"/>
+      <c r="M59" s="96"/>
+      <c r="N59" s="97"/>
+      <c r="O59" s="98"/>
+      <c r="P59" s="99"/>
+      <c r="Q59" s="99"/>
+      <c r="R59" s="99"/>
+      <c r="S59" s="100"/>
+      <c r="T59" s="98"/>
+      <c r="U59" s="99"/>
+      <c r="V59" s="99"/>
+      <c r="W59" s="99"/>
+      <c r="X59" s="100"/>
+      <c r="Y59" s="98"/>
+      <c r="Z59" s="99"/>
+      <c r="AA59" s="99"/>
+      <c r="AB59" s="99"/>
+      <c r="AC59" s="100"/>
+      <c r="AD59" s="82">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AE59" s="104"/>
-      <c r="AF59" s="104"/>
-      <c r="AG59" s="104"/>
-      <c r="AH59" s="112"/>
-      <c r="AI59" s="103"/>
-      <c r="AJ59" s="104"/>
-      <c r="AK59" s="104"/>
-      <c r="AL59" s="104"/>
-      <c r="AM59" s="104"/>
-      <c r="AN59" s="105"/>
+      <c r="AE59" s="83"/>
+      <c r="AF59" s="83"/>
+      <c r="AG59" s="83"/>
+      <c r="AH59" s="103"/>
+      <c r="AI59" s="82"/>
+      <c r="AJ59" s="83"/>
+      <c r="AK59" s="83"/>
+      <c r="AL59" s="83"/>
+      <c r="AM59" s="83"/>
+      <c r="AN59" s="84"/>
     </row>
     <row r="60" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="119" t="s">
+      <c r="A60" s="92" t="s">
         <v>25</v>
       </c>
-      <c r="B60" s="120"/>
-      <c r="C60" s="120"/>
-      <c r="D60" s="120"/>
-      <c r="E60" s="120"/>
-      <c r="F60" s="120"/>
-      <c r="G60" s="120"/>
-      <c r="H60" s="120"/>
-      <c r="I60" s="120"/>
-      <c r="J60" s="120"/>
-      <c r="K60" s="121"/>
-      <c r="L60" s="106"/>
-      <c r="M60" s="107"/>
-      <c r="N60" s="108"/>
-      <c r="O60" s="109"/>
-      <c r="P60" s="110"/>
-      <c r="Q60" s="110"/>
-      <c r="R60" s="110"/>
-      <c r="S60" s="111"/>
-      <c r="T60" s="109"/>
-      <c r="U60" s="110"/>
-      <c r="V60" s="110"/>
-      <c r="W60" s="110"/>
-      <c r="X60" s="111"/>
-      <c r="Y60" s="109"/>
-      <c r="Z60" s="110"/>
-      <c r="AA60" s="110"/>
-      <c r="AB60" s="110"/>
-      <c r="AC60" s="111"/>
-      <c r="AD60" s="106"/>
-      <c r="AE60" s="107"/>
-      <c r="AF60" s="107"/>
-      <c r="AG60" s="107"/>
-      <c r="AH60" s="108"/>
-      <c r="AI60" s="103">
+      <c r="B60" s="93"/>
+      <c r="C60" s="93"/>
+      <c r="D60" s="93"/>
+      <c r="E60" s="93"/>
+      <c r="F60" s="93"/>
+      <c r="G60" s="93"/>
+      <c r="H60" s="93"/>
+      <c r="I60" s="93"/>
+      <c r="J60" s="93"/>
+      <c r="K60" s="94"/>
+      <c r="L60" s="95"/>
+      <c r="M60" s="96"/>
+      <c r="N60" s="97"/>
+      <c r="O60" s="98"/>
+      <c r="P60" s="99"/>
+      <c r="Q60" s="99"/>
+      <c r="R60" s="99"/>
+      <c r="S60" s="100"/>
+      <c r="T60" s="98"/>
+      <c r="U60" s="99"/>
+      <c r="V60" s="99"/>
+      <c r="W60" s="99"/>
+      <c r="X60" s="100"/>
+      <c r="Y60" s="98"/>
+      <c r="Z60" s="99"/>
+      <c r="AA60" s="99"/>
+      <c r="AB60" s="99"/>
+      <c r="AC60" s="100"/>
+      <c r="AD60" s="95"/>
+      <c r="AE60" s="96"/>
+      <c r="AF60" s="96"/>
+      <c r="AG60" s="96"/>
+      <c r="AH60" s="97"/>
+      <c r="AI60" s="82">
         <f>SUM(AI50:AN59)</f>
         <v>0</v>
       </c>
-      <c r="AJ60" s="104"/>
-      <c r="AK60" s="104"/>
-      <c r="AL60" s="104"/>
-      <c r="AM60" s="104"/>
-      <c r="AN60" s="105"/>
+      <c r="AJ60" s="83"/>
+      <c r="AK60" s="83"/>
+      <c r="AL60" s="83"/>
+      <c r="AM60" s="83"/>
+      <c r="AN60" s="84"/>
     </row>
     <row r="61" spans="1:40" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="122" t="s">
+      <c r="A61" s="85" t="s">
         <v>38</v>
       </c>
-      <c r="B61" s="123"/>
-      <c r="C61" s="123"/>
-      <c r="D61" s="123"/>
-      <c r="E61" s="123"/>
-      <c r="F61" s="123"/>
-      <c r="G61" s="123"/>
-      <c r="H61" s="123"/>
-      <c r="I61" s="123"/>
-      <c r="J61" s="123"/>
-      <c r="K61" s="123"/>
-      <c r="L61" s="123"/>
-      <c r="M61" s="123"/>
-      <c r="N61" s="123"/>
-      <c r="O61" s="123"/>
-      <c r="P61" s="123"/>
-      <c r="Q61" s="123"/>
-      <c r="R61" s="123"/>
-      <c r="S61" s="123"/>
-      <c r="T61" s="123"/>
-      <c r="U61" s="123"/>
-      <c r="V61" s="123"/>
-      <c r="W61" s="123"/>
-      <c r="X61" s="123"/>
-      <c r="Y61" s="123"/>
-      <c r="Z61" s="123"/>
-      <c r="AA61" s="123"/>
-      <c r="AB61" s="123"/>
-      <c r="AC61" s="123"/>
-      <c r="AD61" s="123"/>
-      <c r="AE61" s="123"/>
-      <c r="AF61" s="123"/>
-      <c r="AG61" s="123"/>
-      <c r="AH61" s="123"/>
-      <c r="AI61" s="123"/>
-      <c r="AJ61" s="123"/>
-      <c r="AK61" s="123"/>
-      <c r="AL61" s="123"/>
-      <c r="AM61" s="123"/>
-      <c r="AN61" s="124"/>
+      <c r="B61" s="86"/>
+      <c r="C61" s="86"/>
+      <c r="D61" s="86"/>
+      <c r="E61" s="86"/>
+      <c r="F61" s="86"/>
+      <c r="G61" s="86"/>
+      <c r="H61" s="86"/>
+      <c r="I61" s="86"/>
+      <c r="J61" s="86"/>
+      <c r="K61" s="86"/>
+      <c r="L61" s="86"/>
+      <c r="M61" s="86"/>
+      <c r="N61" s="86"/>
+      <c r="O61" s="86"/>
+      <c r="P61" s="86"/>
+      <c r="Q61" s="86"/>
+      <c r="R61" s="86"/>
+      <c r="S61" s="86"/>
+      <c r="T61" s="86"/>
+      <c r="U61" s="86"/>
+      <c r="V61" s="86"/>
+      <c r="W61" s="86"/>
+      <c r="X61" s="86"/>
+      <c r="Y61" s="86"/>
+      <c r="Z61" s="86"/>
+      <c r="AA61" s="86"/>
+      <c r="AB61" s="86"/>
+      <c r="AC61" s="86"/>
+      <c r="AD61" s="86"/>
+      <c r="AE61" s="86"/>
+      <c r="AF61" s="86"/>
+      <c r="AG61" s="86"/>
+      <c r="AH61" s="86"/>
+      <c r="AI61" s="86"/>
+      <c r="AJ61" s="86"/>
+      <c r="AK61" s="86"/>
+      <c r="AL61" s="86"/>
+      <c r="AM61" s="86"/>
+      <c r="AN61" s="87"/>
     </row>
     <row r="62" spans="1:40" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="43"/>
@@ -7575,17 +7569,17 @@
       <c r="M62" s="44"/>
       <c r="N62" s="44"/>
       <c r="O62" s="44"/>
-      <c r="P62" s="139"/>
-      <c r="Q62" s="139"/>
-      <c r="R62" s="139"/>
-      <c r="S62" s="139"/>
-      <c r="T62" s="139"/>
-      <c r="U62" s="139"/>
-      <c r="V62" s="139"/>
-      <c r="W62" s="139"/>
-      <c r="X62" s="139"/>
-      <c r="Y62" s="139"/>
-      <c r="Z62" s="139"/>
+      <c r="P62" s="101"/>
+      <c r="Q62" s="101"/>
+      <c r="R62" s="101"/>
+      <c r="S62" s="101"/>
+      <c r="T62" s="101"/>
+      <c r="U62" s="101"/>
+      <c r="V62" s="101"/>
+      <c r="W62" s="101"/>
+      <c r="X62" s="101"/>
+      <c r="Y62" s="101"/>
+      <c r="Z62" s="101"/>
       <c r="AA62" s="44"/>
       <c r="AB62" s="44"/>
       <c r="AC62" s="44"/>
@@ -7617,17 +7611,17 @@
       <c r="M63" s="47"/>
       <c r="N63" s="47"/>
       <c r="O63" s="47"/>
-      <c r="P63" s="140"/>
-      <c r="Q63" s="140"/>
-      <c r="R63" s="140"/>
-      <c r="S63" s="140"/>
-      <c r="T63" s="140"/>
-      <c r="U63" s="140"/>
-      <c r="V63" s="140"/>
-      <c r="W63" s="140"/>
-      <c r="X63" s="140"/>
-      <c r="Y63" s="140"/>
-      <c r="Z63" s="140"/>
+      <c r="P63" s="102"/>
+      <c r="Q63" s="102"/>
+      <c r="R63" s="102"/>
+      <c r="S63" s="102"/>
+      <c r="T63" s="102"/>
+      <c r="U63" s="102"/>
+      <c r="V63" s="102"/>
+      <c r="W63" s="102"/>
+      <c r="X63" s="102"/>
+      <c r="Y63" s="102"/>
+      <c r="Z63" s="102"/>
       <c r="AA63" s="47"/>
       <c r="AB63" s="47"/>
       <c r="AC63" s="47"/>
@@ -7659,17 +7653,17 @@
       <c r="M64" s="49"/>
       <c r="N64" s="49"/>
       <c r="O64" s="49"/>
-      <c r="P64" s="49"/>
-      <c r="Q64" s="49"/>
-      <c r="R64" s="49"/>
-      <c r="S64" s="49"/>
-      <c r="T64" s="50"/>
-      <c r="U64" s="49"/>
-      <c r="V64" s="49"/>
-      <c r="W64" s="49"/>
-      <c r="X64" s="49"/>
-      <c r="Y64" s="49"/>
-      <c r="Z64" s="49"/>
+      <c r="P64" s="157"/>
+      <c r="Q64" s="157"/>
+      <c r="R64" s="157"/>
+      <c r="S64" s="157"/>
+      <c r="T64" s="157"/>
+      <c r="U64" s="157"/>
+      <c r="V64" s="157"/>
+      <c r="W64" s="157"/>
+      <c r="X64" s="157"/>
+      <c r="Y64" s="157"/>
+      <c r="Z64" s="157"/>
       <c r="AA64" s="49"/>
       <c r="AB64" s="49"/>
       <c r="AC64" s="49"/>
@@ -7728,104 +7722,104 @@
       <c r="AN65" s="52"/>
     </row>
     <row r="66" spans="1:40" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="125" t="s">
+      <c r="A66" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="B66" s="126"/>
-      <c r="C66" s="126"/>
-      <c r="D66" s="126"/>
-      <c r="E66" s="126"/>
-      <c r="F66" s="126"/>
-      <c r="G66" s="126"/>
-      <c r="H66" s="126"/>
-      <c r="I66" s="126"/>
-      <c r="J66" s="126"/>
-      <c r="K66" s="126"/>
-      <c r="L66" s="126"/>
-      <c r="M66" s="126"/>
-      <c r="N66" s="126"/>
-      <c r="O66" s="126"/>
-      <c r="P66" s="126"/>
-      <c r="Q66" s="126"/>
-      <c r="R66" s="126"/>
-      <c r="S66" s="126"/>
-      <c r="T66" s="126"/>
-      <c r="U66" s="126"/>
-      <c r="V66" s="126"/>
-      <c r="W66" s="126"/>
-      <c r="X66" s="126"/>
-      <c r="Y66" s="126"/>
-      <c r="Z66" s="126"/>
-      <c r="AA66" s="126"/>
-      <c r="AB66" s="126"/>
-      <c r="AC66" s="126"/>
-      <c r="AD66" s="126"/>
-      <c r="AE66" s="126"/>
-      <c r="AF66" s="126"/>
-      <c r="AG66" s="126"/>
-      <c r="AH66" s="126"/>
-      <c r="AI66" s="126"/>
-      <c r="AJ66" s="126"/>
-      <c r="AK66" s="126"/>
-      <c r="AL66" s="126"/>
-      <c r="AM66" s="126"/>
-      <c r="AN66" s="127"/>
+      <c r="B66" s="69"/>
+      <c r="C66" s="69"/>
+      <c r="D66" s="69"/>
+      <c r="E66" s="69"/>
+      <c r="F66" s="69"/>
+      <c r="G66" s="69"/>
+      <c r="H66" s="69"/>
+      <c r="I66" s="69"/>
+      <c r="J66" s="69"/>
+      <c r="K66" s="69"/>
+      <c r="L66" s="69"/>
+      <c r="M66" s="69"/>
+      <c r="N66" s="69"/>
+      <c r="O66" s="69"/>
+      <c r="P66" s="69"/>
+      <c r="Q66" s="69"/>
+      <c r="R66" s="69"/>
+      <c r="S66" s="69"/>
+      <c r="T66" s="69"/>
+      <c r="U66" s="69"/>
+      <c r="V66" s="69"/>
+      <c r="W66" s="69"/>
+      <c r="X66" s="69"/>
+      <c r="Y66" s="69"/>
+      <c r="Z66" s="69"/>
+      <c r="AA66" s="69"/>
+      <c r="AB66" s="69"/>
+      <c r="AC66" s="69"/>
+      <c r="AD66" s="69"/>
+      <c r="AE66" s="69"/>
+      <c r="AF66" s="69"/>
+      <c r="AG66" s="69"/>
+      <c r="AH66" s="69"/>
+      <c r="AI66" s="69"/>
+      <c r="AJ66" s="69"/>
+      <c r="AK66" s="69"/>
+      <c r="AL66" s="69"/>
+      <c r="AM66" s="69"/>
+      <c r="AN66" s="70"/>
     </row>
     <row r="67" spans="1:40" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="128" t="s">
+      <c r="A67" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="B67" s="129"/>
-      <c r="C67" s="129"/>
-      <c r="D67" s="129"/>
-      <c r="E67" s="129"/>
-      <c r="F67" s="129"/>
-      <c r="G67" s="129"/>
-      <c r="H67" s="129"/>
-      <c r="I67" s="129"/>
-      <c r="J67" s="129"/>
-      <c r="K67" s="129"/>
-      <c r="L67" s="129"/>
-      <c r="M67" s="129"/>
-      <c r="N67" s="129"/>
-      <c r="O67" s="129"/>
-      <c r="P67" s="129"/>
-      <c r="Q67" s="129"/>
-      <c r="R67" s="129"/>
-      <c r="S67" s="129"/>
-      <c r="T67" s="129"/>
-      <c r="U67" s="129"/>
-      <c r="V67" s="129"/>
-      <c r="W67" s="129"/>
-      <c r="X67" s="129"/>
-      <c r="Y67" s="129"/>
-      <c r="Z67" s="129"/>
-      <c r="AA67" s="129"/>
-      <c r="AB67" s="129"/>
-      <c r="AC67" s="129"/>
-      <c r="AD67" s="129"/>
-      <c r="AE67" s="129"/>
-      <c r="AF67" s="129"/>
-      <c r="AG67" s="129"/>
-      <c r="AH67" s="129"/>
-      <c r="AI67" s="129"/>
-      <c r="AJ67" s="129"/>
-      <c r="AK67" s="129"/>
-      <c r="AL67" s="129"/>
-      <c r="AM67" s="129"/>
-      <c r="AN67" s="130"/>
+      <c r="B67" s="72"/>
+      <c r="C67" s="72"/>
+      <c r="D67" s="72"/>
+      <c r="E67" s="72"/>
+      <c r="F67" s="72"/>
+      <c r="G67" s="72"/>
+      <c r="H67" s="72"/>
+      <c r="I67" s="72"/>
+      <c r="J67" s="72"/>
+      <c r="K67" s="72"/>
+      <c r="L67" s="72"/>
+      <c r="M67" s="72"/>
+      <c r="N67" s="72"/>
+      <c r="O67" s="72"/>
+      <c r="P67" s="72"/>
+      <c r="Q67" s="72"/>
+      <c r="R67" s="72"/>
+      <c r="S67" s="72"/>
+      <c r="T67" s="72"/>
+      <c r="U67" s="72"/>
+      <c r="V67" s="72"/>
+      <c r="W67" s="72"/>
+      <c r="X67" s="72"/>
+      <c r="Y67" s="72"/>
+      <c r="Z67" s="72"/>
+      <c r="AA67" s="72"/>
+      <c r="AB67" s="72"/>
+      <c r="AC67" s="72"/>
+      <c r="AD67" s="72"/>
+      <c r="AE67" s="72"/>
+      <c r="AF67" s="72"/>
+      <c r="AG67" s="72"/>
+      <c r="AH67" s="72"/>
+      <c r="AI67" s="72"/>
+      <c r="AJ67" s="72"/>
+      <c r="AK67" s="72"/>
+      <c r="AL67" s="72"/>
+      <c r="AM67" s="72"/>
+      <c r="AN67" s="73"/>
     </row>
     <row r="68" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="131" t="s">
+      <c r="A68" s="74" t="s">
         <v>33</v>
       </c>
-      <c r="B68" s="132"/>
-      <c r="C68" s="132"/>
-      <c r="D68" s="132"/>
-      <c r="E68" s="132"/>
-      <c r="F68" s="132"/>
-      <c r="G68" s="132"/>
-      <c r="H68" s="132"/>
+      <c r="B68" s="75"/>
+      <c r="C68" s="75"/>
+      <c r="D68" s="75"/>
+      <c r="E68" s="75"/>
+      <c r="F68" s="75"/>
+      <c r="G68" s="75"/>
+      <c r="H68" s="75"/>
       <c r="I68" s="25"/>
       <c r="J68" s="25"/>
       <c r="K68" s="25"/>
@@ -7835,12 +7829,12 @@
       <c r="O68" s="25"/>
       <c r="P68" s="25"/>
       <c r="Q68" s="39"/>
-      <c r="R68" s="133" t="s">
+      <c r="R68" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="S68" s="133"/>
-      <c r="T68" s="133"/>
-      <c r="U68" s="133"/>
+      <c r="S68" s="76"/>
+      <c r="T68" s="76"/>
+      <c r="U68" s="76"/>
       <c r="V68" s="25"/>
       <c r="W68" s="25"/>
       <c r="X68" s="25"/>
@@ -7848,13 +7842,13 @@
       <c r="Z68" s="25"/>
       <c r="AA68" s="25"/>
       <c r="AB68" s="25"/>
-      <c r="AC68" s="135" t="s">
+      <c r="AC68" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="AD68" s="135"/>
-      <c r="AE68" s="135"/>
-      <c r="AF68" s="135"/>
-      <c r="AG68" s="135"/>
+      <c r="AD68" s="78"/>
+      <c r="AE68" s="78"/>
+      <c r="AF68" s="78"/>
+      <c r="AG68" s="78"/>
       <c r="AH68" s="25"/>
       <c r="AI68" s="25"/>
       <c r="AJ68" s="25"/>
@@ -7864,16 +7858,16 @@
       <c r="AN68" s="26"/>
     </row>
     <row r="69" spans="1:40" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="136" t="s">
+      <c r="A69" s="89" t="s">
         <v>34</v>
       </c>
-      <c r="B69" s="137"/>
-      <c r="C69" s="137"/>
-      <c r="D69" s="137"/>
-      <c r="E69" s="137"/>
-      <c r="F69" s="137"/>
-      <c r="G69" s="137"/>
-      <c r="H69" s="137"/>
+      <c r="B69" s="90"/>
+      <c r="C69" s="90"/>
+      <c r="D69" s="90"/>
+      <c r="E69" s="90"/>
+      <c r="F69" s="90"/>
+      <c r="G69" s="90"/>
+      <c r="H69" s="90"/>
       <c r="I69" s="14"/>
       <c r="J69" s="14"/>
       <c r="K69" s="14"/>
@@ -7883,10 +7877,10 @@
       <c r="O69" s="14"/>
       <c r="P69" s="14"/>
       <c r="Q69" s="14"/>
-      <c r="R69" s="134"/>
-      <c r="S69" s="134"/>
-      <c r="T69" s="134"/>
-      <c r="U69" s="134"/>
+      <c r="R69" s="88"/>
+      <c r="S69" s="88"/>
+      <c r="T69" s="88"/>
+      <c r="U69" s="88"/>
       <c r="V69" s="14"/>
       <c r="W69" s="14"/>
       <c r="X69" s="14"/>
@@ -7894,13 +7888,13 @@
       <c r="Z69" s="14"/>
       <c r="AA69" s="14"/>
       <c r="AB69" s="14"/>
-      <c r="AC69" s="138" t="s">
+      <c r="AC69" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="AD69" s="138"/>
-      <c r="AE69" s="138"/>
-      <c r="AF69" s="138"/>
-      <c r="AG69" s="138"/>
+      <c r="AD69" s="91"/>
+      <c r="AE69" s="91"/>
+      <c r="AF69" s="91"/>
+      <c r="AG69" s="91"/>
       <c r="AH69" s="14"/>
       <c r="AI69" s="14"/>
       <c r="AJ69" s="14"/>
@@ -7954,230 +7948,230 @@
       <c r="AN70" s="58"/>
     </row>
     <row r="71" spans="1:40" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="141"/>
-      <c r="B71" s="142"/>
-      <c r="C71" s="142"/>
-      <c r="D71" s="142"/>
-      <c r="E71" s="142"/>
-      <c r="F71" s="142"/>
-      <c r="G71" s="142"/>
-      <c r="H71" s="142"/>
-      <c r="I71" s="142"/>
-      <c r="J71" s="142"/>
-      <c r="K71" s="142"/>
-      <c r="L71" s="142"/>
-      <c r="M71" s="142"/>
-      <c r="N71" s="142"/>
-      <c r="O71" s="142"/>
-      <c r="P71" s="142"/>
-      <c r="Q71" s="142"/>
-      <c r="R71" s="142"/>
-      <c r="S71" s="142"/>
-      <c r="T71" s="142"/>
-      <c r="U71" s="142"/>
-      <c r="V71" s="142"/>
-      <c r="W71" s="142"/>
-      <c r="X71" s="142"/>
-      <c r="Y71" s="142"/>
-      <c r="Z71" s="142"/>
-      <c r="AA71" s="142"/>
-      <c r="AB71" s="142"/>
-      <c r="AC71" s="142"/>
-      <c r="AD71" s="142"/>
-      <c r="AE71" s="142"/>
-      <c r="AF71" s="142"/>
-      <c r="AG71" s="142"/>
-      <c r="AH71" s="142"/>
-      <c r="AI71" s="142"/>
-      <c r="AJ71" s="142"/>
-      <c r="AK71" s="142"/>
-      <c r="AL71" s="142"/>
-      <c r="AM71" s="142"/>
-      <c r="AN71" s="143"/>
+      <c r="A71" s="59"/>
+      <c r="B71" s="60"/>
+      <c r="C71" s="60"/>
+      <c r="D71" s="60"/>
+      <c r="E71" s="60"/>
+      <c r="F71" s="60"/>
+      <c r="G71" s="60"/>
+      <c r="H71" s="60"/>
+      <c r="I71" s="60"/>
+      <c r="J71" s="60"/>
+      <c r="K71" s="60"/>
+      <c r="L71" s="60"/>
+      <c r="M71" s="60"/>
+      <c r="N71" s="60"/>
+      <c r="O71" s="60"/>
+      <c r="P71" s="60"/>
+      <c r="Q71" s="60"/>
+      <c r="R71" s="60"/>
+      <c r="S71" s="60"/>
+      <c r="T71" s="60"/>
+      <c r="U71" s="60"/>
+      <c r="V71" s="60"/>
+      <c r="W71" s="60"/>
+      <c r="X71" s="60"/>
+      <c r="Y71" s="60"/>
+      <c r="Z71" s="60"/>
+      <c r="AA71" s="60"/>
+      <c r="AB71" s="60"/>
+      <c r="AC71" s="60"/>
+      <c r="AD71" s="60"/>
+      <c r="AE71" s="60"/>
+      <c r="AF71" s="60"/>
+      <c r="AG71" s="60"/>
+      <c r="AH71" s="60"/>
+      <c r="AI71" s="60"/>
+      <c r="AJ71" s="60"/>
+      <c r="AK71" s="60"/>
+      <c r="AL71" s="60"/>
+      <c r="AM71" s="60"/>
+      <c r="AN71" s="61"/>
     </row>
     <row r="72" spans="1:40" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="144"/>
-      <c r="B72" s="145"/>
-      <c r="C72" s="145"/>
-      <c r="D72" s="145"/>
-      <c r="E72" s="145"/>
-      <c r="F72" s="145"/>
-      <c r="G72" s="145"/>
-      <c r="H72" s="145"/>
-      <c r="I72" s="145"/>
-      <c r="J72" s="145"/>
-      <c r="K72" s="145"/>
-      <c r="L72" s="145"/>
-      <c r="M72" s="145"/>
-      <c r="N72" s="145"/>
-      <c r="O72" s="145"/>
-      <c r="P72" s="145"/>
-      <c r="Q72" s="145"/>
-      <c r="R72" s="145"/>
-      <c r="S72" s="145"/>
-      <c r="T72" s="145"/>
-      <c r="U72" s="145"/>
-      <c r="V72" s="145"/>
-      <c r="W72" s="145"/>
-      <c r="X72" s="145"/>
-      <c r="Y72" s="145"/>
-      <c r="Z72" s="145"/>
-      <c r="AA72" s="145"/>
-      <c r="AB72" s="145"/>
-      <c r="AC72" s="145"/>
-      <c r="AD72" s="145"/>
-      <c r="AE72" s="145"/>
-      <c r="AF72" s="145"/>
-      <c r="AG72" s="145"/>
-      <c r="AH72" s="145"/>
-      <c r="AI72" s="145"/>
-      <c r="AJ72" s="145"/>
-      <c r="AK72" s="145"/>
-      <c r="AL72" s="145"/>
-      <c r="AM72" s="145"/>
-      <c r="AN72" s="146"/>
+      <c r="A72" s="62"/>
+      <c r="B72" s="63"/>
+      <c r="C72" s="63"/>
+      <c r="D72" s="63"/>
+      <c r="E72" s="63"/>
+      <c r="F72" s="63"/>
+      <c r="G72" s="63"/>
+      <c r="H72" s="63"/>
+      <c r="I72" s="63"/>
+      <c r="J72" s="63"/>
+      <c r="K72" s="63"/>
+      <c r="L72" s="63"/>
+      <c r="M72" s="63"/>
+      <c r="N72" s="63"/>
+      <c r="O72" s="63"/>
+      <c r="P72" s="63"/>
+      <c r="Q72" s="63"/>
+      <c r="R72" s="63"/>
+      <c r="S72" s="63"/>
+      <c r="T72" s="63"/>
+      <c r="U72" s="63"/>
+      <c r="V72" s="63"/>
+      <c r="W72" s="63"/>
+      <c r="X72" s="63"/>
+      <c r="Y72" s="63"/>
+      <c r="Z72" s="63"/>
+      <c r="AA72" s="63"/>
+      <c r="AB72" s="63"/>
+      <c r="AC72" s="63"/>
+      <c r="AD72" s="63"/>
+      <c r="AE72" s="63"/>
+      <c r="AF72" s="63"/>
+      <c r="AG72" s="63"/>
+      <c r="AH72" s="63"/>
+      <c r="AI72" s="63"/>
+      <c r="AJ72" s="63"/>
+      <c r="AK72" s="63"/>
+      <c r="AL72" s="63"/>
+      <c r="AM72" s="63"/>
+      <c r="AN72" s="64"/>
     </row>
     <row r="73" spans="1:40" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="147"/>
-      <c r="B73" s="148"/>
-      <c r="C73" s="148"/>
-      <c r="D73" s="148"/>
-      <c r="E73" s="148"/>
-      <c r="F73" s="148"/>
-      <c r="G73" s="148"/>
-      <c r="H73" s="148"/>
-      <c r="I73" s="148"/>
-      <c r="J73" s="148"/>
-      <c r="K73" s="148"/>
-      <c r="L73" s="148"/>
-      <c r="M73" s="148"/>
-      <c r="N73" s="148"/>
-      <c r="O73" s="148"/>
-      <c r="P73" s="148"/>
-      <c r="Q73" s="148"/>
-      <c r="R73" s="148"/>
-      <c r="S73" s="148"/>
-      <c r="T73" s="148"/>
-      <c r="U73" s="148"/>
-      <c r="V73" s="148"/>
-      <c r="W73" s="148"/>
-      <c r="X73" s="148"/>
-      <c r="Y73" s="148"/>
-      <c r="Z73" s="148"/>
-      <c r="AA73" s="148"/>
-      <c r="AB73" s="148"/>
-      <c r="AC73" s="148"/>
-      <c r="AD73" s="148"/>
-      <c r="AE73" s="148"/>
-      <c r="AF73" s="148"/>
-      <c r="AG73" s="148"/>
-      <c r="AH73" s="148"/>
-      <c r="AI73" s="148"/>
-      <c r="AJ73" s="148"/>
-      <c r="AK73" s="148"/>
-      <c r="AL73" s="148"/>
-      <c r="AM73" s="148"/>
-      <c r="AN73" s="149"/>
+      <c r="A73" s="65"/>
+      <c r="B73" s="66"/>
+      <c r="C73" s="66"/>
+      <c r="D73" s="66"/>
+      <c r="E73" s="66"/>
+      <c r="F73" s="66"/>
+      <c r="G73" s="66"/>
+      <c r="H73" s="66"/>
+      <c r="I73" s="66"/>
+      <c r="J73" s="66"/>
+      <c r="K73" s="66"/>
+      <c r="L73" s="66"/>
+      <c r="M73" s="66"/>
+      <c r="N73" s="66"/>
+      <c r="O73" s="66"/>
+      <c r="P73" s="66"/>
+      <c r="Q73" s="66"/>
+      <c r="R73" s="66"/>
+      <c r="S73" s="66"/>
+      <c r="T73" s="66"/>
+      <c r="U73" s="66"/>
+      <c r="V73" s="66"/>
+      <c r="W73" s="66"/>
+      <c r="X73" s="66"/>
+      <c r="Y73" s="66"/>
+      <c r="Z73" s="66"/>
+      <c r="AA73" s="66"/>
+      <c r="AB73" s="66"/>
+      <c r="AC73" s="66"/>
+      <c r="AD73" s="66"/>
+      <c r="AE73" s="66"/>
+      <c r="AF73" s="66"/>
+      <c r="AG73" s="66"/>
+      <c r="AH73" s="66"/>
+      <c r="AI73" s="66"/>
+      <c r="AJ73" s="66"/>
+      <c r="AK73" s="66"/>
+      <c r="AL73" s="66"/>
+      <c r="AM73" s="66"/>
+      <c r="AN73" s="67"/>
     </row>
     <row r="74" spans="1:40" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="125" t="s">
+      <c r="A74" s="68" t="s">
         <v>36</v>
       </c>
-      <c r="B74" s="126"/>
-      <c r="C74" s="126"/>
-      <c r="D74" s="126"/>
-      <c r="E74" s="126"/>
-      <c r="F74" s="126"/>
-      <c r="G74" s="126"/>
-      <c r="H74" s="126"/>
-      <c r="I74" s="126"/>
-      <c r="J74" s="126"/>
-      <c r="K74" s="126"/>
-      <c r="L74" s="126"/>
-      <c r="M74" s="126"/>
-      <c r="N74" s="126"/>
-      <c r="O74" s="126"/>
-      <c r="P74" s="126"/>
-      <c r="Q74" s="126"/>
-      <c r="R74" s="126"/>
-      <c r="S74" s="126"/>
-      <c r="T74" s="126"/>
-      <c r="U74" s="126"/>
-      <c r="V74" s="126"/>
-      <c r="W74" s="126"/>
-      <c r="X74" s="126"/>
-      <c r="Y74" s="126"/>
-      <c r="Z74" s="126"/>
-      <c r="AA74" s="126"/>
-      <c r="AB74" s="126"/>
-      <c r="AC74" s="126"/>
-      <c r="AD74" s="126"/>
-      <c r="AE74" s="126"/>
-      <c r="AF74" s="126"/>
-      <c r="AG74" s="126"/>
-      <c r="AH74" s="126"/>
-      <c r="AI74" s="126"/>
-      <c r="AJ74" s="126"/>
-      <c r="AK74" s="126"/>
-      <c r="AL74" s="126"/>
-      <c r="AM74" s="126"/>
-      <c r="AN74" s="127"/>
+      <c r="B74" s="69"/>
+      <c r="C74" s="69"/>
+      <c r="D74" s="69"/>
+      <c r="E74" s="69"/>
+      <c r="F74" s="69"/>
+      <c r="G74" s="69"/>
+      <c r="H74" s="69"/>
+      <c r="I74" s="69"/>
+      <c r="J74" s="69"/>
+      <c r="K74" s="69"/>
+      <c r="L74" s="69"/>
+      <c r="M74" s="69"/>
+      <c r="N74" s="69"/>
+      <c r="O74" s="69"/>
+      <c r="P74" s="69"/>
+      <c r="Q74" s="69"/>
+      <c r="R74" s="69"/>
+      <c r="S74" s="69"/>
+      <c r="T74" s="69"/>
+      <c r="U74" s="69"/>
+      <c r="V74" s="69"/>
+      <c r="W74" s="69"/>
+      <c r="X74" s="69"/>
+      <c r="Y74" s="69"/>
+      <c r="Z74" s="69"/>
+      <c r="AA74" s="69"/>
+      <c r="AB74" s="69"/>
+      <c r="AC74" s="69"/>
+      <c r="AD74" s="69"/>
+      <c r="AE74" s="69"/>
+      <c r="AF74" s="69"/>
+      <c r="AG74" s="69"/>
+      <c r="AH74" s="69"/>
+      <c r="AI74" s="69"/>
+      <c r="AJ74" s="69"/>
+      <c r="AK74" s="69"/>
+      <c r="AL74" s="69"/>
+      <c r="AM74" s="69"/>
+      <c r="AN74" s="70"/>
     </row>
     <row r="75" spans="1:40" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="128" t="s">
+      <c r="A75" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="B75" s="129"/>
-      <c r="C75" s="129"/>
-      <c r="D75" s="129"/>
-      <c r="E75" s="129"/>
-      <c r="F75" s="129"/>
-      <c r="G75" s="129"/>
-      <c r="H75" s="129"/>
-      <c r="I75" s="129"/>
-      <c r="J75" s="129"/>
-      <c r="K75" s="129"/>
-      <c r="L75" s="129"/>
-      <c r="M75" s="129"/>
-      <c r="N75" s="129"/>
-      <c r="O75" s="129"/>
-      <c r="P75" s="129"/>
-      <c r="Q75" s="129"/>
-      <c r="R75" s="129"/>
-      <c r="S75" s="129"/>
-      <c r="T75" s="129"/>
-      <c r="U75" s="129"/>
-      <c r="V75" s="129"/>
-      <c r="W75" s="129"/>
-      <c r="X75" s="129"/>
-      <c r="Y75" s="129"/>
-      <c r="Z75" s="129"/>
-      <c r="AA75" s="129"/>
-      <c r="AB75" s="129"/>
-      <c r="AC75" s="129"/>
-      <c r="AD75" s="129"/>
-      <c r="AE75" s="129"/>
-      <c r="AF75" s="129"/>
-      <c r="AG75" s="129"/>
-      <c r="AH75" s="129"/>
-      <c r="AI75" s="129"/>
-      <c r="AJ75" s="129"/>
-      <c r="AK75" s="129"/>
-      <c r="AL75" s="129"/>
-      <c r="AM75" s="129"/>
-      <c r="AN75" s="130"/>
+      <c r="B75" s="72"/>
+      <c r="C75" s="72"/>
+      <c r="D75" s="72"/>
+      <c r="E75" s="72"/>
+      <c r="F75" s="72"/>
+      <c r="G75" s="72"/>
+      <c r="H75" s="72"/>
+      <c r="I75" s="72"/>
+      <c r="J75" s="72"/>
+      <c r="K75" s="72"/>
+      <c r="L75" s="72"/>
+      <c r="M75" s="72"/>
+      <c r="N75" s="72"/>
+      <c r="O75" s="72"/>
+      <c r="P75" s="72"/>
+      <c r="Q75" s="72"/>
+      <c r="R75" s="72"/>
+      <c r="S75" s="72"/>
+      <c r="T75" s="72"/>
+      <c r="U75" s="72"/>
+      <c r="V75" s="72"/>
+      <c r="W75" s="72"/>
+      <c r="X75" s="72"/>
+      <c r="Y75" s="72"/>
+      <c r="Z75" s="72"/>
+      <c r="AA75" s="72"/>
+      <c r="AB75" s="72"/>
+      <c r="AC75" s="72"/>
+      <c r="AD75" s="72"/>
+      <c r="AE75" s="72"/>
+      <c r="AF75" s="72"/>
+      <c r="AG75" s="72"/>
+      <c r="AH75" s="72"/>
+      <c r="AI75" s="72"/>
+      <c r="AJ75" s="72"/>
+      <c r="AK75" s="72"/>
+      <c r="AL75" s="72"/>
+      <c r="AM75" s="72"/>
+      <c r="AN75" s="73"/>
     </row>
     <row r="76" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="131" t="s">
+      <c r="A76" s="74" t="s">
         <v>33</v>
       </c>
-      <c r="B76" s="132"/>
-      <c r="C76" s="132"/>
-      <c r="D76" s="132"/>
-      <c r="E76" s="132"/>
-      <c r="F76" s="132"/>
-      <c r="G76" s="132"/>
-      <c r="H76" s="132"/>
+      <c r="B76" s="75"/>
+      <c r="C76" s="75"/>
+      <c r="D76" s="75"/>
+      <c r="E76" s="75"/>
+      <c r="F76" s="75"/>
+      <c r="G76" s="75"/>
+      <c r="H76" s="75"/>
       <c r="I76" s="25"/>
       <c r="J76" s="25"/>
       <c r="K76" s="25"/>
@@ -8187,12 +8181,12 @@
       <c r="O76" s="25"/>
       <c r="P76" s="25"/>
       <c r="Q76" s="39"/>
-      <c r="R76" s="133" t="s">
+      <c r="R76" s="76" t="s">
         <v>35</v>
       </c>
-      <c r="S76" s="133"/>
-      <c r="T76" s="133"/>
-      <c r="U76" s="133"/>
+      <c r="S76" s="76"/>
+      <c r="T76" s="76"/>
+      <c r="U76" s="76"/>
       <c r="V76" s="25"/>
       <c r="W76" s="25"/>
       <c r="X76" s="25"/>
@@ -8200,13 +8194,13 @@
       <c r="Z76" s="25"/>
       <c r="AA76" s="25"/>
       <c r="AB76" s="25"/>
-      <c r="AC76" s="135" t="s">
+      <c r="AC76" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="AD76" s="135"/>
-      <c r="AE76" s="135"/>
-      <c r="AF76" s="135"/>
-      <c r="AG76" s="135"/>
+      <c r="AD76" s="78"/>
+      <c r="AE76" s="78"/>
+      <c r="AF76" s="78"/>
+      <c r="AG76" s="78"/>
       <c r="AH76" s="25"/>
       <c r="AI76" s="25"/>
       <c r="AJ76" s="25"/>
@@ -8216,16 +8210,16 @@
       <c r="AN76" s="26"/>
     </row>
     <row r="77" spans="1:40" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="151" t="s">
+      <c r="A77" s="79" t="s">
         <v>34</v>
       </c>
-      <c r="B77" s="152"/>
-      <c r="C77" s="152"/>
-      <c r="D77" s="152"/>
-      <c r="E77" s="152"/>
-      <c r="F77" s="152"/>
-      <c r="G77" s="152"/>
-      <c r="H77" s="152"/>
+      <c r="B77" s="80"/>
+      <c r="C77" s="80"/>
+      <c r="D77" s="80"/>
+      <c r="E77" s="80"/>
+      <c r="F77" s="80"/>
+      <c r="G77" s="80"/>
+      <c r="H77" s="80"/>
       <c r="I77" s="28"/>
       <c r="J77" s="28"/>
       <c r="K77" s="28"/>
@@ -8235,10 +8229,10 @@
       <c r="O77" s="28"/>
       <c r="P77" s="28"/>
       <c r="Q77" s="28"/>
-      <c r="R77" s="150"/>
-      <c r="S77" s="150"/>
-      <c r="T77" s="150"/>
-      <c r="U77" s="150"/>
+      <c r="R77" s="77"/>
+      <c r="S77" s="77"/>
+      <c r="T77" s="77"/>
+      <c r="U77" s="77"/>
       <c r="V77" s="28"/>
       <c r="W77" s="28"/>
       <c r="X77" s="28"/>
@@ -8246,13 +8240,13 @@
       <c r="Z77" s="28"/>
       <c r="AA77" s="28"/>
       <c r="AB77" s="28"/>
-      <c r="AC77" s="153" t="s">
+      <c r="AC77" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="AD77" s="153"/>
-      <c r="AE77" s="153"/>
-      <c r="AF77" s="153"/>
-      <c r="AG77" s="153"/>
+      <c r="AD77" s="81"/>
+      <c r="AE77" s="81"/>
+      <c r="AF77" s="81"/>
+      <c r="AG77" s="81"/>
       <c r="AH77" s="28"/>
       <c r="AI77" s="28"/>
       <c r="AJ77" s="28"/>
@@ -8347,16 +8341,173 @@
       <c r="AN79" s="40"/>
     </row>
   </sheetData>
-  <mergeCells count="191">
-    <mergeCell ref="A70:AN70"/>
-    <mergeCell ref="A71:AN73"/>
-    <mergeCell ref="A74:AN74"/>
-    <mergeCell ref="A75:AN75"/>
-    <mergeCell ref="A76:H76"/>
-    <mergeCell ref="R76:U77"/>
-    <mergeCell ref="AC76:AG76"/>
-    <mergeCell ref="A77:H77"/>
-    <mergeCell ref="AC77:AG77"/>
+  <mergeCells count="192">
+    <mergeCell ref="A13:AN13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:M15"/>
+    <mergeCell ref="A25:AN25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:M27"/>
+    <mergeCell ref="A2:AN2"/>
+    <mergeCell ref="A3:AN3"/>
+    <mergeCell ref="A4:AN4"/>
+    <mergeCell ref="L5:AB9"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:E12"/>
+    <mergeCell ref="H11:I12"/>
+    <mergeCell ref="R11:U12"/>
+    <mergeCell ref="Y11:AA12"/>
+    <mergeCell ref="AI11:AN12"/>
+    <mergeCell ref="A34:AN34"/>
+    <mergeCell ref="A35:K37"/>
+    <mergeCell ref="L35:N37"/>
+    <mergeCell ref="O35:AH35"/>
+    <mergeCell ref="AI35:AN37"/>
+    <mergeCell ref="O36:S37"/>
+    <mergeCell ref="T36:X37"/>
+    <mergeCell ref="Y36:AC37"/>
+    <mergeCell ref="AD36:AH37"/>
+    <mergeCell ref="AI38:AN38"/>
+    <mergeCell ref="A39:K39"/>
+    <mergeCell ref="L39:N39"/>
+    <mergeCell ref="O39:S39"/>
+    <mergeCell ref="T39:X39"/>
+    <mergeCell ref="Y39:AC39"/>
+    <mergeCell ref="AD39:AH39"/>
+    <mergeCell ref="AI39:AN39"/>
+    <mergeCell ref="A38:K38"/>
+    <mergeCell ref="L38:N38"/>
+    <mergeCell ref="O38:S38"/>
+    <mergeCell ref="T38:X38"/>
+    <mergeCell ref="Y38:AC38"/>
+    <mergeCell ref="AD38:AH38"/>
+    <mergeCell ref="AI40:AN40"/>
+    <mergeCell ref="A41:K41"/>
+    <mergeCell ref="L41:N41"/>
+    <mergeCell ref="O41:S41"/>
+    <mergeCell ref="T41:X41"/>
+    <mergeCell ref="Y41:AC41"/>
+    <mergeCell ref="AD41:AH41"/>
+    <mergeCell ref="AI41:AN41"/>
+    <mergeCell ref="A40:K40"/>
+    <mergeCell ref="L40:N40"/>
+    <mergeCell ref="O40:S40"/>
+    <mergeCell ref="T40:X40"/>
+    <mergeCell ref="Y40:AC40"/>
+    <mergeCell ref="AD40:AH40"/>
+    <mergeCell ref="AI42:AN42"/>
+    <mergeCell ref="A43:K43"/>
+    <mergeCell ref="L43:N43"/>
+    <mergeCell ref="O43:S43"/>
+    <mergeCell ref="T43:X43"/>
+    <mergeCell ref="Y43:AC43"/>
+    <mergeCell ref="AD43:AH43"/>
+    <mergeCell ref="AI43:AN43"/>
+    <mergeCell ref="A42:K42"/>
+    <mergeCell ref="L42:N42"/>
+    <mergeCell ref="O42:S42"/>
+    <mergeCell ref="T42:X42"/>
+    <mergeCell ref="Y42:AC42"/>
+    <mergeCell ref="AD42:AH42"/>
+    <mergeCell ref="AI44:AN44"/>
+    <mergeCell ref="A45:K45"/>
+    <mergeCell ref="L45:N45"/>
+    <mergeCell ref="O45:S45"/>
+    <mergeCell ref="T45:X45"/>
+    <mergeCell ref="Y45:AC45"/>
+    <mergeCell ref="AD45:AH45"/>
+    <mergeCell ref="AI45:AN45"/>
+    <mergeCell ref="A44:K44"/>
+    <mergeCell ref="L44:N44"/>
+    <mergeCell ref="O44:S44"/>
+    <mergeCell ref="T44:X44"/>
+    <mergeCell ref="Y44:AC44"/>
+    <mergeCell ref="AD44:AH44"/>
+    <mergeCell ref="AI46:AN46"/>
+    <mergeCell ref="A47:K47"/>
+    <mergeCell ref="L47:N47"/>
+    <mergeCell ref="O47:S47"/>
+    <mergeCell ref="T47:X47"/>
+    <mergeCell ref="Y47:AC47"/>
+    <mergeCell ref="AD47:AH47"/>
+    <mergeCell ref="AI47:AN47"/>
+    <mergeCell ref="A46:K46"/>
+    <mergeCell ref="L46:N46"/>
+    <mergeCell ref="O46:S46"/>
+    <mergeCell ref="T46:X46"/>
+    <mergeCell ref="Y46:AC46"/>
+    <mergeCell ref="AD46:AH46"/>
+    <mergeCell ref="AI48:AN48"/>
+    <mergeCell ref="A49:K50"/>
+    <mergeCell ref="A51:K51"/>
+    <mergeCell ref="L51:N51"/>
+    <mergeCell ref="O51:S51"/>
+    <mergeCell ref="T51:X51"/>
+    <mergeCell ref="Y51:AC51"/>
+    <mergeCell ref="AD51:AH51"/>
+    <mergeCell ref="AI51:AN51"/>
+    <mergeCell ref="A48:K48"/>
+    <mergeCell ref="L48:N48"/>
+    <mergeCell ref="O48:S48"/>
+    <mergeCell ref="T48:X48"/>
+    <mergeCell ref="Y48:AC48"/>
+    <mergeCell ref="AD48:AH48"/>
+    <mergeCell ref="AI52:AN52"/>
+    <mergeCell ref="A53:K53"/>
+    <mergeCell ref="L53:N53"/>
+    <mergeCell ref="O53:S53"/>
+    <mergeCell ref="T53:X53"/>
+    <mergeCell ref="Y53:AC53"/>
+    <mergeCell ref="AD53:AH53"/>
+    <mergeCell ref="AI53:AN53"/>
+    <mergeCell ref="A52:K52"/>
+    <mergeCell ref="L52:N52"/>
+    <mergeCell ref="O52:S52"/>
+    <mergeCell ref="T52:X52"/>
+    <mergeCell ref="Y52:AC52"/>
+    <mergeCell ref="AD52:AH52"/>
+    <mergeCell ref="AI54:AN54"/>
+    <mergeCell ref="A55:K55"/>
+    <mergeCell ref="L55:N55"/>
+    <mergeCell ref="O55:S55"/>
+    <mergeCell ref="T55:X55"/>
+    <mergeCell ref="Y55:AC55"/>
+    <mergeCell ref="AD55:AH55"/>
+    <mergeCell ref="AI55:AN55"/>
+    <mergeCell ref="A54:K54"/>
+    <mergeCell ref="L54:N54"/>
+    <mergeCell ref="O54:S54"/>
+    <mergeCell ref="T54:X54"/>
+    <mergeCell ref="Y54:AC54"/>
+    <mergeCell ref="AD54:AH54"/>
+    <mergeCell ref="AI56:AN56"/>
+    <mergeCell ref="A57:K57"/>
+    <mergeCell ref="L57:N57"/>
+    <mergeCell ref="O57:S57"/>
+    <mergeCell ref="T57:X57"/>
+    <mergeCell ref="Y57:AC57"/>
+    <mergeCell ref="AD57:AH57"/>
+    <mergeCell ref="AI57:AN57"/>
+    <mergeCell ref="A56:K56"/>
+    <mergeCell ref="L56:N56"/>
+    <mergeCell ref="O56:S56"/>
+    <mergeCell ref="T56:X56"/>
+    <mergeCell ref="Y56:AC56"/>
+    <mergeCell ref="AD56:AH56"/>
+    <mergeCell ref="AI58:AN58"/>
+    <mergeCell ref="A59:K59"/>
+    <mergeCell ref="L59:N59"/>
+    <mergeCell ref="O59:S59"/>
+    <mergeCell ref="T59:X59"/>
+    <mergeCell ref="Y59:AC59"/>
+    <mergeCell ref="AD59:AH59"/>
+    <mergeCell ref="AI59:AN59"/>
+    <mergeCell ref="A58:K58"/>
+    <mergeCell ref="L58:N58"/>
+    <mergeCell ref="O58:S58"/>
+    <mergeCell ref="T58:X58"/>
+    <mergeCell ref="Y58:AC58"/>
+    <mergeCell ref="AD58:AH58"/>
     <mergeCell ref="AI60:AN60"/>
     <mergeCell ref="A61:AN61"/>
     <mergeCell ref="A66:AN66"/>
@@ -8373,172 +8524,16 @@
     <mergeCell ref="Y60:AC60"/>
     <mergeCell ref="AD60:AH60"/>
     <mergeCell ref="P62:Z63"/>
-    <mergeCell ref="AI58:AN58"/>
-    <mergeCell ref="A59:K59"/>
-    <mergeCell ref="L59:N59"/>
-    <mergeCell ref="O59:S59"/>
-    <mergeCell ref="T59:X59"/>
-    <mergeCell ref="Y59:AC59"/>
-    <mergeCell ref="AD59:AH59"/>
-    <mergeCell ref="AI59:AN59"/>
-    <mergeCell ref="A58:K58"/>
-    <mergeCell ref="L58:N58"/>
-    <mergeCell ref="O58:S58"/>
-    <mergeCell ref="T58:X58"/>
-    <mergeCell ref="Y58:AC58"/>
-    <mergeCell ref="AD58:AH58"/>
-    <mergeCell ref="AI56:AN56"/>
-    <mergeCell ref="A57:K57"/>
-    <mergeCell ref="L57:N57"/>
-    <mergeCell ref="O57:S57"/>
-    <mergeCell ref="T57:X57"/>
-    <mergeCell ref="Y57:AC57"/>
-    <mergeCell ref="AD57:AH57"/>
-    <mergeCell ref="AI57:AN57"/>
-    <mergeCell ref="A56:K56"/>
-    <mergeCell ref="L56:N56"/>
-    <mergeCell ref="O56:S56"/>
-    <mergeCell ref="T56:X56"/>
-    <mergeCell ref="Y56:AC56"/>
-    <mergeCell ref="AD56:AH56"/>
-    <mergeCell ref="AI54:AN54"/>
-    <mergeCell ref="A55:K55"/>
-    <mergeCell ref="L55:N55"/>
-    <mergeCell ref="O55:S55"/>
-    <mergeCell ref="T55:X55"/>
-    <mergeCell ref="Y55:AC55"/>
-    <mergeCell ref="AD55:AH55"/>
-    <mergeCell ref="AI55:AN55"/>
-    <mergeCell ref="A54:K54"/>
-    <mergeCell ref="L54:N54"/>
-    <mergeCell ref="O54:S54"/>
-    <mergeCell ref="T54:X54"/>
-    <mergeCell ref="Y54:AC54"/>
-    <mergeCell ref="AD54:AH54"/>
-    <mergeCell ref="AI52:AN52"/>
-    <mergeCell ref="A53:K53"/>
-    <mergeCell ref="L53:N53"/>
-    <mergeCell ref="O53:S53"/>
-    <mergeCell ref="T53:X53"/>
-    <mergeCell ref="Y53:AC53"/>
-    <mergeCell ref="AD53:AH53"/>
-    <mergeCell ref="AI53:AN53"/>
-    <mergeCell ref="A52:K52"/>
-    <mergeCell ref="L52:N52"/>
-    <mergeCell ref="O52:S52"/>
-    <mergeCell ref="T52:X52"/>
-    <mergeCell ref="Y52:AC52"/>
-    <mergeCell ref="AD52:AH52"/>
-    <mergeCell ref="AI48:AN48"/>
-    <mergeCell ref="A49:K50"/>
-    <mergeCell ref="A51:K51"/>
-    <mergeCell ref="L51:N51"/>
-    <mergeCell ref="O51:S51"/>
-    <mergeCell ref="T51:X51"/>
-    <mergeCell ref="Y51:AC51"/>
-    <mergeCell ref="AD51:AH51"/>
-    <mergeCell ref="AI51:AN51"/>
-    <mergeCell ref="A48:K48"/>
-    <mergeCell ref="L48:N48"/>
-    <mergeCell ref="O48:S48"/>
-    <mergeCell ref="T48:X48"/>
-    <mergeCell ref="Y48:AC48"/>
-    <mergeCell ref="AD48:AH48"/>
-    <mergeCell ref="AI46:AN46"/>
-    <mergeCell ref="A47:K47"/>
-    <mergeCell ref="L47:N47"/>
-    <mergeCell ref="O47:S47"/>
-    <mergeCell ref="T47:X47"/>
-    <mergeCell ref="Y47:AC47"/>
-    <mergeCell ref="AD47:AH47"/>
-    <mergeCell ref="AI47:AN47"/>
-    <mergeCell ref="A46:K46"/>
-    <mergeCell ref="L46:N46"/>
-    <mergeCell ref="O46:S46"/>
-    <mergeCell ref="T46:X46"/>
-    <mergeCell ref="Y46:AC46"/>
-    <mergeCell ref="AD46:AH46"/>
-    <mergeCell ref="AI44:AN44"/>
-    <mergeCell ref="A45:K45"/>
-    <mergeCell ref="L45:N45"/>
-    <mergeCell ref="O45:S45"/>
-    <mergeCell ref="T45:X45"/>
-    <mergeCell ref="Y45:AC45"/>
-    <mergeCell ref="AD45:AH45"/>
-    <mergeCell ref="AI45:AN45"/>
-    <mergeCell ref="A44:K44"/>
-    <mergeCell ref="L44:N44"/>
-    <mergeCell ref="O44:S44"/>
-    <mergeCell ref="T44:X44"/>
-    <mergeCell ref="Y44:AC44"/>
-    <mergeCell ref="AD44:AH44"/>
-    <mergeCell ref="AI42:AN42"/>
-    <mergeCell ref="A43:K43"/>
-    <mergeCell ref="L43:N43"/>
-    <mergeCell ref="O43:S43"/>
-    <mergeCell ref="T43:X43"/>
-    <mergeCell ref="Y43:AC43"/>
-    <mergeCell ref="AD43:AH43"/>
-    <mergeCell ref="AI43:AN43"/>
-    <mergeCell ref="A42:K42"/>
-    <mergeCell ref="L42:N42"/>
-    <mergeCell ref="O42:S42"/>
-    <mergeCell ref="T42:X42"/>
-    <mergeCell ref="Y42:AC42"/>
-    <mergeCell ref="AD42:AH42"/>
-    <mergeCell ref="AI40:AN40"/>
-    <mergeCell ref="A41:K41"/>
-    <mergeCell ref="L41:N41"/>
-    <mergeCell ref="O41:S41"/>
-    <mergeCell ref="T41:X41"/>
-    <mergeCell ref="Y41:AC41"/>
-    <mergeCell ref="AD41:AH41"/>
-    <mergeCell ref="AI41:AN41"/>
-    <mergeCell ref="A40:K40"/>
-    <mergeCell ref="L40:N40"/>
-    <mergeCell ref="O40:S40"/>
-    <mergeCell ref="T40:X40"/>
-    <mergeCell ref="Y40:AC40"/>
-    <mergeCell ref="AD40:AH40"/>
-    <mergeCell ref="AI38:AN38"/>
-    <mergeCell ref="A39:K39"/>
-    <mergeCell ref="L39:N39"/>
-    <mergeCell ref="O39:S39"/>
-    <mergeCell ref="T39:X39"/>
-    <mergeCell ref="Y39:AC39"/>
-    <mergeCell ref="AD39:AH39"/>
-    <mergeCell ref="AI39:AN39"/>
-    <mergeCell ref="A38:K38"/>
-    <mergeCell ref="L38:N38"/>
-    <mergeCell ref="O38:S38"/>
-    <mergeCell ref="T38:X38"/>
-    <mergeCell ref="Y38:AC38"/>
-    <mergeCell ref="AD38:AH38"/>
-    <mergeCell ref="A34:AN34"/>
-    <mergeCell ref="A35:K37"/>
-    <mergeCell ref="L35:N37"/>
-    <mergeCell ref="O35:AH35"/>
-    <mergeCell ref="AI35:AN37"/>
-    <mergeCell ref="O36:S37"/>
-    <mergeCell ref="T36:X37"/>
-    <mergeCell ref="Y36:AC37"/>
-    <mergeCell ref="AD36:AH37"/>
-    <mergeCell ref="A13:AN13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:M15"/>
-    <mergeCell ref="A25:AN25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:M27"/>
-    <mergeCell ref="A2:AN2"/>
-    <mergeCell ref="A3:AN3"/>
-    <mergeCell ref="A4:AN4"/>
-    <mergeCell ref="L5:AB9"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:E12"/>
-    <mergeCell ref="H11:I12"/>
-    <mergeCell ref="R11:U12"/>
-    <mergeCell ref="Y11:AA12"/>
-    <mergeCell ref="AI11:AN12"/>
+    <mergeCell ref="P64:Z64"/>
+    <mergeCell ref="A70:AN70"/>
+    <mergeCell ref="A71:AN73"/>
+    <mergeCell ref="A74:AN74"/>
+    <mergeCell ref="A75:AN75"/>
+    <mergeCell ref="A76:H76"/>
+    <mergeCell ref="R76:U77"/>
+    <mergeCell ref="AC76:AG76"/>
+    <mergeCell ref="A77:H77"/>
+    <mergeCell ref="AC77:AG77"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0" top="0.15748031496062992" bottom="0" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
BIR2307 new format, adjusted based on the user request.
</commit_message>
<xml_diff>
--- a/ExpenseProcessingSystem/ExpenseProcessingSystem/wwwroot/ExcelTemplates/_BIR2307_New.xlsx
+++ b/ExpenseProcessingSystem/ExpenseProcessingSystem/wwwroot/ExcelTemplates/_BIR2307_New.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Mizuho EPS\eps_source\ExpenseProcessingSystem\ExpenseProcessingSystem\wwwroot\ExcelTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F79945F7-3CCD-49D9-A1E6-64626C4950AC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22A5805D-61FE-4C34-B521-0826C60DB70C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="-1590" windowWidth="24240" windowHeight="13140" tabRatio="876" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -996,6 +996,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="43" fontId="2" fillId="2" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1148,18 +1160,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4868,7 +4868,9 @@
   </sheetPr>
   <dimension ref="A1:AN79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="160" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="160" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:K38"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4880,136 +4882,136 @@
   <sheetData>
     <row r="1" spans="1:40" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="138" t="s">
+      <c r="A2" s="142" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="138"/>
-      <c r="C2" s="138"/>
-      <c r="D2" s="138"/>
-      <c r="E2" s="138"/>
-      <c r="F2" s="138"/>
-      <c r="G2" s="138"/>
-      <c r="H2" s="138"/>
-      <c r="I2" s="138"/>
-      <c r="J2" s="138"/>
-      <c r="K2" s="138"/>
-      <c r="L2" s="138"/>
-      <c r="M2" s="138"/>
-      <c r="N2" s="138"/>
-      <c r="O2" s="138"/>
-      <c r="P2" s="138"/>
-      <c r="Q2" s="138"/>
-      <c r="R2" s="138"/>
-      <c r="S2" s="138"/>
-      <c r="T2" s="138"/>
-      <c r="U2" s="138"/>
-      <c r="V2" s="138"/>
-      <c r="W2" s="138"/>
-      <c r="X2" s="138"/>
-      <c r="Y2" s="138"/>
-      <c r="Z2" s="138"/>
-      <c r="AA2" s="138"/>
-      <c r="AB2" s="138"/>
-      <c r="AC2" s="138"/>
-      <c r="AD2" s="138"/>
-      <c r="AE2" s="138"/>
-      <c r="AF2" s="138"/>
-      <c r="AG2" s="138"/>
-      <c r="AH2" s="138"/>
-      <c r="AI2" s="138"/>
-      <c r="AJ2" s="138"/>
-      <c r="AK2" s="138"/>
-      <c r="AL2" s="138"/>
-      <c r="AM2" s="138"/>
-      <c r="AN2" s="138"/>
+      <c r="B2" s="142"/>
+      <c r="C2" s="142"/>
+      <c r="D2" s="142"/>
+      <c r="E2" s="142"/>
+      <c r="F2" s="142"/>
+      <c r="G2" s="142"/>
+      <c r="H2" s="142"/>
+      <c r="I2" s="142"/>
+      <c r="J2" s="142"/>
+      <c r="K2" s="142"/>
+      <c r="L2" s="142"/>
+      <c r="M2" s="142"/>
+      <c r="N2" s="142"/>
+      <c r="O2" s="142"/>
+      <c r="P2" s="142"/>
+      <c r="Q2" s="142"/>
+      <c r="R2" s="142"/>
+      <c r="S2" s="142"/>
+      <c r="T2" s="142"/>
+      <c r="U2" s="142"/>
+      <c r="V2" s="142"/>
+      <c r="W2" s="142"/>
+      <c r="X2" s="142"/>
+      <c r="Y2" s="142"/>
+      <c r="Z2" s="142"/>
+      <c r="AA2" s="142"/>
+      <c r="AB2" s="142"/>
+      <c r="AC2" s="142"/>
+      <c r="AD2" s="142"/>
+      <c r="AE2" s="142"/>
+      <c r="AF2" s="142"/>
+      <c r="AG2" s="142"/>
+      <c r="AH2" s="142"/>
+      <c r="AI2" s="142"/>
+      <c r="AJ2" s="142"/>
+      <c r="AK2" s="142"/>
+      <c r="AL2" s="142"/>
+      <c r="AM2" s="142"/>
+      <c r="AN2" s="142"/>
     </row>
     <row r="3" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="138" t="s">
+      <c r="A3" s="142" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="138"/>
-      <c r="C3" s="138"/>
-      <c r="D3" s="138"/>
-      <c r="E3" s="138"/>
-      <c r="F3" s="138"/>
-      <c r="G3" s="138"/>
-      <c r="H3" s="138"/>
-      <c r="I3" s="138"/>
-      <c r="J3" s="138"/>
-      <c r="K3" s="138"/>
-      <c r="L3" s="138"/>
-      <c r="M3" s="138"/>
-      <c r="N3" s="138"/>
-      <c r="O3" s="138"/>
-      <c r="P3" s="138"/>
-      <c r="Q3" s="138"/>
-      <c r="R3" s="138"/>
-      <c r="S3" s="138"/>
-      <c r="T3" s="138"/>
-      <c r="U3" s="138"/>
-      <c r="V3" s="138"/>
-      <c r="W3" s="138"/>
-      <c r="X3" s="138"/>
-      <c r="Y3" s="138"/>
-      <c r="Z3" s="138"/>
-      <c r="AA3" s="138"/>
-      <c r="AB3" s="138"/>
-      <c r="AC3" s="138"/>
-      <c r="AD3" s="138"/>
-      <c r="AE3" s="138"/>
-      <c r="AF3" s="138"/>
-      <c r="AG3" s="138"/>
-      <c r="AH3" s="138"/>
-      <c r="AI3" s="138"/>
-      <c r="AJ3" s="138"/>
-      <c r="AK3" s="138"/>
-      <c r="AL3" s="138"/>
-      <c r="AM3" s="138"/>
-      <c r="AN3" s="138"/>
+      <c r="B3" s="142"/>
+      <c r="C3" s="142"/>
+      <c r="D3" s="142"/>
+      <c r="E3" s="142"/>
+      <c r="F3" s="142"/>
+      <c r="G3" s="142"/>
+      <c r="H3" s="142"/>
+      <c r="I3" s="142"/>
+      <c r="J3" s="142"/>
+      <c r="K3" s="142"/>
+      <c r="L3" s="142"/>
+      <c r="M3" s="142"/>
+      <c r="N3" s="142"/>
+      <c r="O3" s="142"/>
+      <c r="P3" s="142"/>
+      <c r="Q3" s="142"/>
+      <c r="R3" s="142"/>
+      <c r="S3" s="142"/>
+      <c r="T3" s="142"/>
+      <c r="U3" s="142"/>
+      <c r="V3" s="142"/>
+      <c r="W3" s="142"/>
+      <c r="X3" s="142"/>
+      <c r="Y3" s="142"/>
+      <c r="Z3" s="142"/>
+      <c r="AA3" s="142"/>
+      <c r="AB3" s="142"/>
+      <c r="AC3" s="142"/>
+      <c r="AD3" s="142"/>
+      <c r="AE3" s="142"/>
+      <c r="AF3" s="142"/>
+      <c r="AG3" s="142"/>
+      <c r="AH3" s="142"/>
+      <c r="AI3" s="142"/>
+      <c r="AJ3" s="142"/>
+      <c r="AK3" s="142"/>
+      <c r="AL3" s="142"/>
+      <c r="AM3" s="142"/>
+      <c r="AN3" s="142"/>
     </row>
     <row r="4" spans="1:40" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="139" t="s">
+      <c r="A4" s="143" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="139"/>
-      <c r="C4" s="139"/>
-      <c r="D4" s="139"/>
-      <c r="E4" s="139"/>
-      <c r="F4" s="139"/>
-      <c r="G4" s="139"/>
-      <c r="H4" s="139"/>
-      <c r="I4" s="139"/>
-      <c r="J4" s="139"/>
-      <c r="K4" s="139"/>
-      <c r="L4" s="139"/>
-      <c r="M4" s="139"/>
-      <c r="N4" s="139"/>
-      <c r="O4" s="139"/>
-      <c r="P4" s="139"/>
-      <c r="Q4" s="139"/>
-      <c r="R4" s="139"/>
-      <c r="S4" s="139"/>
-      <c r="T4" s="139"/>
-      <c r="U4" s="139"/>
-      <c r="V4" s="139"/>
-      <c r="W4" s="139"/>
-      <c r="X4" s="139"/>
-      <c r="Y4" s="139"/>
-      <c r="Z4" s="139"/>
-      <c r="AA4" s="139"/>
-      <c r="AB4" s="139"/>
-      <c r="AC4" s="139"/>
-      <c r="AD4" s="139"/>
-      <c r="AE4" s="139"/>
-      <c r="AF4" s="139"/>
-      <c r="AG4" s="139"/>
-      <c r="AH4" s="139"/>
-      <c r="AI4" s="139"/>
-      <c r="AJ4" s="139"/>
-      <c r="AK4" s="139"/>
-      <c r="AL4" s="139"/>
-      <c r="AM4" s="139"/>
-      <c r="AN4" s="139"/>
+      <c r="B4" s="143"/>
+      <c r="C4" s="143"/>
+      <c r="D4" s="143"/>
+      <c r="E4" s="143"/>
+      <c r="F4" s="143"/>
+      <c r="G4" s="143"/>
+      <c r="H4" s="143"/>
+      <c r="I4" s="143"/>
+      <c r="J4" s="143"/>
+      <c r="K4" s="143"/>
+      <c r="L4" s="143"/>
+      <c r="M4" s="143"/>
+      <c r="N4" s="143"/>
+      <c r="O4" s="143"/>
+      <c r="P4" s="143"/>
+      <c r="Q4" s="143"/>
+      <c r="R4" s="143"/>
+      <c r="S4" s="143"/>
+      <c r="T4" s="143"/>
+      <c r="U4" s="143"/>
+      <c r="V4" s="143"/>
+      <c r="W4" s="143"/>
+      <c r="X4" s="143"/>
+      <c r="Y4" s="143"/>
+      <c r="Z4" s="143"/>
+      <c r="AA4" s="143"/>
+      <c r="AB4" s="143"/>
+      <c r="AC4" s="143"/>
+      <c r="AD4" s="143"/>
+      <c r="AE4" s="143"/>
+      <c r="AF4" s="143"/>
+      <c r="AG4" s="143"/>
+      <c r="AH4" s="143"/>
+      <c r="AI4" s="143"/>
+      <c r="AJ4" s="143"/>
+      <c r="AK4" s="143"/>
+      <c r="AL4" s="143"/>
+      <c r="AM4" s="143"/>
+      <c r="AN4" s="143"/>
     </row>
     <row r="5" spans="1:40" ht="9.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
@@ -5023,25 +5025,25 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-      <c r="L5" s="140" t="s">
+      <c r="L5" s="144" t="s">
         <v>7</v>
       </c>
-      <c r="M5" s="140"/>
-      <c r="N5" s="140"/>
-      <c r="O5" s="140"/>
-      <c r="P5" s="140"/>
-      <c r="Q5" s="140"/>
-      <c r="R5" s="140"/>
-      <c r="S5" s="140"/>
-      <c r="T5" s="140"/>
-      <c r="U5" s="140"/>
-      <c r="V5" s="140"/>
-      <c r="W5" s="140"/>
-      <c r="X5" s="140"/>
-      <c r="Y5" s="140"/>
-      <c r="Z5" s="140"/>
-      <c r="AA5" s="140"/>
-      <c r="AB5" s="140"/>
+      <c r="M5" s="144"/>
+      <c r="N5" s="144"/>
+      <c r="O5" s="144"/>
+      <c r="P5" s="144"/>
+      <c r="Q5" s="144"/>
+      <c r="R5" s="144"/>
+      <c r="S5" s="144"/>
+      <c r="T5" s="144"/>
+      <c r="U5" s="144"/>
+      <c r="V5" s="144"/>
+      <c r="W5" s="144"/>
+      <c r="X5" s="144"/>
+      <c r="Y5" s="144"/>
+      <c r="Z5" s="144"/>
+      <c r="AA5" s="144"/>
+      <c r="AB5" s="144"/>
       <c r="AC5" s="1"/>
       <c r="AD5" s="7"/>
       <c r="AE5" s="1"/>
@@ -5067,23 +5069,23 @@
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
-      <c r="L6" s="141"/>
-      <c r="M6" s="141"/>
-      <c r="N6" s="141"/>
-      <c r="O6" s="141"/>
-      <c r="P6" s="141"/>
-      <c r="Q6" s="141"/>
-      <c r="R6" s="141"/>
-      <c r="S6" s="141"/>
-      <c r="T6" s="141"/>
-      <c r="U6" s="141"/>
-      <c r="V6" s="141"/>
-      <c r="W6" s="141"/>
-      <c r="X6" s="141"/>
-      <c r="Y6" s="141"/>
-      <c r="Z6" s="141"/>
-      <c r="AA6" s="141"/>
-      <c r="AB6" s="141"/>
+      <c r="L6" s="145"/>
+      <c r="M6" s="145"/>
+      <c r="N6" s="145"/>
+      <c r="O6" s="145"/>
+      <c r="P6" s="145"/>
+      <c r="Q6" s="145"/>
+      <c r="R6" s="145"/>
+      <c r="S6" s="145"/>
+      <c r="T6" s="145"/>
+      <c r="U6" s="145"/>
+      <c r="V6" s="145"/>
+      <c r="W6" s="145"/>
+      <c r="X6" s="145"/>
+      <c r="Y6" s="145"/>
+      <c r="Z6" s="145"/>
+      <c r="AA6" s="145"/>
+      <c r="AB6" s="145"/>
       <c r="AC6" s="4"/>
       <c r="AD6" s="8"/>
       <c r="AE6" s="4"/>
@@ -5109,23 +5111,23 @@
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
-      <c r="L7" s="141"/>
-      <c r="M7" s="141"/>
-      <c r="N7" s="141"/>
-      <c r="O7" s="141"/>
-      <c r="P7" s="141"/>
-      <c r="Q7" s="141"/>
-      <c r="R7" s="141"/>
-      <c r="S7" s="141"/>
-      <c r="T7" s="141"/>
-      <c r="U7" s="141"/>
-      <c r="V7" s="141"/>
-      <c r="W7" s="141"/>
-      <c r="X7" s="141"/>
-      <c r="Y7" s="141"/>
-      <c r="Z7" s="141"/>
-      <c r="AA7" s="141"/>
-      <c r="AB7" s="141"/>
+      <c r="L7" s="145"/>
+      <c r="M7" s="145"/>
+      <c r="N7" s="145"/>
+      <c r="O7" s="145"/>
+      <c r="P7" s="145"/>
+      <c r="Q7" s="145"/>
+      <c r="R7" s="145"/>
+      <c r="S7" s="145"/>
+      <c r="T7" s="145"/>
+      <c r="U7" s="145"/>
+      <c r="V7" s="145"/>
+      <c r="W7" s="145"/>
+      <c r="X7" s="145"/>
+      <c r="Y7" s="145"/>
+      <c r="Z7" s="145"/>
+      <c r="AA7" s="145"/>
+      <c r="AB7" s="145"/>
       <c r="AC7" s="4"/>
       <c r="AD7" s="8"/>
       <c r="AE7" s="4"/>
@@ -5151,23 +5153,23 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
-      <c r="L8" s="141"/>
-      <c r="M8" s="141"/>
-      <c r="N8" s="141"/>
-      <c r="O8" s="141"/>
-      <c r="P8" s="141"/>
-      <c r="Q8" s="141"/>
-      <c r="R8" s="141"/>
-      <c r="S8" s="141"/>
-      <c r="T8" s="141"/>
-      <c r="U8" s="141"/>
-      <c r="V8" s="141"/>
-      <c r="W8" s="141"/>
-      <c r="X8" s="141"/>
-      <c r="Y8" s="141"/>
-      <c r="Z8" s="141"/>
-      <c r="AA8" s="141"/>
-      <c r="AB8" s="141"/>
+      <c r="L8" s="145"/>
+      <c r="M8" s="145"/>
+      <c r="N8" s="145"/>
+      <c r="O8" s="145"/>
+      <c r="P8" s="145"/>
+      <c r="Q8" s="145"/>
+      <c r="R8" s="145"/>
+      <c r="S8" s="145"/>
+      <c r="T8" s="145"/>
+      <c r="U8" s="145"/>
+      <c r="V8" s="145"/>
+      <c r="W8" s="145"/>
+      <c r="X8" s="145"/>
+      <c r="Y8" s="145"/>
+      <c r="Z8" s="145"/>
+      <c r="AA8" s="145"/>
+      <c r="AB8" s="145"/>
       <c r="AC8" s="4"/>
       <c r="AD8" s="8"/>
       <c r="AE8" s="4"/>
@@ -5193,23 +5195,23 @@
       <c r="I9" s="13"/>
       <c r="J9" s="13"/>
       <c r="K9" s="13"/>
-      <c r="L9" s="142"/>
-      <c r="M9" s="142"/>
-      <c r="N9" s="142"/>
-      <c r="O9" s="142"/>
-      <c r="P9" s="142"/>
-      <c r="Q9" s="142"/>
-      <c r="R9" s="142"/>
-      <c r="S9" s="142"/>
-      <c r="T9" s="142"/>
-      <c r="U9" s="142"/>
-      <c r="V9" s="142"/>
-      <c r="W9" s="142"/>
-      <c r="X9" s="142"/>
-      <c r="Y9" s="142"/>
-      <c r="Z9" s="142"/>
-      <c r="AA9" s="142"/>
-      <c r="AB9" s="142"/>
+      <c r="L9" s="146"/>
+      <c r="M9" s="146"/>
+      <c r="N9" s="146"/>
+      <c r="O9" s="146"/>
+      <c r="P9" s="146"/>
+      <c r="Q9" s="146"/>
+      <c r="R9" s="146"/>
+      <c r="S9" s="146"/>
+      <c r="T9" s="146"/>
+      <c r="U9" s="146"/>
+      <c r="V9" s="146"/>
+      <c r="W9" s="146"/>
+      <c r="X9" s="146"/>
+      <c r="Y9" s="146"/>
+      <c r="Z9" s="146"/>
+      <c r="AA9" s="146"/>
+      <c r="AB9" s="146"/>
       <c r="AC9" s="32"/>
       <c r="AD9" s="19"/>
       <c r="AE9" s="42"/>
@@ -5268,21 +5270,21 @@
       <c r="AN10" s="21"/>
     </row>
     <row r="11" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A11" s="134">
+      <c r="A11" s="138">
         <v>1</v>
       </c>
-      <c r="B11" s="144" t="s">
+      <c r="B11" s="148" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="144"/>
-      <c r="D11" s="144"/>
-      <c r="E11" s="144"/>
+      <c r="C11" s="148"/>
+      <c r="D11" s="148"/>
+      <c r="E11" s="148"/>
       <c r="F11" s="33"/>
       <c r="G11" s="33"/>
-      <c r="H11" s="146" t="s">
+      <c r="H11" s="150" t="s">
         <v>37</v>
       </c>
-      <c r="I11" s="146"/>
+      <c r="I11" s="150"/>
       <c r="J11" s="33"/>
       <c r="K11" s="33"/>
       <c r="L11" s="33"/>
@@ -5291,20 +5293,20 @@
       <c r="O11" s="33"/>
       <c r="P11" s="33"/>
       <c r="Q11" s="33"/>
-      <c r="R11" s="148" t="s">
+      <c r="R11" s="152" t="s">
         <v>8</v>
       </c>
-      <c r="S11" s="148"/>
-      <c r="T11" s="148"/>
-      <c r="U11" s="148"/>
+      <c r="S11" s="152"/>
+      <c r="T11" s="152"/>
+      <c r="U11" s="152"/>
       <c r="V11" s="33"/>
       <c r="W11" s="33"/>
       <c r="X11" s="33"/>
-      <c r="Y11" s="144" t="s">
+      <c r="Y11" s="148" t="s">
         <v>9</v>
       </c>
-      <c r="Z11" s="144"/>
-      <c r="AA11" s="144"/>
+      <c r="Z11" s="148"/>
+      <c r="AA11" s="148"/>
       <c r="AB11" s="33"/>
       <c r="AC11" s="33"/>
       <c r="AD11" s="33"/>
@@ -5312,25 +5314,25 @@
       <c r="AF11" s="33"/>
       <c r="AG11" s="33"/>
       <c r="AH11" s="33"/>
-      <c r="AI11" s="150" t="s">
+      <c r="AI11" s="154" t="s">
         <v>8</v>
       </c>
-      <c r="AJ11" s="150"/>
-      <c r="AK11" s="150"/>
-      <c r="AL11" s="150"/>
-      <c r="AM11" s="150"/>
-      <c r="AN11" s="151"/>
+      <c r="AJ11" s="154"/>
+      <c r="AK11" s="154"/>
+      <c r="AL11" s="154"/>
+      <c r="AM11" s="154"/>
+      <c r="AN11" s="155"/>
     </row>
     <row r="12" spans="1:40" s="55" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="143"/>
-      <c r="B12" s="145"/>
-      <c r="C12" s="145"/>
-      <c r="D12" s="145"/>
-      <c r="E12" s="145"/>
+      <c r="A12" s="147"/>
+      <c r="B12" s="149"/>
+      <c r="C12" s="149"/>
+      <c r="D12" s="149"/>
+      <c r="E12" s="149"/>
       <c r="F12" s="54"/>
       <c r="G12" s="54"/>
-      <c r="H12" s="147"/>
-      <c r="I12" s="147"/>
+      <c r="H12" s="151"/>
+      <c r="I12" s="151"/>
       <c r="J12" s="54"/>
       <c r="K12" s="54"/>
       <c r="L12" s="54"/>
@@ -5339,16 +5341,16 @@
       <c r="O12" s="54"/>
       <c r="P12" s="54"/>
       <c r="Q12" s="54"/>
-      <c r="R12" s="149"/>
-      <c r="S12" s="149"/>
-      <c r="T12" s="149"/>
-      <c r="U12" s="149"/>
+      <c r="R12" s="153"/>
+      <c r="S12" s="153"/>
+      <c r="T12" s="153"/>
+      <c r="U12" s="153"/>
       <c r="V12" s="54"/>
       <c r="W12" s="54"/>
       <c r="X12" s="54"/>
-      <c r="Y12" s="145"/>
-      <c r="Z12" s="145"/>
-      <c r="AA12" s="145"/>
+      <c r="Y12" s="149"/>
+      <c r="Z12" s="149"/>
+      <c r="AA12" s="149"/>
       <c r="AB12" s="54"/>
       <c r="AC12" s="54"/>
       <c r="AD12" s="54"/>
@@ -5356,12 +5358,12 @@
       <c r="AF12" s="54"/>
       <c r="AG12" s="54"/>
       <c r="AH12" s="54"/>
-      <c r="AI12" s="152"/>
-      <c r="AJ12" s="152"/>
-      <c r="AK12" s="152"/>
-      <c r="AL12" s="152"/>
-      <c r="AM12" s="152"/>
-      <c r="AN12" s="153"/>
+      <c r="AI12" s="156"/>
+      <c r="AJ12" s="156"/>
+      <c r="AK12" s="156"/>
+      <c r="AL12" s="156"/>
+      <c r="AM12" s="156"/>
+      <c r="AN12" s="157"/>
     </row>
     <row r="13" spans="1:40" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="56" t="s">
@@ -5408,23 +5410,23 @@
       <c r="AN13" s="58"/>
     </row>
     <row r="14" spans="1:40" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="134">
+      <c r="A14" s="138">
         <v>2</v>
       </c>
-      <c r="B14" s="136" t="s">
+      <c r="B14" s="140" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="136"/>
-      <c r="D14" s="136"/>
-      <c r="E14" s="136"/>
-      <c r="F14" s="136"/>
-      <c r="G14" s="136"/>
-      <c r="H14" s="136"/>
-      <c r="I14" s="136"/>
-      <c r="J14" s="136"/>
-      <c r="K14" s="136"/>
-      <c r="L14" s="136"/>
-      <c r="M14" s="136"/>
+      <c r="C14" s="140"/>
+      <c r="D14" s="140"/>
+      <c r="E14" s="140"/>
+      <c r="F14" s="140"/>
+      <c r="G14" s="140"/>
+      <c r="H14" s="140"/>
+      <c r="I14" s="140"/>
+      <c r="J14" s="140"/>
+      <c r="K14" s="140"/>
+      <c r="L14" s="140"/>
+      <c r="M14" s="140"/>
       <c r="N14" s="33"/>
       <c r="O14" s="33"/>
       <c r="P14" s="33"/>
@@ -5454,19 +5456,19 @@
       <c r="AN14" s="34"/>
     </row>
     <row r="15" spans="1:40" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="135"/>
-      <c r="B15" s="137"/>
-      <c r="C15" s="137"/>
-      <c r="D15" s="137"/>
-      <c r="E15" s="137"/>
-      <c r="F15" s="137"/>
-      <c r="G15" s="137"/>
-      <c r="H15" s="137"/>
-      <c r="I15" s="137"/>
-      <c r="J15" s="137"/>
-      <c r="K15" s="137"/>
-      <c r="L15" s="137"/>
-      <c r="M15" s="137"/>
+      <c r="A15" s="139"/>
+      <c r="B15" s="141"/>
+      <c r="C15" s="141"/>
+      <c r="D15" s="141"/>
+      <c r="E15" s="141"/>
+      <c r="F15" s="141"/>
+      <c r="G15" s="141"/>
+      <c r="H15" s="141"/>
+      <c r="I15" s="141"/>
+      <c r="J15" s="141"/>
+      <c r="K15" s="141"/>
+      <c r="L15" s="141"/>
+      <c r="M15" s="141"/>
       <c r="N15" s="16"/>
       <c r="O15" s="16"/>
       <c r="P15" s="16"/>
@@ -5934,23 +5936,23 @@
       <c r="AN25" s="58"/>
     </row>
     <row r="26" spans="1:40" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="134">
+      <c r="A26" s="138">
         <v>6</v>
       </c>
-      <c r="B26" s="136" t="s">
+      <c r="B26" s="140" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="136"/>
-      <c r="D26" s="136"/>
-      <c r="E26" s="136"/>
-      <c r="F26" s="136"/>
-      <c r="G26" s="136"/>
-      <c r="H26" s="136"/>
-      <c r="I26" s="136"/>
-      <c r="J26" s="136"/>
-      <c r="K26" s="136"/>
-      <c r="L26" s="136"/>
-      <c r="M26" s="136"/>
+      <c r="C26" s="140"/>
+      <c r="D26" s="140"/>
+      <c r="E26" s="140"/>
+      <c r="F26" s="140"/>
+      <c r="G26" s="140"/>
+      <c r="H26" s="140"/>
+      <c r="I26" s="140"/>
+      <c r="J26" s="140"/>
+      <c r="K26" s="140"/>
+      <c r="L26" s="140"/>
+      <c r="M26" s="140"/>
       <c r="N26" s="33"/>
       <c r="O26" s="33"/>
       <c r="P26" s="33"/>
@@ -5980,19 +5982,19 @@
       <c r="AN26" s="34"/>
     </row>
     <row r="27" spans="1:40" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="135"/>
-      <c r="B27" s="137"/>
-      <c r="C27" s="137"/>
-      <c r="D27" s="137"/>
-      <c r="E27" s="137"/>
-      <c r="F27" s="137"/>
-      <c r="G27" s="137"/>
-      <c r="H27" s="137"/>
-      <c r="I27" s="137"/>
-      <c r="J27" s="137"/>
-      <c r="K27" s="137"/>
-      <c r="L27" s="137"/>
-      <c r="M27" s="137"/>
+      <c r="A27" s="139"/>
+      <c r="B27" s="141"/>
+      <c r="C27" s="141"/>
+      <c r="D27" s="141"/>
+      <c r="E27" s="141"/>
+      <c r="F27" s="141"/>
+      <c r="G27" s="141"/>
+      <c r="H27" s="141"/>
+      <c r="I27" s="141"/>
+      <c r="J27" s="141"/>
+      <c r="K27" s="141"/>
+      <c r="L27" s="141"/>
+      <c r="M27" s="141"/>
       <c r="N27" s="16"/>
       <c r="O27" s="16"/>
       <c r="P27" s="16"/>
@@ -6286,203 +6288,203 @@
       <c r="AN33" s="29"/>
     </row>
     <row r="34" spans="1:40" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="115" t="s">
+      <c r="A34" s="119" t="s">
         <v>20</v>
       </c>
-      <c r="B34" s="116"/>
-      <c r="C34" s="116"/>
-      <c r="D34" s="116"/>
-      <c r="E34" s="116"/>
-      <c r="F34" s="116"/>
-      <c r="G34" s="116"/>
-      <c r="H34" s="116"/>
-      <c r="I34" s="116"/>
-      <c r="J34" s="116"/>
-      <c r="K34" s="116"/>
-      <c r="L34" s="116"/>
-      <c r="M34" s="116"/>
-      <c r="N34" s="116"/>
-      <c r="O34" s="116"/>
-      <c r="P34" s="116"/>
-      <c r="Q34" s="116"/>
-      <c r="R34" s="116"/>
-      <c r="S34" s="116"/>
-      <c r="T34" s="116"/>
-      <c r="U34" s="116"/>
-      <c r="V34" s="116"/>
-      <c r="W34" s="116"/>
-      <c r="X34" s="116"/>
-      <c r="Y34" s="116"/>
-      <c r="Z34" s="116"/>
-      <c r="AA34" s="116"/>
-      <c r="AB34" s="116"/>
-      <c r="AC34" s="116"/>
-      <c r="AD34" s="116"/>
-      <c r="AE34" s="116"/>
-      <c r="AF34" s="116"/>
-      <c r="AG34" s="116"/>
-      <c r="AH34" s="116"/>
-      <c r="AI34" s="116"/>
-      <c r="AJ34" s="116"/>
-      <c r="AK34" s="116"/>
-      <c r="AL34" s="116"/>
-      <c r="AM34" s="116"/>
-      <c r="AN34" s="117"/>
+      <c r="B34" s="120"/>
+      <c r="C34" s="120"/>
+      <c r="D34" s="120"/>
+      <c r="E34" s="120"/>
+      <c r="F34" s="120"/>
+      <c r="G34" s="120"/>
+      <c r="H34" s="120"/>
+      <c r="I34" s="120"/>
+      <c r="J34" s="120"/>
+      <c r="K34" s="120"/>
+      <c r="L34" s="120"/>
+      <c r="M34" s="120"/>
+      <c r="N34" s="120"/>
+      <c r="O34" s="120"/>
+      <c r="P34" s="120"/>
+      <c r="Q34" s="120"/>
+      <c r="R34" s="120"/>
+      <c r="S34" s="120"/>
+      <c r="T34" s="120"/>
+      <c r="U34" s="120"/>
+      <c r="V34" s="120"/>
+      <c r="W34" s="120"/>
+      <c r="X34" s="120"/>
+      <c r="Y34" s="120"/>
+      <c r="Z34" s="120"/>
+      <c r="AA34" s="120"/>
+      <c r="AB34" s="120"/>
+      <c r="AC34" s="120"/>
+      <c r="AD34" s="120"/>
+      <c r="AE34" s="120"/>
+      <c r="AF34" s="120"/>
+      <c r="AG34" s="120"/>
+      <c r="AH34" s="120"/>
+      <c r="AI34" s="120"/>
+      <c r="AJ34" s="120"/>
+      <c r="AK34" s="120"/>
+      <c r="AL34" s="120"/>
+      <c r="AM34" s="120"/>
+      <c r="AN34" s="121"/>
     </row>
     <row r="35" spans="1:40" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="118" t="s">
+      <c r="A35" s="122" t="s">
         <v>22</v>
       </c>
-      <c r="B35" s="119"/>
-      <c r="C35" s="119"/>
-      <c r="D35" s="119"/>
-      <c r="E35" s="119"/>
-      <c r="F35" s="119"/>
-      <c r="G35" s="119"/>
-      <c r="H35" s="119"/>
-      <c r="I35" s="119"/>
-      <c r="J35" s="119"/>
-      <c r="K35" s="120"/>
-      <c r="L35" s="124" t="s">
+      <c r="B35" s="123"/>
+      <c r="C35" s="123"/>
+      <c r="D35" s="123"/>
+      <c r="E35" s="123"/>
+      <c r="F35" s="123"/>
+      <c r="G35" s="123"/>
+      <c r="H35" s="123"/>
+      <c r="I35" s="123"/>
+      <c r="J35" s="123"/>
+      <c r="K35" s="124"/>
+      <c r="L35" s="128" t="s">
         <v>23</v>
       </c>
-      <c r="M35" s="119"/>
-      <c r="N35" s="120"/>
-      <c r="O35" s="127" t="s">
+      <c r="M35" s="123"/>
+      <c r="N35" s="124"/>
+      <c r="O35" s="131" t="s">
         <v>24</v>
       </c>
-      <c r="P35" s="128"/>
-      <c r="Q35" s="128"/>
-      <c r="R35" s="128"/>
-      <c r="S35" s="128"/>
-      <c r="T35" s="128"/>
-      <c r="U35" s="128"/>
-      <c r="V35" s="128"/>
-      <c r="W35" s="128"/>
-      <c r="X35" s="128"/>
-      <c r="Y35" s="128"/>
-      <c r="Z35" s="128"/>
-      <c r="AA35" s="128"/>
-      <c r="AB35" s="128"/>
-      <c r="AC35" s="128"/>
-      <c r="AD35" s="128"/>
-      <c r="AE35" s="128"/>
-      <c r="AF35" s="128"/>
-      <c r="AG35" s="128"/>
-      <c r="AH35" s="129"/>
-      <c r="AI35" s="124" t="s">
+      <c r="P35" s="132"/>
+      <c r="Q35" s="132"/>
+      <c r="R35" s="132"/>
+      <c r="S35" s="132"/>
+      <c r="T35" s="132"/>
+      <c r="U35" s="132"/>
+      <c r="V35" s="132"/>
+      <c r="W35" s="132"/>
+      <c r="X35" s="132"/>
+      <c r="Y35" s="132"/>
+      <c r="Z35" s="132"/>
+      <c r="AA35" s="132"/>
+      <c r="AB35" s="132"/>
+      <c r="AC35" s="132"/>
+      <c r="AD35" s="132"/>
+      <c r="AE35" s="132"/>
+      <c r="AF35" s="132"/>
+      <c r="AG35" s="132"/>
+      <c r="AH35" s="133"/>
+      <c r="AI35" s="128" t="s">
         <v>21</v>
       </c>
-      <c r="AJ35" s="119"/>
-      <c r="AK35" s="119"/>
-      <c r="AL35" s="119"/>
-      <c r="AM35" s="119"/>
-      <c r="AN35" s="130"/>
+      <c r="AJ35" s="123"/>
+      <c r="AK35" s="123"/>
+      <c r="AL35" s="123"/>
+      <c r="AM35" s="123"/>
+      <c r="AN35" s="134"/>
     </row>
     <row r="36" spans="1:40" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="121"/>
-      <c r="B36" s="122"/>
-      <c r="C36" s="122"/>
-      <c r="D36" s="122"/>
-      <c r="E36" s="122"/>
-      <c r="F36" s="122"/>
-      <c r="G36" s="122"/>
-      <c r="H36" s="122"/>
-      <c r="I36" s="122"/>
-      <c r="J36" s="122"/>
-      <c r="K36" s="123"/>
-      <c r="L36" s="125"/>
-      <c r="M36" s="122"/>
-      <c r="N36" s="123"/>
-      <c r="O36" s="133" t="s">
+      <c r="A36" s="125"/>
+      <c r="B36" s="126"/>
+      <c r="C36" s="126"/>
+      <c r="D36" s="126"/>
+      <c r="E36" s="126"/>
+      <c r="F36" s="126"/>
+      <c r="G36" s="126"/>
+      <c r="H36" s="126"/>
+      <c r="I36" s="126"/>
+      <c r="J36" s="126"/>
+      <c r="K36" s="127"/>
+      <c r="L36" s="129"/>
+      <c r="M36" s="126"/>
+      <c r="N36" s="127"/>
+      <c r="O36" s="137" t="s">
         <v>28</v>
       </c>
-      <c r="P36" s="108"/>
-      <c r="Q36" s="108"/>
-      <c r="R36" s="108"/>
-      <c r="S36" s="109"/>
-      <c r="T36" s="133" t="s">
+      <c r="P36" s="112"/>
+      <c r="Q36" s="112"/>
+      <c r="R36" s="112"/>
+      <c r="S36" s="113"/>
+      <c r="T36" s="137" t="s">
         <v>27</v>
       </c>
-      <c r="U36" s="108"/>
-      <c r="V36" s="108"/>
-      <c r="W36" s="108"/>
-      <c r="X36" s="109"/>
-      <c r="Y36" s="133" t="s">
+      <c r="U36" s="112"/>
+      <c r="V36" s="112"/>
+      <c r="W36" s="112"/>
+      <c r="X36" s="113"/>
+      <c r="Y36" s="137" t="s">
         <v>26</v>
       </c>
-      <c r="Z36" s="108"/>
-      <c r="AA36" s="108"/>
-      <c r="AB36" s="108"/>
-      <c r="AC36" s="109"/>
-      <c r="AD36" s="133" t="s">
+      <c r="Z36" s="112"/>
+      <c r="AA36" s="112"/>
+      <c r="AB36" s="112"/>
+      <c r="AC36" s="113"/>
+      <c r="AD36" s="137" t="s">
         <v>25</v>
       </c>
-      <c r="AE36" s="108"/>
-      <c r="AF36" s="108"/>
-      <c r="AG36" s="108"/>
-      <c r="AH36" s="109"/>
-      <c r="AI36" s="125"/>
-      <c r="AJ36" s="122"/>
-      <c r="AK36" s="122"/>
-      <c r="AL36" s="122"/>
-      <c r="AM36" s="122"/>
-      <c r="AN36" s="131"/>
+      <c r="AE36" s="112"/>
+      <c r="AF36" s="112"/>
+      <c r="AG36" s="112"/>
+      <c r="AH36" s="113"/>
+      <c r="AI36" s="129"/>
+      <c r="AJ36" s="126"/>
+      <c r="AK36" s="126"/>
+      <c r="AL36" s="126"/>
+      <c r="AM36" s="126"/>
+      <c r="AN36" s="135"/>
     </row>
     <row r="37" spans="1:40" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="110"/>
-      <c r="B37" s="111"/>
-      <c r="C37" s="111"/>
-      <c r="D37" s="111"/>
-      <c r="E37" s="111"/>
-      <c r="F37" s="111"/>
-      <c r="G37" s="111"/>
-      <c r="H37" s="111"/>
-      <c r="I37" s="111"/>
-      <c r="J37" s="111"/>
-      <c r="K37" s="112"/>
-      <c r="L37" s="126"/>
-      <c r="M37" s="111"/>
-      <c r="N37" s="112"/>
-      <c r="O37" s="126"/>
-      <c r="P37" s="111"/>
-      <c r="Q37" s="111"/>
-      <c r="R37" s="111"/>
-      <c r="S37" s="112"/>
-      <c r="T37" s="126"/>
-      <c r="U37" s="111"/>
-      <c r="V37" s="111"/>
-      <c r="W37" s="111"/>
-      <c r="X37" s="112"/>
-      <c r="Y37" s="126"/>
-      <c r="Z37" s="111"/>
-      <c r="AA37" s="111"/>
-      <c r="AB37" s="111"/>
-      <c r="AC37" s="112"/>
-      <c r="AD37" s="126"/>
-      <c r="AE37" s="111"/>
-      <c r="AF37" s="111"/>
-      <c r="AG37" s="111"/>
-      <c r="AH37" s="112"/>
-      <c r="AI37" s="126"/>
-      <c r="AJ37" s="111"/>
-      <c r="AK37" s="111"/>
-      <c r="AL37" s="111"/>
-      <c r="AM37" s="111"/>
-      <c r="AN37" s="132"/>
+      <c r="A37" s="114"/>
+      <c r="B37" s="115"/>
+      <c r="C37" s="115"/>
+      <c r="D37" s="115"/>
+      <c r="E37" s="115"/>
+      <c r="F37" s="115"/>
+      <c r="G37" s="115"/>
+      <c r="H37" s="115"/>
+      <c r="I37" s="115"/>
+      <c r="J37" s="115"/>
+      <c r="K37" s="116"/>
+      <c r="L37" s="130"/>
+      <c r="M37" s="115"/>
+      <c r="N37" s="116"/>
+      <c r="O37" s="130"/>
+      <c r="P37" s="115"/>
+      <c r="Q37" s="115"/>
+      <c r="R37" s="115"/>
+      <c r="S37" s="116"/>
+      <c r="T37" s="130"/>
+      <c r="U37" s="115"/>
+      <c r="V37" s="115"/>
+      <c r="W37" s="115"/>
+      <c r="X37" s="116"/>
+      <c r="Y37" s="130"/>
+      <c r="Z37" s="115"/>
+      <c r="AA37" s="115"/>
+      <c r="AB37" s="115"/>
+      <c r="AC37" s="116"/>
+      <c r="AD37" s="130"/>
+      <c r="AE37" s="115"/>
+      <c r="AF37" s="115"/>
+      <c r="AG37" s="115"/>
+      <c r="AH37" s="116"/>
+      <c r="AI37" s="130"/>
+      <c r="AJ37" s="115"/>
+      <c r="AK37" s="115"/>
+      <c r="AL37" s="115"/>
+      <c r="AM37" s="115"/>
+      <c r="AN37" s="136"/>
     </row>
     <row r="38" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="154"/>
-      <c r="B38" s="155"/>
-      <c r="C38" s="155"/>
-      <c r="D38" s="155"/>
-      <c r="E38" s="155"/>
-      <c r="F38" s="155"/>
-      <c r="G38" s="155"/>
-      <c r="H38" s="155"/>
-      <c r="I38" s="155"/>
-      <c r="J38" s="155"/>
-      <c r="K38" s="156"/>
+      <c r="A38" s="104"/>
+      <c r="B38" s="105"/>
+      <c r="C38" s="105"/>
+      <c r="D38" s="105"/>
+      <c r="E38" s="105"/>
+      <c r="F38" s="105"/>
+      <c r="G38" s="105"/>
+      <c r="H38" s="105"/>
+      <c r="I38" s="105"/>
+      <c r="J38" s="105"/>
+      <c r="K38" s="106"/>
       <c r="L38" s="95"/>
       <c r="M38" s="96"/>
       <c r="N38" s="97"/>
@@ -6508,7 +6510,7 @@
       <c r="AE38" s="83"/>
       <c r="AF38" s="83"/>
       <c r="AG38" s="83"/>
-      <c r="AH38" s="103"/>
+      <c r="AH38" s="107"/>
       <c r="AI38" s="82"/>
       <c r="AJ38" s="83"/>
       <c r="AK38" s="83"/>
@@ -6517,17 +6519,17 @@
       <c r="AN38" s="84"/>
     </row>
     <row r="39" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="154"/>
-      <c r="B39" s="155"/>
-      <c r="C39" s="155"/>
-      <c r="D39" s="155"/>
-      <c r="E39" s="155"/>
-      <c r="F39" s="155"/>
-      <c r="G39" s="155"/>
-      <c r="H39" s="155"/>
-      <c r="I39" s="155"/>
-      <c r="J39" s="155"/>
-      <c r="K39" s="156"/>
+      <c r="A39" s="104"/>
+      <c r="B39" s="105"/>
+      <c r="C39" s="105"/>
+      <c r="D39" s="105"/>
+      <c r="E39" s="105"/>
+      <c r="F39" s="105"/>
+      <c r="G39" s="105"/>
+      <c r="H39" s="105"/>
+      <c r="I39" s="105"/>
+      <c r="J39" s="105"/>
+      <c r="K39" s="106"/>
       <c r="L39" s="95"/>
       <c r="M39" s="96"/>
       <c r="N39" s="97"/>
@@ -6553,26 +6555,26 @@
       <c r="AE39" s="83"/>
       <c r="AF39" s="83"/>
       <c r="AG39" s="83"/>
-      <c r="AH39" s="103"/>
+      <c r="AH39" s="107"/>
       <c r="AI39" s="95"/>
       <c r="AJ39" s="96"/>
       <c r="AK39" s="96"/>
       <c r="AL39" s="96"/>
       <c r="AM39" s="96"/>
-      <c r="AN39" s="114"/>
+      <c r="AN39" s="118"/>
     </row>
     <row r="40" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="154"/>
-      <c r="B40" s="155"/>
-      <c r="C40" s="155"/>
-      <c r="D40" s="155"/>
-      <c r="E40" s="155"/>
-      <c r="F40" s="155"/>
-      <c r="G40" s="155"/>
-      <c r="H40" s="155"/>
-      <c r="I40" s="155"/>
-      <c r="J40" s="155"/>
-      <c r="K40" s="156"/>
+      <c r="A40" s="104"/>
+      <c r="B40" s="105"/>
+      <c r="C40" s="105"/>
+      <c r="D40" s="105"/>
+      <c r="E40" s="105"/>
+      <c r="F40" s="105"/>
+      <c r="G40" s="105"/>
+      <c r="H40" s="105"/>
+      <c r="I40" s="105"/>
+      <c r="J40" s="105"/>
+      <c r="K40" s="106"/>
       <c r="L40" s="95"/>
       <c r="M40" s="96"/>
       <c r="N40" s="97"/>
@@ -6598,26 +6600,26 @@
       <c r="AE40" s="83"/>
       <c r="AF40" s="83"/>
       <c r="AG40" s="83"/>
-      <c r="AH40" s="103"/>
+      <c r="AH40" s="107"/>
       <c r="AI40" s="95"/>
       <c r="AJ40" s="96"/>
       <c r="AK40" s="96"/>
       <c r="AL40" s="96"/>
       <c r="AM40" s="96"/>
-      <c r="AN40" s="114"/>
+      <c r="AN40" s="118"/>
     </row>
     <row r="41" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="154"/>
-      <c r="B41" s="155"/>
-      <c r="C41" s="155"/>
-      <c r="D41" s="155"/>
-      <c r="E41" s="155"/>
-      <c r="F41" s="155"/>
-      <c r="G41" s="155"/>
-      <c r="H41" s="155"/>
-      <c r="I41" s="155"/>
-      <c r="J41" s="155"/>
-      <c r="K41" s="156"/>
+      <c r="A41" s="104"/>
+      <c r="B41" s="105"/>
+      <c r="C41" s="105"/>
+      <c r="D41" s="105"/>
+      <c r="E41" s="105"/>
+      <c r="F41" s="105"/>
+      <c r="G41" s="105"/>
+      <c r="H41" s="105"/>
+      <c r="I41" s="105"/>
+      <c r="J41" s="105"/>
+      <c r="K41" s="106"/>
       <c r="L41" s="95"/>
       <c r="M41" s="96"/>
       <c r="N41" s="97"/>
@@ -6643,26 +6645,26 @@
       <c r="AE41" s="83"/>
       <c r="AF41" s="83"/>
       <c r="AG41" s="83"/>
-      <c r="AH41" s="103"/>
+      <c r="AH41" s="107"/>
       <c r="AI41" s="95"/>
       <c r="AJ41" s="96"/>
       <c r="AK41" s="96"/>
       <c r="AL41" s="96"/>
       <c r="AM41" s="96"/>
-      <c r="AN41" s="114"/>
+      <c r="AN41" s="118"/>
     </row>
     <row r="42" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="154"/>
-      <c r="B42" s="155"/>
-      <c r="C42" s="155"/>
-      <c r="D42" s="155"/>
-      <c r="E42" s="155"/>
-      <c r="F42" s="155"/>
-      <c r="G42" s="155"/>
-      <c r="H42" s="155"/>
-      <c r="I42" s="155"/>
-      <c r="J42" s="155"/>
-      <c r="K42" s="156"/>
+      <c r="A42" s="104"/>
+      <c r="B42" s="105"/>
+      <c r="C42" s="105"/>
+      <c r="D42" s="105"/>
+      <c r="E42" s="105"/>
+      <c r="F42" s="105"/>
+      <c r="G42" s="105"/>
+      <c r="H42" s="105"/>
+      <c r="I42" s="105"/>
+      <c r="J42" s="105"/>
+      <c r="K42" s="106"/>
       <c r="L42" s="95"/>
       <c r="M42" s="96"/>
       <c r="N42" s="97"/>
@@ -6688,26 +6690,26 @@
       <c r="AE42" s="83"/>
       <c r="AF42" s="83"/>
       <c r="AG42" s="83"/>
-      <c r="AH42" s="103"/>
+      <c r="AH42" s="107"/>
       <c r="AI42" s="95"/>
       <c r="AJ42" s="96"/>
       <c r="AK42" s="96"/>
       <c r="AL42" s="96"/>
       <c r="AM42" s="96"/>
-      <c r="AN42" s="114"/>
+      <c r="AN42" s="118"/>
     </row>
     <row r="43" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="154"/>
-      <c r="B43" s="155"/>
-      <c r="C43" s="155"/>
-      <c r="D43" s="155"/>
-      <c r="E43" s="155"/>
-      <c r="F43" s="155"/>
-      <c r="G43" s="155"/>
-      <c r="H43" s="155"/>
-      <c r="I43" s="155"/>
-      <c r="J43" s="155"/>
-      <c r="K43" s="156"/>
+      <c r="A43" s="104"/>
+      <c r="B43" s="105"/>
+      <c r="C43" s="105"/>
+      <c r="D43" s="105"/>
+      <c r="E43" s="105"/>
+      <c r="F43" s="105"/>
+      <c r="G43" s="105"/>
+      <c r="H43" s="105"/>
+      <c r="I43" s="105"/>
+      <c r="J43" s="105"/>
+      <c r="K43" s="106"/>
       <c r="L43" s="95"/>
       <c r="M43" s="96"/>
       <c r="N43" s="97"/>
@@ -6733,26 +6735,26 @@
       <c r="AE43" s="83"/>
       <c r="AF43" s="83"/>
       <c r="AG43" s="83"/>
-      <c r="AH43" s="103"/>
+      <c r="AH43" s="107"/>
       <c r="AI43" s="95"/>
       <c r="AJ43" s="96"/>
       <c r="AK43" s="96"/>
       <c r="AL43" s="96"/>
       <c r="AM43" s="96"/>
-      <c r="AN43" s="114"/>
+      <c r="AN43" s="118"/>
     </row>
     <row r="44" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="154"/>
-      <c r="B44" s="155"/>
-      <c r="C44" s="155"/>
-      <c r="D44" s="155"/>
-      <c r="E44" s="155"/>
-      <c r="F44" s="155"/>
-      <c r="G44" s="155"/>
-      <c r="H44" s="155"/>
-      <c r="I44" s="155"/>
-      <c r="J44" s="155"/>
-      <c r="K44" s="156"/>
+      <c r="A44" s="104"/>
+      <c r="B44" s="105"/>
+      <c r="C44" s="105"/>
+      <c r="D44" s="105"/>
+      <c r="E44" s="105"/>
+      <c r="F44" s="105"/>
+      <c r="G44" s="105"/>
+      <c r="H44" s="105"/>
+      <c r="I44" s="105"/>
+      <c r="J44" s="105"/>
+      <c r="K44" s="106"/>
       <c r="L44" s="95"/>
       <c r="M44" s="96"/>
       <c r="N44" s="97"/>
@@ -6778,26 +6780,26 @@
       <c r="AE44" s="83"/>
       <c r="AF44" s="83"/>
       <c r="AG44" s="83"/>
-      <c r="AH44" s="103"/>
+      <c r="AH44" s="107"/>
       <c r="AI44" s="95"/>
       <c r="AJ44" s="96"/>
       <c r="AK44" s="96"/>
       <c r="AL44" s="96"/>
       <c r="AM44" s="96"/>
-      <c r="AN44" s="114"/>
+      <c r="AN44" s="118"/>
     </row>
     <row r="45" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="154"/>
-      <c r="B45" s="155"/>
-      <c r="C45" s="155"/>
-      <c r="D45" s="155"/>
-      <c r="E45" s="155"/>
-      <c r="F45" s="155"/>
-      <c r="G45" s="155"/>
-      <c r="H45" s="155"/>
-      <c r="I45" s="155"/>
-      <c r="J45" s="155"/>
-      <c r="K45" s="156"/>
+      <c r="A45" s="104"/>
+      <c r="B45" s="105"/>
+      <c r="C45" s="105"/>
+      <c r="D45" s="105"/>
+      <c r="E45" s="105"/>
+      <c r="F45" s="105"/>
+      <c r="G45" s="105"/>
+      <c r="H45" s="105"/>
+      <c r="I45" s="105"/>
+      <c r="J45" s="105"/>
+      <c r="K45" s="106"/>
       <c r="L45" s="95"/>
       <c r="M45" s="96"/>
       <c r="N45" s="97"/>
@@ -6823,26 +6825,26 @@
       <c r="AE45" s="83"/>
       <c r="AF45" s="83"/>
       <c r="AG45" s="83"/>
-      <c r="AH45" s="103"/>
+      <c r="AH45" s="107"/>
       <c r="AI45" s="95"/>
       <c r="AJ45" s="96"/>
       <c r="AK45" s="96"/>
       <c r="AL45" s="96"/>
       <c r="AM45" s="96"/>
-      <c r="AN45" s="114"/>
+      <c r="AN45" s="118"/>
     </row>
     <row r="46" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="154"/>
-      <c r="B46" s="155"/>
-      <c r="C46" s="155"/>
-      <c r="D46" s="155"/>
-      <c r="E46" s="155"/>
-      <c r="F46" s="155"/>
-      <c r="G46" s="155"/>
-      <c r="H46" s="155"/>
-      <c r="I46" s="155"/>
-      <c r="J46" s="155"/>
-      <c r="K46" s="156"/>
+      <c r="A46" s="104"/>
+      <c r="B46" s="105"/>
+      <c r="C46" s="105"/>
+      <c r="D46" s="105"/>
+      <c r="E46" s="105"/>
+      <c r="F46" s="105"/>
+      <c r="G46" s="105"/>
+      <c r="H46" s="105"/>
+      <c r="I46" s="105"/>
+      <c r="J46" s="105"/>
+      <c r="K46" s="106"/>
       <c r="L46" s="95"/>
       <c r="M46" s="96"/>
       <c r="N46" s="97"/>
@@ -6868,26 +6870,26 @@
       <c r="AE46" s="83"/>
       <c r="AF46" s="83"/>
       <c r="AG46" s="83"/>
-      <c r="AH46" s="103"/>
+      <c r="AH46" s="107"/>
       <c r="AI46" s="95"/>
       <c r="AJ46" s="96"/>
       <c r="AK46" s="96"/>
       <c r="AL46" s="96"/>
       <c r="AM46" s="96"/>
-      <c r="AN46" s="114"/>
+      <c r="AN46" s="118"/>
     </row>
     <row r="47" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="154"/>
-      <c r="B47" s="155"/>
-      <c r="C47" s="155"/>
-      <c r="D47" s="155"/>
-      <c r="E47" s="155"/>
-      <c r="F47" s="155"/>
-      <c r="G47" s="155"/>
-      <c r="H47" s="155"/>
-      <c r="I47" s="155"/>
-      <c r="J47" s="155"/>
-      <c r="K47" s="156"/>
+      <c r="A47" s="104"/>
+      <c r="B47" s="105"/>
+      <c r="C47" s="105"/>
+      <c r="D47" s="105"/>
+      <c r="E47" s="105"/>
+      <c r="F47" s="105"/>
+      <c r="G47" s="105"/>
+      <c r="H47" s="105"/>
+      <c r="I47" s="105"/>
+      <c r="J47" s="105"/>
+      <c r="K47" s="106"/>
       <c r="L47" s="95"/>
       <c r="M47" s="96"/>
       <c r="N47" s="97"/>
@@ -6913,13 +6915,13 @@
       <c r="AE47" s="83"/>
       <c r="AF47" s="83"/>
       <c r="AG47" s="83"/>
-      <c r="AH47" s="103"/>
+      <c r="AH47" s="107"/>
       <c r="AI47" s="95"/>
       <c r="AJ47" s="96"/>
       <c r="AK47" s="96"/>
       <c r="AL47" s="96"/>
       <c r="AM47" s="96"/>
-      <c r="AN47" s="114"/>
+      <c r="AN47" s="118"/>
     </row>
     <row r="48" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="92" t="s">
@@ -6953,38 +6955,38 @@
       <c r="AA48" s="99"/>
       <c r="AB48" s="99"/>
       <c r="AC48" s="100"/>
-      <c r="AD48" s="104">
+      <c r="AD48" s="108">
         <f>SUM(AD38:AH47)</f>
         <v>0</v>
       </c>
-      <c r="AE48" s="105"/>
-      <c r="AF48" s="105"/>
-      <c r="AG48" s="105"/>
-      <c r="AH48" s="113"/>
-      <c r="AI48" s="104">
+      <c r="AE48" s="109"/>
+      <c r="AF48" s="109"/>
+      <c r="AG48" s="109"/>
+      <c r="AH48" s="117"/>
+      <c r="AI48" s="108">
         <f>SUM(AI38:AN47)</f>
         <v>0</v>
       </c>
-      <c r="AJ48" s="105"/>
-      <c r="AK48" s="105"/>
-      <c r="AL48" s="105"/>
-      <c r="AM48" s="105"/>
-      <c r="AN48" s="106"/>
+      <c r="AJ48" s="109"/>
+      <c r="AK48" s="109"/>
+      <c r="AL48" s="109"/>
+      <c r="AM48" s="109"/>
+      <c r="AN48" s="110"/>
     </row>
     <row r="49" spans="1:40" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="107" t="s">
+      <c r="A49" s="111" t="s">
         <v>29</v>
       </c>
-      <c r="B49" s="108"/>
-      <c r="C49" s="108"/>
-      <c r="D49" s="108"/>
-      <c r="E49" s="108"/>
-      <c r="F49" s="108"/>
-      <c r="G49" s="108"/>
-      <c r="H49" s="108"/>
-      <c r="I49" s="108"/>
-      <c r="J49" s="108"/>
-      <c r="K49" s="109"/>
+      <c r="B49" s="112"/>
+      <c r="C49" s="112"/>
+      <c r="D49" s="112"/>
+      <c r="E49" s="112"/>
+      <c r="F49" s="112"/>
+      <c r="G49" s="112"/>
+      <c r="H49" s="112"/>
+      <c r="I49" s="112"/>
+      <c r="J49" s="112"/>
+      <c r="K49" s="113"/>
       <c r="L49" s="23"/>
       <c r="M49" s="25"/>
       <c r="N49" s="38"/>
@@ -7016,17 +7018,17 @@
       <c r="AN49" s="26"/>
     </row>
     <row r="50" spans="1:40" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="110"/>
-      <c r="B50" s="111"/>
-      <c r="C50" s="111"/>
-      <c r="D50" s="111"/>
-      <c r="E50" s="111"/>
-      <c r="F50" s="111"/>
-      <c r="G50" s="111"/>
-      <c r="H50" s="111"/>
-      <c r="I50" s="111"/>
-      <c r="J50" s="111"/>
-      <c r="K50" s="112"/>
+      <c r="A50" s="114"/>
+      <c r="B50" s="115"/>
+      <c r="C50" s="115"/>
+      <c r="D50" s="115"/>
+      <c r="E50" s="115"/>
+      <c r="F50" s="115"/>
+      <c r="G50" s="115"/>
+      <c r="H50" s="115"/>
+      <c r="I50" s="115"/>
+      <c r="J50" s="115"/>
+      <c r="K50" s="116"/>
       <c r="L50" s="24"/>
       <c r="M50" s="16"/>
       <c r="N50" s="37"/>
@@ -7058,17 +7060,17 @@
       <c r="AN50" s="17"/>
     </row>
     <row r="51" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="154"/>
-      <c r="B51" s="155"/>
-      <c r="C51" s="155"/>
-      <c r="D51" s="155"/>
-      <c r="E51" s="155"/>
-      <c r="F51" s="155"/>
-      <c r="G51" s="155"/>
-      <c r="H51" s="155"/>
-      <c r="I51" s="155"/>
-      <c r="J51" s="155"/>
-      <c r="K51" s="156"/>
+      <c r="A51" s="104"/>
+      <c r="B51" s="105"/>
+      <c r="C51" s="105"/>
+      <c r="D51" s="105"/>
+      <c r="E51" s="105"/>
+      <c r="F51" s="105"/>
+      <c r="G51" s="105"/>
+      <c r="H51" s="105"/>
+      <c r="I51" s="105"/>
+      <c r="J51" s="105"/>
+      <c r="K51" s="106"/>
       <c r="L51" s="95"/>
       <c r="M51" s="96"/>
       <c r="N51" s="97"/>
@@ -7094,7 +7096,7 @@
       <c r="AE51" s="83"/>
       <c r="AF51" s="83"/>
       <c r="AG51" s="83"/>
-      <c r="AH51" s="103"/>
+      <c r="AH51" s="107"/>
       <c r="AI51" s="82"/>
       <c r="AJ51" s="83"/>
       <c r="AK51" s="83"/>
@@ -7103,17 +7105,17 @@
       <c r="AN51" s="84"/>
     </row>
     <row r="52" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="154"/>
-      <c r="B52" s="155"/>
-      <c r="C52" s="155"/>
-      <c r="D52" s="155"/>
-      <c r="E52" s="155"/>
-      <c r="F52" s="155"/>
-      <c r="G52" s="155"/>
-      <c r="H52" s="155"/>
-      <c r="I52" s="155"/>
-      <c r="J52" s="155"/>
-      <c r="K52" s="156"/>
+      <c r="A52" s="104"/>
+      <c r="B52" s="105"/>
+      <c r="C52" s="105"/>
+      <c r="D52" s="105"/>
+      <c r="E52" s="105"/>
+      <c r="F52" s="105"/>
+      <c r="G52" s="105"/>
+      <c r="H52" s="105"/>
+      <c r="I52" s="105"/>
+      <c r="J52" s="105"/>
+      <c r="K52" s="106"/>
       <c r="L52" s="95"/>
       <c r="M52" s="96"/>
       <c r="N52" s="97"/>
@@ -7139,7 +7141,7 @@
       <c r="AE52" s="83"/>
       <c r="AF52" s="83"/>
       <c r="AG52" s="83"/>
-      <c r="AH52" s="103"/>
+      <c r="AH52" s="107"/>
       <c r="AI52" s="82"/>
       <c r="AJ52" s="83"/>
       <c r="AK52" s="83"/>
@@ -7148,17 +7150,17 @@
       <c r="AN52" s="84"/>
     </row>
     <row r="53" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="154"/>
-      <c r="B53" s="155"/>
-      <c r="C53" s="155"/>
-      <c r="D53" s="155"/>
-      <c r="E53" s="155"/>
-      <c r="F53" s="155"/>
-      <c r="G53" s="155"/>
-      <c r="H53" s="155"/>
-      <c r="I53" s="155"/>
-      <c r="J53" s="155"/>
-      <c r="K53" s="156"/>
+      <c r="A53" s="104"/>
+      <c r="B53" s="105"/>
+      <c r="C53" s="105"/>
+      <c r="D53" s="105"/>
+      <c r="E53" s="105"/>
+      <c r="F53" s="105"/>
+      <c r="G53" s="105"/>
+      <c r="H53" s="105"/>
+      <c r="I53" s="105"/>
+      <c r="J53" s="105"/>
+      <c r="K53" s="106"/>
       <c r="L53" s="95"/>
       <c r="M53" s="96"/>
       <c r="N53" s="97"/>
@@ -7184,7 +7186,7 @@
       <c r="AE53" s="83"/>
       <c r="AF53" s="83"/>
       <c r="AG53" s="83"/>
-      <c r="AH53" s="103"/>
+      <c r="AH53" s="107"/>
       <c r="AI53" s="82"/>
       <c r="AJ53" s="83"/>
       <c r="AK53" s="83"/>
@@ -7193,17 +7195,17 @@
       <c r="AN53" s="84"/>
     </row>
     <row r="54" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="154"/>
-      <c r="B54" s="155"/>
-      <c r="C54" s="155"/>
-      <c r="D54" s="155"/>
-      <c r="E54" s="155"/>
-      <c r="F54" s="155"/>
-      <c r="G54" s="155"/>
-      <c r="H54" s="155"/>
-      <c r="I54" s="155"/>
-      <c r="J54" s="155"/>
-      <c r="K54" s="156"/>
+      <c r="A54" s="104"/>
+      <c r="B54" s="105"/>
+      <c r="C54" s="105"/>
+      <c r="D54" s="105"/>
+      <c r="E54" s="105"/>
+      <c r="F54" s="105"/>
+      <c r="G54" s="105"/>
+      <c r="H54" s="105"/>
+      <c r="I54" s="105"/>
+      <c r="J54" s="105"/>
+      <c r="K54" s="106"/>
       <c r="L54" s="95"/>
       <c r="M54" s="96"/>
       <c r="N54" s="97"/>
@@ -7229,7 +7231,7 @@
       <c r="AE54" s="83"/>
       <c r="AF54" s="83"/>
       <c r="AG54" s="83"/>
-      <c r="AH54" s="103"/>
+      <c r="AH54" s="107"/>
       <c r="AI54" s="82"/>
       <c r="AJ54" s="83"/>
       <c r="AK54" s="83"/>
@@ -7238,17 +7240,17 @@
       <c r="AN54" s="84"/>
     </row>
     <row r="55" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="154"/>
-      <c r="B55" s="155"/>
-      <c r="C55" s="155"/>
-      <c r="D55" s="155"/>
-      <c r="E55" s="155"/>
-      <c r="F55" s="155"/>
-      <c r="G55" s="155"/>
-      <c r="H55" s="155"/>
-      <c r="I55" s="155"/>
-      <c r="J55" s="155"/>
-      <c r="K55" s="156"/>
+      <c r="A55" s="104"/>
+      <c r="B55" s="105"/>
+      <c r="C55" s="105"/>
+      <c r="D55" s="105"/>
+      <c r="E55" s="105"/>
+      <c r="F55" s="105"/>
+      <c r="G55" s="105"/>
+      <c r="H55" s="105"/>
+      <c r="I55" s="105"/>
+      <c r="J55" s="105"/>
+      <c r="K55" s="106"/>
       <c r="L55" s="95"/>
       <c r="M55" s="96"/>
       <c r="N55" s="97"/>
@@ -7274,7 +7276,7 @@
       <c r="AE55" s="83"/>
       <c r="AF55" s="83"/>
       <c r="AG55" s="83"/>
-      <c r="AH55" s="103"/>
+      <c r="AH55" s="107"/>
       <c r="AI55" s="82"/>
       <c r="AJ55" s="83"/>
       <c r="AK55" s="83"/>
@@ -7283,17 +7285,17 @@
       <c r="AN55" s="84"/>
     </row>
     <row r="56" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="154"/>
-      <c r="B56" s="155"/>
-      <c r="C56" s="155"/>
-      <c r="D56" s="155"/>
-      <c r="E56" s="155"/>
-      <c r="F56" s="155"/>
-      <c r="G56" s="155"/>
-      <c r="H56" s="155"/>
-      <c r="I56" s="155"/>
-      <c r="J56" s="155"/>
-      <c r="K56" s="156"/>
+      <c r="A56" s="104"/>
+      <c r="B56" s="105"/>
+      <c r="C56" s="105"/>
+      <c r="D56" s="105"/>
+      <c r="E56" s="105"/>
+      <c r="F56" s="105"/>
+      <c r="G56" s="105"/>
+      <c r="H56" s="105"/>
+      <c r="I56" s="105"/>
+      <c r="J56" s="105"/>
+      <c r="K56" s="106"/>
       <c r="L56" s="95"/>
       <c r="M56" s="96"/>
       <c r="N56" s="97"/>
@@ -7319,7 +7321,7 @@
       <c r="AE56" s="83"/>
       <c r="AF56" s="83"/>
       <c r="AG56" s="83"/>
-      <c r="AH56" s="103"/>
+      <c r="AH56" s="107"/>
       <c r="AI56" s="82"/>
       <c r="AJ56" s="83"/>
       <c r="AK56" s="83"/>
@@ -7328,17 +7330,17 @@
       <c r="AN56" s="84"/>
     </row>
     <row r="57" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="154"/>
-      <c r="B57" s="155"/>
-      <c r="C57" s="155"/>
-      <c r="D57" s="155"/>
-      <c r="E57" s="155"/>
-      <c r="F57" s="155"/>
-      <c r="G57" s="155"/>
-      <c r="H57" s="155"/>
-      <c r="I57" s="155"/>
-      <c r="J57" s="155"/>
-      <c r="K57" s="156"/>
+      <c r="A57" s="104"/>
+      <c r="B57" s="105"/>
+      <c r="C57" s="105"/>
+      <c r="D57" s="105"/>
+      <c r="E57" s="105"/>
+      <c r="F57" s="105"/>
+      <c r="G57" s="105"/>
+      <c r="H57" s="105"/>
+      <c r="I57" s="105"/>
+      <c r="J57" s="105"/>
+      <c r="K57" s="106"/>
       <c r="L57" s="95"/>
       <c r="M57" s="96"/>
       <c r="N57" s="97"/>
@@ -7364,7 +7366,7 @@
       <c r="AE57" s="83"/>
       <c r="AF57" s="83"/>
       <c r="AG57" s="83"/>
-      <c r="AH57" s="103"/>
+      <c r="AH57" s="107"/>
       <c r="AI57" s="82"/>
       <c r="AJ57" s="83"/>
       <c r="AK57" s="83"/>
@@ -7373,17 +7375,17 @@
       <c r="AN57" s="84"/>
     </row>
     <row r="58" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="154"/>
-      <c r="B58" s="155"/>
-      <c r="C58" s="155"/>
-      <c r="D58" s="155"/>
-      <c r="E58" s="155"/>
-      <c r="F58" s="155"/>
-      <c r="G58" s="155"/>
-      <c r="H58" s="155"/>
-      <c r="I58" s="155"/>
-      <c r="J58" s="155"/>
-      <c r="K58" s="156"/>
+      <c r="A58" s="104"/>
+      <c r="B58" s="105"/>
+      <c r="C58" s="105"/>
+      <c r="D58" s="105"/>
+      <c r="E58" s="105"/>
+      <c r="F58" s="105"/>
+      <c r="G58" s="105"/>
+      <c r="H58" s="105"/>
+      <c r="I58" s="105"/>
+      <c r="J58" s="105"/>
+      <c r="K58" s="106"/>
       <c r="L58" s="95"/>
       <c r="M58" s="96"/>
       <c r="N58" s="97"/>
@@ -7409,7 +7411,7 @@
       <c r="AE58" s="83"/>
       <c r="AF58" s="83"/>
       <c r="AG58" s="83"/>
-      <c r="AH58" s="103"/>
+      <c r="AH58" s="107"/>
       <c r="AI58" s="82"/>
       <c r="AJ58" s="83"/>
       <c r="AK58" s="83"/>
@@ -7418,17 +7420,17 @@
       <c r="AN58" s="84"/>
     </row>
     <row r="59" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="154"/>
-      <c r="B59" s="155"/>
-      <c r="C59" s="155"/>
-      <c r="D59" s="155"/>
-      <c r="E59" s="155"/>
-      <c r="F59" s="155"/>
-      <c r="G59" s="155"/>
-      <c r="H59" s="155"/>
-      <c r="I59" s="155"/>
-      <c r="J59" s="155"/>
-      <c r="K59" s="156"/>
+      <c r="A59" s="104"/>
+      <c r="B59" s="105"/>
+      <c r="C59" s="105"/>
+      <c r="D59" s="105"/>
+      <c r="E59" s="105"/>
+      <c r="F59" s="105"/>
+      <c r="G59" s="105"/>
+      <c r="H59" s="105"/>
+      <c r="I59" s="105"/>
+      <c r="J59" s="105"/>
+      <c r="K59" s="106"/>
       <c r="L59" s="95"/>
       <c r="M59" s="96"/>
       <c r="N59" s="97"/>
@@ -7454,7 +7456,7 @@
       <c r="AE59" s="83"/>
       <c r="AF59" s="83"/>
       <c r="AG59" s="83"/>
-      <c r="AH59" s="103"/>
+      <c r="AH59" s="107"/>
       <c r="AI59" s="82"/>
       <c r="AJ59" s="83"/>
       <c r="AK59" s="83"/>
@@ -7653,17 +7655,17 @@
       <c r="M64" s="49"/>
       <c r="N64" s="49"/>
       <c r="O64" s="49"/>
-      <c r="P64" s="157"/>
-      <c r="Q64" s="157"/>
-      <c r="R64" s="157"/>
-      <c r="S64" s="157"/>
-      <c r="T64" s="157"/>
-      <c r="U64" s="157"/>
-      <c r="V64" s="157"/>
-      <c r="W64" s="157"/>
-      <c r="X64" s="157"/>
-      <c r="Y64" s="157"/>
-      <c r="Z64" s="157"/>
+      <c r="P64" s="103"/>
+      <c r="Q64" s="103"/>
+      <c r="R64" s="103"/>
+      <c r="S64" s="103"/>
+      <c r="T64" s="103"/>
+      <c r="U64" s="103"/>
+      <c r="V64" s="103"/>
+      <c r="W64" s="103"/>
+      <c r="X64" s="103"/>
+      <c r="Y64" s="103"/>
+      <c r="Z64" s="103"/>
       <c r="AA64" s="49"/>
       <c r="AB64" s="49"/>
       <c r="AC64" s="49"/>

</xml_diff>